<commit_message>
Modificate le pagine dei menù e delle view
Creati i primi due casi d'uso
</commit_message>
<xml_diff>
--- a/Documentazioni/Codifica pagine sito.xlsx
+++ b/Documentazioni/Codifica pagine sito.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05745DCC-8B85-4274-930D-FBE0A6EA0768}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDC33F4A-EEF7-4542-AC82-1D0B9ADAC3C9}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -11,7 +11,7 @@
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Foglio1!$A$1:$C$31</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Foglio1!$A$1:$C$36</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="86">
   <si>
     <t>Nome gabbia logica</t>
   </si>
@@ -46,30 +46,12 @@
     <t>form di registrazione ASD</t>
   </si>
   <si>
-    <t>Registrazione socio fondatore</t>
-  </si>
-  <si>
-    <t>successivamente la registrazione ASD si deve registrare il socio fondatore</t>
-  </si>
-  <si>
-    <t>Messaggio di registrazione effettuata</t>
-  </si>
-  <si>
     <t>messaggio di registrazione riuscita per il socio fondatore</t>
   </si>
   <si>
-    <t>All'avvio del gestionale, se è presente una ASD in memoria, si procede direttamente al login del personale</t>
-  </si>
-  <si>
     <t>Login utente gestionale</t>
   </si>
   <si>
-    <t>Registrazione utente del gestionale</t>
-  </si>
-  <si>
-    <t>se al momento del login, l'utente non è ancora registrato può registrarsi tramite il form in questa pagina</t>
-  </si>
-  <si>
     <t>Homepage</t>
   </si>
   <si>
@@ -229,13 +211,76 @@
     <t>A030</t>
   </si>
   <si>
-    <t>B000</t>
-  </si>
-  <si>
-    <t>B010</t>
-  </si>
-  <si>
     <t>VOCE MENU'</t>
+  </si>
+  <si>
+    <t>B005</t>
+  </si>
+  <si>
+    <t>L'utente accede al gestionale all'ASD già registrata</t>
+  </si>
+  <si>
+    <t>Registrazione primo socio fondatore</t>
+  </si>
+  <si>
+    <t>successivamente la registrazione ASD si deve registrare il primo socio fondatore (è mostrata solo una volta)</t>
+  </si>
+  <si>
+    <t>B006</t>
+  </si>
+  <si>
+    <t>Login effettuato con successo</t>
+  </si>
+  <si>
+    <t>Avverte l'utente che il login è andato a buon fine e lo reindirizza alla M000 dopo qualche secondo</t>
+  </si>
+  <si>
+    <t>B007</t>
+  </si>
+  <si>
+    <t>Login avviso fallimento</t>
+  </si>
+  <si>
+    <t>Avverte l'utente che il login non è andato a buon fine e lo reindirizza alla B005</t>
+  </si>
+  <si>
+    <t>Registrazione primo socio fond effettuata</t>
+  </si>
+  <si>
+    <t>A011</t>
+  </si>
+  <si>
+    <t>Registrazione ASD con successo</t>
+  </si>
+  <si>
+    <t>messaggio di registrazione riuscita per l'ASD</t>
+  </si>
+  <si>
+    <t>C000</t>
+  </si>
+  <si>
+    <t>Pagina Chi siamo</t>
+  </si>
+  <si>
+    <t>Contiene le foto del gruppo di lavoro</t>
+  </si>
+  <si>
+    <t>Pagina Contatti</t>
+  </si>
+  <si>
+    <t>Contiene tutti  i recapiti del gruppo di lavoro</t>
+  </si>
+  <si>
+    <t>C010</t>
+  </si>
+  <si>
+    <t>D000</t>
+  </si>
+  <si>
+    <t>Account personale</t>
+  </si>
+  <si>
+    <t>Permette di modificare l'anagrafica dell'utente acceduto</t>
   </si>
 </sst>
 </file>
@@ -251,12 +296,30 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -271,8 +334,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -553,17 +629,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C31"/>
+  <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="25.77734375" customWidth="1"/>
-    <col min="2" max="2" width="33.6640625" customWidth="1"/>
-    <col min="3" max="3" width="30.6640625" customWidth="1"/>
+    <col min="2" max="2" width="35.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="87.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="28.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -580,7 +656,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
@@ -591,7 +667,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
@@ -602,263 +678,318 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>75</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>65</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>73</v>
       </c>
       <c r="C6" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>14</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>68</v>
       </c>
       <c r="C8" t="s">
-        <v>16</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>31</v>
+        <v>70</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>71</v>
       </c>
       <c r="C9" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>32</v>
+        <v>77</v>
       </c>
       <c r="B10" t="s">
-        <v>23</v>
+        <v>78</v>
       </c>
       <c r="C10" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>33</v>
+        <v>82</v>
       </c>
       <c r="B11" t="s">
-        <v>25</v>
+        <v>80</v>
+      </c>
+      <c r="C11" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>34</v>
+        <v>83</v>
       </c>
       <c r="B12" t="s">
-        <v>26</v>
+        <v>84</v>
+      </c>
+      <c r="C12" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>35</v>
+        <v>57</v>
       </c>
       <c r="B13" t="s">
-        <v>27</v>
+        <v>9</v>
+      </c>
+      <c r="C13" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>36</v>
-      </c>
-      <c r="B14" t="s">
-        <v>28</v>
+        <v>25</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>37</v>
-      </c>
-      <c r="B15" t="s">
-        <v>24</v>
+        <v>26</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="C15" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>38</v>
-      </c>
-      <c r="B16" t="s">
-        <v>29</v>
+        <v>27</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>39</v>
-      </c>
-      <c r="B17" t="s">
-        <v>30</v>
+        <v>28</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>40</v>
-      </c>
-      <c r="B18" t="s">
-        <v>18</v>
-      </c>
-      <c r="C18" t="s">
-        <v>70</v>
+        <v>29</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>41</v>
-      </c>
-      <c r="B19" t="s">
-        <v>47</v>
-      </c>
-      <c r="C19" t="s">
-        <v>70</v>
+        <v>30</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>51</v>
-      </c>
-      <c r="B20" t="s">
-        <v>48</v>
+        <v>31</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>52</v>
-      </c>
-      <c r="B21" t="s">
-        <v>49</v>
+        <v>32</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>53</v>
-      </c>
-      <c r="B22" t="s">
-        <v>50</v>
+        <v>33</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>54</v>
-      </c>
-      <c r="B23" t="s">
-        <v>19</v>
+        <v>34</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>12</v>
       </c>
       <c r="C23" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>55</v>
-      </c>
-      <c r="B24" t="s">
-        <v>42</v>
+        <v>35</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C24" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>56</v>
-      </c>
-      <c r="B25" t="s">
-        <v>43</v>
+        <v>45</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>58</v>
-      </c>
-      <c r="B26" t="s">
-        <v>44</v>
+        <v>46</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>57</v>
-      </c>
-      <c r="B27" t="s">
-        <v>45</v>
+        <v>47</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>59</v>
-      </c>
-      <c r="B28" t="s">
-        <v>46</v>
+        <v>48</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C28" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>60</v>
-      </c>
-      <c r="B29" t="s">
-        <v>20</v>
+        <v>49</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>61</v>
-      </c>
-      <c r="B30" t="s">
-        <v>21</v>
+        <v>50</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>62</v>
-      </c>
-      <c r="B31" t="s">
-        <v>22</v>
+        <v>52</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>51</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>53</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>54</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>55</v>
+      </c>
+      <c r="B35" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>56</v>
+      </c>
+      <c r="B36" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C31" xr:uid="{34684D11-7ACD-45A4-AA96-0CE6C7239D98}"/>
+  <autoFilter ref="A1:C36" xr:uid="{34684D11-7ACD-45A4-AA96-0CE6C7239D98}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Scambiato il codice con la view boot_socio
</commit_message>
<xml_diff>
--- a/Documentazioni/Codifica pagine sito.xlsx
+++ b/Documentazioni/Codifica pagine sito.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr filterPrivacy="1" codeName="Questa_cartella_di_lavoro"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12A20B44-D483-420A-8939-38B7C6248617}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BD3C96D-B3F6-4E6B-A668-2560D5784ACA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8988" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,6 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -184,9 +183,6 @@
     <t>A010</t>
   </si>
   <si>
-    <t>A020</t>
-  </si>
-  <si>
     <t>A030</t>
   </si>
   <si>
@@ -316,9 +312,6 @@
     <t>Login fallito</t>
   </si>
   <si>
-    <t>boot_done</t>
-  </si>
-  <si>
     <t>Registrazione socio fondatore</t>
   </si>
   <si>
@@ -452,6 +445,12 @@
   </si>
   <si>
     <t>Messaggio di registrazione riuscita per il socio fondatore</t>
+  </si>
+  <si>
+    <t>boot_asd_done</t>
+  </si>
+  <si>
+    <t>A025</t>
   </si>
 </sst>
 </file>
@@ -654,53 +653,6 @@
   </cellStyles>
   <dxfs count="17">
     <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <font>
         <strike val="0"/>
         <outline val="0"/>
@@ -714,6 +666,9 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -761,14 +716,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <strike val="0"/>
         <outline val="0"/>
@@ -790,6 +737,29 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -805,7 +775,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -844,19 +814,48 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <font>
+        <b/>
+        <i val="0"/>
         <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="10"/>
+        <sz val="11"/>
         <color theme="1"/>
         <name val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -872,34 +871,34 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{905F6574-56C3-4E36-86AD-16F4E970F9D2}" name="Tabella4" displayName="Tabella4" ref="A1:H34" dataDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{905F6574-56C3-4E36-86AD-16F4E970F9D2}" name="Tabella4" displayName="Tabella4" ref="A1:H34" dataDxfId="13">
   <autoFilter ref="A1:H34" xr:uid="{34684D11-7ACD-45A4-AA96-0CE6C7239D98}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{E7D98D43-EB7B-46CE-B0B0-C555D83773A6}" name="Codice gabbia logica" dataDxfId="15" totalsRowDxfId="14"/>
-    <tableColumn id="2" xr3:uid="{DB39DBBD-231C-4393-B53A-31DA54EF2B6B}" name="Tipo" dataDxfId="13" totalsRowDxfId="12"/>
-    <tableColumn id="3" xr3:uid="{267C913B-0C60-4A11-8D31-6129F6A6699A}" name="Nome gabbia logica" dataDxfId="11" totalsRowDxfId="10"/>
-    <tableColumn id="5" xr3:uid="{251AE08F-697F-47EC-9FB6-7CEF1CCB916E}" name="view" dataDxfId="9" totalsRowDxfId="8"/>
-    <tableColumn id="6" xr3:uid="{E87D751D-6B30-48F2-95B8-E2DCF4172ECA}" name="Nome file" dataDxfId="7">
+    <tableColumn id="1" xr3:uid="{E7D98D43-EB7B-46CE-B0B0-C555D83773A6}" name="Codice gabbia logica" dataDxfId="11" totalsRowDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{DB39DBBD-231C-4393-B53A-31DA54EF2B6B}" name="Tipo" dataDxfId="9" totalsRowDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{267C913B-0C60-4A11-8D31-6129F6A6699A}" name="Nome gabbia logica" dataDxfId="7" totalsRowDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{251AE08F-697F-47EC-9FB6-7CEF1CCB916E}" name="view" dataDxfId="5" totalsRowDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{E87D751D-6B30-48F2-95B8-E2DCF4172ECA}" name="Nome file" dataDxfId="4">
       <calculatedColumnFormula>IF($D2="Da definire",$D2,_xlfn.CONCAT($D2,".blade.php"))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{CAF26B0C-D3E2-4A71-A7C5-519E983C334C}" name="Rotta" dataDxfId="6">
+    <tableColumn id="8" xr3:uid="{CAF26B0C-D3E2-4A71-A7C5-519E983C334C}" name="Rotta" dataDxfId="3">
       <calculatedColumnFormula>"/" &amp; D2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{C8498EB6-2C5F-47B9-B993-99AA78B7EEAA}" name="Controller" dataDxfId="5"/>
-    <tableColumn id="10" xr3:uid="{E6E3AEA2-F019-429B-B8B1-54C1BCAF6687}" name="Commento" dataDxfId="4" totalsRowDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{C8498EB6-2C5F-47B9-B993-99AA78B7EEAA}" name="Controller" dataDxfId="2"/>
+    <tableColumn id="10" xr3:uid="{E6E3AEA2-F019-429B-B8B1-54C1BCAF6687}" name="Commento" dataDxfId="0" totalsRowDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium12" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{45120F09-8607-4F6A-A989-7184307236A1}" name="Tipo" displayName="Tipo" ref="B1:B8" totalsRowShown="0" headerRowDxfId="2" tableBorderDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{45120F09-8607-4F6A-A989-7184307236A1}" name="Tipo" displayName="Tipo" ref="B1:B8" totalsRowShown="0" headerRowDxfId="16" tableBorderDxfId="15">
   <autoFilter ref="B1:B8" xr:uid="{B0803B6A-3448-4A89-AC43-1127F3DBD833}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:B8">
+  <sortState ref="B2:B8">
     <sortCondition ref="B1:B8"/>
   </sortState>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{95A47413-48BC-4507-BE9E-0DFA740DC4DC}" name="Tipi di pagina" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{95A47413-48BC-4507-BE9E-0DFA740DC4DC}" name="Tipi di pagina" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1181,66 +1180,66 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Foglio2"/>
-  <dimension ref="A1:I34"/>
+  <dimension ref="A1:I35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="106" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H34"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="3" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" outlineLevelRow="3" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.5546875" style="14" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.5703125" style="14" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13" style="12" customWidth="1"/>
-    <col min="3" max="3" width="35.5546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.21875" style="15" customWidth="1"/>
-    <col min="5" max="5" width="24.44140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="29.33203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" style="15" customWidth="1"/>
+    <col min="5" max="5" width="24.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.28515625" style="13" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17" style="13" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="89.77734375" style="11" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="28.6640625" style="13" customWidth="1"/>
-    <col min="10" max="11" width="8.88671875" style="13"/>
+    <col min="8" max="8" width="89.7109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="28.7109375" style="13" customWidth="1"/>
+    <col min="10" max="11" width="8.85546875" style="13"/>
     <col min="12" max="12" width="19" style="13" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="8.88671875" style="13"/>
+    <col min="13" max="16384" width="8.85546875" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C1" s="11" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="13" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F1" s="13" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G1" s="13" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H1" s="11" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>48</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C2" s="19" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D2" s="20" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E2" s="18" t="str">
         <f t="shared" ref="E2:E34" si="0">IF($D2="Da definire",$D2,_xlfn.CONCAT($D2,".blade.php"))</f>
@@ -1251,24 +1250,24 @@
         <v>/welcome</v>
       </c>
       <c r="G2" s="18" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H2" s="19" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
         <v>49</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C3" s="19" t="s">
         <v>3</v>
       </c>
       <c r="D3" s="20" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E3" s="18" t="str">
         <f t="shared" si="0"/>
@@ -1279,109 +1278,108 @@
         <v>/boot</v>
       </c>
       <c r="G3" s="18" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H3" s="19" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C4" s="19" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D4" s="20" t="s">
-        <v>94</v>
+        <v>138</v>
       </c>
       <c r="E4" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>boot_done.blade.php</v>
+        <v>boot_asd_done.blade.php</v>
       </c>
       <c r="F4" s="18" t="str">
         <f t="shared" si="1"/>
-        <v>/boot_done</v>
+        <v>/boot_asd_done</v>
       </c>
       <c r="G4" s="18" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H4" s="19" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
+        <v>139</v>
+      </c>
+      <c r="B5" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="D5" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="E5" s="18" t="str">
+        <f>IF($D5="Da definire",$D5,_xlfn.CONCAT($D5,".blade.php"))</f>
+        <v>boot_socio.blade.php</v>
+      </c>
+      <c r="F5" s="18" t="str">
+        <f>"/" &amp; D5</f>
+        <v>/boot_socio</v>
+      </c>
+      <c r="G5" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="H5" s="19" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="B5" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="C5" s="19" t="s">
+      <c r="B6" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="C6" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="D6" s="20" t="s">
         <v>96</v>
       </c>
-      <c r="D5" s="20" t="s">
-        <v>98</v>
-      </c>
-      <c r="E5" s="18" t="str">
+      <c r="E6" s="18" t="str">
         <f t="shared" si="0"/>
         <v>boot_finished.blade.php</v>
       </c>
-      <c r="F5" s="18" t="str">
+      <c r="F6" s="18" t="str">
         <f t="shared" si="1"/>
         <v>/boot_finished</v>
       </c>
-      <c r="G5" s="18" t="s">
-        <v>77</v>
-      </c>
-      <c r="H5" s="19" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="18" t="s">
-        <v>51</v>
-      </c>
-      <c r="B6" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="C6" s="19" t="s">
-        <v>95</v>
-      </c>
-      <c r="D6" s="20" t="s">
-        <v>97</v>
-      </c>
-      <c r="E6" s="18" t="str">
-        <f t="shared" si="0"/>
-        <v>boot_socio.blade.php</v>
-      </c>
-      <c r="F6" s="18" t="str">
-        <f t="shared" si="1"/>
-        <v>/boot_socio</v>
-      </c>
       <c r="G6" s="18" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H6" s="19" t="s">
-        <v>139</v>
-      </c>
-      <c r="I6" s="12"/>
-    </row>
-    <row r="7" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D7" s="20" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E7" s="18" t="str">
         <f t="shared" si="0"/>
@@ -1392,25 +1390,25 @@
         <v>/login</v>
       </c>
       <c r="G7" s="18" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H7" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="I7" s="12"/>
+    </row>
+    <row r="8" spans="1:9" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="I7" s="12"/>
-    </row>
-    <row r="8" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="18" t="s">
-        <v>55</v>
-      </c>
       <c r="B8" s="18" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C8" s="19" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D8" s="20" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E8" s="18" t="str">
         <f t="shared" si="0"/>
@@ -1421,25 +1419,25 @@
         <v>/login_done</v>
       </c>
       <c r="G8" s="18" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H8" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="I8" s="12"/>
+    </row>
+    <row r="9" spans="1:9" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="I8" s="12"/>
-    </row>
-    <row r="9" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="18" t="s">
-        <v>57</v>
-      </c>
       <c r="B9" s="18" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C9" s="19" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D9" s="20" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E9" s="18" t="str">
         <f t="shared" si="0"/>
@@ -1450,25 +1448,25 @@
         <v>/login_failure</v>
       </c>
       <c r="G9" s="18" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H9" s="19" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I9" s="12"/>
     </row>
-    <row r="10" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C10" s="19" t="s">
         <v>9</v>
       </c>
       <c r="D10" s="20" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E10" s="18" t="str">
         <f t="shared" si="0"/>
@@ -1479,24 +1477,24 @@
         <v>/our_team</v>
       </c>
       <c r="G10" s="18" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H10" s="19" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="18" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B11" s="18" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C11" s="19" t="s">
         <v>10</v>
       </c>
       <c r="D11" s="20" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E11" s="18" t="str">
         <f t="shared" si="0"/>
@@ -1507,24 +1505,24 @@
         <v>/contacts</v>
       </c>
       <c r="G11" s="18" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H11" s="19" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="B12" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="C12" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="B12" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="C12" s="19" t="s">
-        <v>65</v>
-      </c>
       <c r="D12" s="20" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E12" s="18" t="str">
         <f t="shared" si="0"/>
@@ -1535,24 +1533,24 @@
         <v>/settings_account</v>
       </c>
       <c r="G12" s="18" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H12" s="19" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="28" t="s">
         <v>47</v>
       </c>
       <c r="B13" s="28" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C13" s="24" t="s">
         <v>4</v>
       </c>
       <c r="D13" s="28" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E13" s="28" t="str">
         <f t="shared" si="0"/>
@@ -1563,24 +1561,24 @@
         <v>/homepage</v>
       </c>
       <c r="G13" s="28" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H13" s="24" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="19.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" ht="19.899999999999999" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A14" s="26" t="s">
         <v>18</v>
       </c>
       <c r="B14" s="26" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C14" s="23" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D14" s="26" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E14" s="26" t="str">
         <f t="shared" si="0"/>
@@ -1591,24 +1589,24 @@
         <v>/managment</v>
       </c>
       <c r="G14" s="26" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="H14" s="23" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="19.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="19.899999999999999" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A15" s="27" t="s">
         <v>19</v>
       </c>
       <c r="B15" s="27" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C15" s="21" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D15" s="27" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E15" s="27" t="str">
         <f t="shared" si="0"/>
@@ -1619,24 +1617,24 @@
         <v>/staff</v>
       </c>
       <c r="G15" s="27" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="H15" s="21" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="19.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="19.899999999999999" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A16" s="25" t="s">
         <v>20</v>
       </c>
       <c r="B16" s="25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C16" s="22" t="s">
         <v>12</v>
       </c>
       <c r="D16" s="25" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E16" s="25" t="str">
         <f t="shared" si="0"/>
@@ -1647,22 +1645,22 @@
         <v>/staff/collab-int</v>
       </c>
       <c r="G16" s="25" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="H16" s="22"/>
     </row>
-    <row r="17" spans="1:8" ht="19.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" ht="19.899999999999999" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A17" s="25" t="s">
         <v>21</v>
       </c>
       <c r="B17" s="25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C17" s="22" t="s">
         <v>13</v>
       </c>
       <c r="D17" s="25" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E17" s="25" t="str">
         <f t="shared" si="0"/>
@@ -1673,22 +1671,22 @@
         <v>/staff/collab-ext</v>
       </c>
       <c r="G17" s="25" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="H17" s="22"/>
     </row>
-    <row r="18" spans="1:8" ht="19.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" ht="19.899999999999999" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A18" s="25" t="s">
         <v>22</v>
       </c>
       <c r="B18" s="25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C18" s="22" t="s">
         <v>14</v>
       </c>
       <c r="D18" s="25" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E18" s="25" t="str">
         <f t="shared" si="0"/>
@@ -1699,22 +1697,22 @@
         <v>/staff/trainee</v>
       </c>
       <c r="G18" s="25" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="H18" s="22"/>
     </row>
-    <row r="19" spans="1:8" ht="19.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" ht="19.899999999999999" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A19" s="25" t="s">
         <v>23</v>
       </c>
       <c r="B19" s="25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C19" s="22" t="s">
         <v>15</v>
       </c>
       <c r="D19" s="25" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E19" s="25" t="str">
         <f t="shared" si="0"/>
@@ -1725,22 +1723,22 @@
         <v>/staff/teacher</v>
       </c>
       <c r="G19" s="25" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="H19" s="22"/>
     </row>
-    <row r="20" spans="1:8" ht="19.95" customHeight="1" outlineLevel="2" collapsed="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" ht="19.899999999999999" hidden="1" customHeight="1" outlineLevel="2" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A20" s="27" t="s">
         <v>24</v>
       </c>
       <c r="B20" s="27" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C20" s="21" t="s">
         <v>11</v>
       </c>
       <c r="D20" s="27" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E20" s="27" t="str">
         <f t="shared" si="0"/>
@@ -1751,24 +1749,24 @@
         <v>/payments</v>
       </c>
       <c r="G20" s="27" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="H20" s="21" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="19.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="19.899999999999999" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A21" s="25" t="s">
         <v>25</v>
       </c>
       <c r="B21" s="25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C21" s="22" t="s">
         <v>16</v>
       </c>
       <c r="D21" s="25" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E21" s="25" t="str">
         <f t="shared" si="0"/>
@@ -1779,22 +1777,22 @@
         <v>/payments/outflow</v>
       </c>
       <c r="G21" s="25" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="H21" s="22"/>
     </row>
-    <row r="22" spans="1:8" ht="19.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" ht="19.899999999999999" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A22" s="25" t="s">
         <v>26</v>
       </c>
       <c r="B22" s="25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C22" s="22" t="s">
         <v>17</v>
       </c>
       <c r="D22" s="25" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E22" s="25" t="str">
         <f t="shared" si="0"/>
@@ -1805,22 +1803,22 @@
         <v>/payments/earn</v>
       </c>
       <c r="G22" s="25" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="H22" s="22"/>
     </row>
-    <row r="23" spans="1:8" ht="19.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" ht="19.899999999999999" hidden="1" customHeight="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A23" s="26" t="s">
         <v>27</v>
       </c>
       <c r="B23" s="26" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C23" s="23" t="s">
         <v>6</v>
       </c>
       <c r="D23" s="26" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E23" s="26" t="str">
         <f t="shared" si="0"/>
@@ -1831,24 +1829,24 @@
         <v>/secretariat</v>
       </c>
       <c r="G23" s="26" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="H23" s="23" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="19.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="19.899999999999999" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A24" s="27" t="s">
         <v>28</v>
       </c>
       <c r="B24" s="27" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C24" s="21" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D24" s="27" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E24" s="27" t="str">
         <f t="shared" si="0"/>
@@ -1859,24 +1857,24 @@
         <v>/subscribers</v>
       </c>
       <c r="G24" s="27" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="H24" s="21" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="19.95" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="19.899999999999999" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A25" s="25" t="s">
         <v>37</v>
       </c>
       <c r="B25" s="25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C25" s="22" t="s">
         <v>34</v>
       </c>
       <c r="D25" s="25" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E25" s="25" t="str">
         <f t="shared" si="0"/>
@@ -1887,22 +1885,22 @@
         <v>/subscribers/students</v>
       </c>
       <c r="G25" s="25" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="H25" s="22"/>
     </row>
-    <row r="26" spans="1:8" ht="19.95" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" ht="19.899999999999999" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A26" s="25" t="s">
         <v>38</v>
       </c>
       <c r="B26" s="25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C26" s="22" t="s">
         <v>35</v>
       </c>
       <c r="D26" s="25" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E26" s="25" t="str">
         <f t="shared" si="0"/>
@@ -1913,22 +1911,22 @@
         <v>/subscribers/cards</v>
       </c>
       <c r="G26" s="25" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="H26" s="22"/>
     </row>
-    <row r="27" spans="1:8" ht="19.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" ht="19.899999999999999" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A27" s="27" t="s">
         <v>39</v>
       </c>
       <c r="B27" s="27" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C27" s="21" t="s">
         <v>36</v>
       </c>
       <c r="D27" s="27" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E27" s="27" t="str">
         <f t="shared" si="0"/>
@@ -1939,22 +1937,22 @@
         <v>/vendors</v>
       </c>
       <c r="G27" s="27" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="H27" s="21"/>
     </row>
-    <row r="28" spans="1:8" ht="19.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" ht="19.899999999999999" hidden="1" customHeight="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A28" s="26" t="s">
         <v>40</v>
       </c>
       <c r="B28" s="26" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C28" s="23" t="s">
         <v>7</v>
       </c>
       <c r="D28" s="26" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E28" s="26" t="str">
         <f t="shared" si="0"/>
@@ -1965,24 +1963,24 @@
         <v>/mng_activity</v>
       </c>
       <c r="G28" s="26" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="H28" s="23" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" ht="19.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="19.899999999999999" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A29" s="25" t="s">
         <v>41</v>
       </c>
       <c r="B29" s="25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C29" s="22" t="s">
         <v>29</v>
       </c>
       <c r="D29" s="25" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E29" s="25" t="str">
         <f t="shared" si="0"/>
@@ -1993,22 +1991,22 @@
         <v>/mng_activity/disciplines</v>
       </c>
       <c r="G29" s="25" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="H29" s="22"/>
     </row>
-    <row r="30" spans="1:8" ht="19.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" ht="19.899999999999999" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A30" s="25" t="s">
         <v>42</v>
       </c>
       <c r="B30" s="25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C30" s="22" t="s">
         <v>30</v>
       </c>
       <c r="D30" s="25" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E30" s="25" t="str">
         <f t="shared" si="0"/>
@@ -2019,22 +2017,22 @@
         <v>/mng_activity/courses</v>
       </c>
       <c r="G30" s="25" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="H30" s="22"/>
     </row>
-    <row r="31" spans="1:8" ht="19.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" ht="19.899999999999999" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A31" s="25" t="s">
         <v>44</v>
       </c>
       <c r="B31" s="25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C31" s="22" t="s">
         <v>31</v>
       </c>
       <c r="D31" s="25" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E31" s="25" t="str">
         <f t="shared" si="0"/>
@@ -2045,22 +2043,22 @@
         <v>/mng_activity/packages</v>
       </c>
       <c r="G31" s="25" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="H31" s="22"/>
     </row>
-    <row r="32" spans="1:8" ht="19.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" ht="19.899999999999999" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A32" s="25" t="s">
         <v>43</v>
       </c>
       <c r="B32" s="25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C32" s="22" t="s">
         <v>32</v>
       </c>
       <c r="D32" s="25" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E32" s="25" t="str">
         <f t="shared" si="0"/>
@@ -2071,22 +2069,22 @@
         <v>/mng_activity/rooms</v>
       </c>
       <c r="G32" s="25" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="H32" s="22"/>
     </row>
-    <row r="33" spans="1:8" ht="19.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" ht="19.899999999999999" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A33" s="25" t="s">
         <v>45</v>
       </c>
       <c r="B33" s="25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C33" s="22" t="s">
         <v>33</v>
       </c>
       <c r="D33" s="25" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E33" s="25" t="str">
         <f t="shared" si="0"/>
@@ -2097,22 +2095,22 @@
         <v>/mng_activity/scheduling</v>
       </c>
       <c r="G33" s="25" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="H33" s="22"/>
     </row>
-    <row r="34" spans="1:8" ht="19.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" ht="19.899999999999999" hidden="1" customHeight="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A34" s="26" t="s">
         <v>46</v>
       </c>
       <c r="B34" s="26" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C34" s="23" t="s">
         <v>8</v>
       </c>
       <c r="D34" s="26" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E34" s="26" t="str">
         <f t="shared" si="0"/>
@@ -2123,22 +2121,23 @@
         <v>/report_stats</v>
       </c>
       <c r="G34" s="26" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="H34" s="23" t="s">
-        <v>112</v>
-      </c>
-    </row>
+        <v>110</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" collapsed="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <dataConsolidate/>
   <dataValidations count="3">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B2:B34" xr:uid="{F340BA2D-9D43-4A9F-86F9-B281B429D2E7}">
-      <formula1>RefTipo</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F36" xr:uid="{C7F42672-59D8-4A95-9804-4B94DD14E8F6}">
       <formula1>RefView_route</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G34" xr:uid="{DFF187B0-2821-4C72-B394-0420A8E90996}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B7:B34 B2:B6" xr:uid="{F340BA2D-9D43-4A9F-86F9-B281B429D2E7}">
+      <formula1>RefTipo</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G7:G34 G2:G6" xr:uid="{DFF187B0-2821-4C72-B394-0420A8E90996}">
       <formula1>RefController_nome</formula1>
     </dataValidation>
   </dataValidations>
@@ -2161,105 +2160,105 @@
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="6" width="25.109375" customWidth="1"/>
-    <col min="7" max="7" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="6" width="25.140625" customWidth="1"/>
+    <col min="7" max="7" width="24.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="19" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.77734375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1" t="s">
         <v>75</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E2" s="5"/>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B3" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="E1" t="s">
-        <v>79</v>
-      </c>
-      <c r="F1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="2" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="D2" t="s">
-        <v>82</v>
-      </c>
-      <c r="E2" s="5"/>
-    </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B3" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>77</v>
-      </c>
       <c r="E3" s="5"/>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E4" s="5"/>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D5" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D6" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B7" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="D7" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B8" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="D8" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B7" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="D7" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B8" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="D8" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="D9" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B15" s="17"/>
       <c r="C15" s="16"/>
       <c r="D15" s="16"/>
       <c r="E15" s="16"/>
     </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B16" s="9"/>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
@@ -2267,7 +2266,7 @@
       <c r="F16" s="10"/>
       <c r="G16" s="8"/>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="9"/>
       <c r="C17" s="6"/>
       <c r="D17" s="7"/>
@@ -2275,7 +2274,7 @@
       <c r="F17" s="10"/>
       <c r="G17" s="8"/>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="9"/>
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
@@ -2283,7 +2282,7 @@
       <c r="F18" s="10"/>
       <c r="G18" s="8"/>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="9"/>
       <c r="C19" s="6"/>
       <c r="D19" s="7"/>
@@ -2291,7 +2290,7 @@
       <c r="F19" s="10"/>
       <c r="G19" s="8"/>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="9"/>
       <c r="C20" s="6"/>
       <c r="D20" s="7"/>
@@ -2299,7 +2298,7 @@
       <c r="F20" s="10"/>
       <c r="G20" s="8"/>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="9"/>
       <c r="C21" s="6"/>
       <c r="D21" s="7"/>
@@ -2307,7 +2306,7 @@
       <c r="F21" s="10"/>
       <c r="G21" s="8"/>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="9"/>
       <c r="C22" s="6"/>
       <c r="D22" s="7"/>
@@ -2315,7 +2314,7 @@
       <c r="F22" s="10"/>
       <c r="G22" s="8"/>
     </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" s="9"/>
       <c r="C23" s="6"/>
       <c r="D23" s="7"/>
@@ -2323,7 +2322,7 @@
       <c r="F23" s="10"/>
       <c r="G23" s="8"/>
     </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" s="9"/>
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
@@ -2331,7 +2330,7 @@
       <c r="F24" s="10"/>
       <c r="G24" s="8"/>
     </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" s="9"/>
       <c r="C25" s="6"/>
       <c r="D25" s="7"/>
@@ -2339,7 +2338,7 @@
       <c r="F25" s="10"/>
       <c r="G25" s="8"/>
     </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" s="9"/>
       <c r="C26" s="6"/>
       <c r="D26" s="7"/>
@@ -2347,7 +2346,7 @@
       <c r="F26" s="10"/>
       <c r="G26" s="8"/>
     </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" s="9"/>
       <c r="C27" s="6"/>
       <c r="D27" s="7"/>
@@ -2355,13 +2354,13 @@
       <c r="F27" s="10"/>
       <c r="G27" s="8"/>
     </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D28" s="7"/>
       <c r="E28" s="10"/>
       <c r="F28" s="10"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="D13:D29">
+  <sortState ref="D13:D29">
     <sortCondition ref="D13"/>
   </sortState>
   <dataConsolidate/>

</xml_diff>

<commit_message>
Aggiunta view dei fondatori
modificati anche i codici delle gabbie logiche
</commit_message>
<xml_diff>
--- a/Documentazioni/Codifica pagine sito.xlsx
+++ b/Documentazioni/Codifica pagine sito.xlsx
@@ -1,18 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
   <workbookPr filterPrivacy="1" codeName="Questa_cartella_di_lavoro"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BD3C96D-B3F6-4E6B-A668-2560D5784ACA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5DF7088-6006-4D9F-82D6-4D19D411D0CA}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
     <sheet name="Foglio utile" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Main!$A$1:$H$34</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Main!$A$1:$H$35</definedName>
     <definedName name="RefController_nome">Controller[Lista Controller]</definedName>
     <definedName name="RefTipo">Tipo[]</definedName>
   </definedNames>
@@ -24,6 +24,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="143">
   <si>
     <t>Nome gabbia logica</t>
   </si>
@@ -147,9 +148,6 @@
     <t>M211</t>
   </si>
   <si>
-    <t>M212</t>
-  </si>
-  <si>
     <t>M220</t>
   </si>
   <si>
@@ -451,6 +449,18 @@
   </si>
   <si>
     <t>A025</t>
+  </si>
+  <si>
+    <t>Fondatori</t>
+  </si>
+  <si>
+    <t>M213</t>
+  </si>
+  <si>
+    <t>M216</t>
+  </si>
+  <si>
+    <t>founders</t>
   </si>
 </sst>
 </file>
@@ -653,6 +663,53 @@
   </cellStyles>
   <dxfs count="17">
     <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <strike val="0"/>
         <outline val="0"/>
@@ -666,9 +723,6 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -716,6 +770,14 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <strike val="0"/>
         <outline val="0"/>
@@ -737,12 +799,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -758,24 +815,6 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -814,48 +853,19 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
       <font>
-        <b/>
-        <i val="0"/>
         <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="11"/>
+        <sz val="10"/>
         <color theme="1"/>
         <name val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -871,34 +881,34 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{905F6574-56C3-4E36-86AD-16F4E970F9D2}" name="Tabella4" displayName="Tabella4" ref="A1:H34" dataDxfId="13">
-  <autoFilter ref="A1:H34" xr:uid="{34684D11-7ACD-45A4-AA96-0CE6C7239D98}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{905F6574-56C3-4E36-86AD-16F4E970F9D2}" name="Tabella4" displayName="Tabella4" ref="A1:H35" dataDxfId="16">
+  <autoFilter ref="A1:H35" xr:uid="{34684D11-7ACD-45A4-AA96-0CE6C7239D98}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{E7D98D43-EB7B-46CE-B0B0-C555D83773A6}" name="Codice gabbia logica" dataDxfId="11" totalsRowDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{DB39DBBD-231C-4393-B53A-31DA54EF2B6B}" name="Tipo" dataDxfId="9" totalsRowDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{267C913B-0C60-4A11-8D31-6129F6A6699A}" name="Nome gabbia logica" dataDxfId="7" totalsRowDxfId="8"/>
-    <tableColumn id="5" xr3:uid="{251AE08F-697F-47EC-9FB6-7CEF1CCB916E}" name="view" dataDxfId="5" totalsRowDxfId="6"/>
-    <tableColumn id="6" xr3:uid="{E87D751D-6B30-48F2-95B8-E2DCF4172ECA}" name="Nome file" dataDxfId="4">
+    <tableColumn id="1" xr3:uid="{E7D98D43-EB7B-46CE-B0B0-C555D83773A6}" name="Codice gabbia logica" dataDxfId="15" totalsRowDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{DB39DBBD-231C-4393-B53A-31DA54EF2B6B}" name="Tipo" dataDxfId="13" totalsRowDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{267C913B-0C60-4A11-8D31-6129F6A6699A}" name="Nome gabbia logica" dataDxfId="11" totalsRowDxfId="10"/>
+    <tableColumn id="5" xr3:uid="{251AE08F-697F-47EC-9FB6-7CEF1CCB916E}" name="view" dataDxfId="9" totalsRowDxfId="8"/>
+    <tableColumn id="6" xr3:uid="{E87D751D-6B30-48F2-95B8-E2DCF4172ECA}" name="Nome file" dataDxfId="7">
       <calculatedColumnFormula>IF($D2="Da definire",$D2,_xlfn.CONCAT($D2,".blade.php"))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{CAF26B0C-D3E2-4A71-A7C5-519E983C334C}" name="Rotta" dataDxfId="3">
+    <tableColumn id="8" xr3:uid="{CAF26B0C-D3E2-4A71-A7C5-519E983C334C}" name="Rotta" dataDxfId="6">
       <calculatedColumnFormula>"/" &amp; D2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{C8498EB6-2C5F-47B9-B993-99AA78B7EEAA}" name="Controller" dataDxfId="2"/>
-    <tableColumn id="10" xr3:uid="{E6E3AEA2-F019-429B-B8B1-54C1BCAF6687}" name="Commento" dataDxfId="0" totalsRowDxfId="1"/>
+    <tableColumn id="9" xr3:uid="{C8498EB6-2C5F-47B9-B993-99AA78B7EEAA}" name="Controller" dataDxfId="5"/>
+    <tableColumn id="10" xr3:uid="{E6E3AEA2-F019-429B-B8B1-54C1BCAF6687}" name="Commento" dataDxfId="4" totalsRowDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium12" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{45120F09-8607-4F6A-A989-7184307236A1}" name="Tipo" displayName="Tipo" ref="B1:B8" totalsRowShown="0" headerRowDxfId="16" tableBorderDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{45120F09-8607-4F6A-A989-7184307236A1}" name="Tipo" displayName="Tipo" ref="B1:B8" totalsRowShown="0" headerRowDxfId="2" tableBorderDxfId="1">
   <autoFilter ref="B1:B8" xr:uid="{B0803B6A-3448-4A89-AC43-1127F3DBD833}"/>
-  <sortState ref="B2:B8">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:B8">
     <sortCondition ref="B1:B8"/>
   </sortState>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{95A47413-48BC-4507-BE9E-0DFA740DC4DC}" name="Tipi di pagina" dataDxfId="14"/>
+    <tableColumn id="1" xr3:uid="{95A47413-48BC-4507-BE9E-0DFA740DC4DC}" name="Tipi di pagina" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1182,67 +1192,67 @@
   <sheetPr codeName="Foglio2"/>
   <dimension ref="A1:I35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" topLeftCell="D20" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H26" sqref="H25:H26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" outlineLevelRow="3" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" outlineLevelRow="3" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.5703125" style="14" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.5546875" style="14" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13" style="12" customWidth="1"/>
-    <col min="3" max="3" width="35.5703125" style="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" style="15" customWidth="1"/>
-    <col min="5" max="5" width="24.42578125" style="13" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="29.28515625" style="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.5546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.33203125" style="15" customWidth="1"/>
+    <col min="5" max="5" width="24.44140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.33203125" style="13" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17" style="13" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="89.7109375" style="11" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="28.7109375" style="13" customWidth="1"/>
-    <col min="10" max="11" width="8.85546875" style="13"/>
+    <col min="8" max="8" width="89.6640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="28.6640625" style="13" customWidth="1"/>
+    <col min="10" max="11" width="8.88671875" style="13"/>
     <col min="12" max="12" width="19" style="13" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="8.85546875" style="13"/>
+    <col min="13" max="16384" width="8.88671875" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C1" s="11" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F1" s="13" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G1" s="13" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H1" s="11" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C2" s="19" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D2" s="20" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E2" s="18" t="str">
-        <f t="shared" ref="E2:E34" si="0">IF($D2="Da definire",$D2,_xlfn.CONCAT($D2,".blade.php"))</f>
+        <f t="shared" ref="E2:E35" si="0">IF($D2="Da definire",$D2,_xlfn.CONCAT($D2,".blade.php"))</f>
         <v>welcome.blade.php</v>
       </c>
       <c r="F2" s="18" t="str">
@@ -1250,52 +1260,52 @@
         <v>/welcome</v>
       </c>
       <c r="G2" s="18" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H2" s="19" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="18" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C3" s="19" t="s">
         <v>3</v>
       </c>
       <c r="D3" s="20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E3" s="18" t="str">
         <f t="shared" si="0"/>
         <v>boot.blade.php</v>
       </c>
       <c r="F3" s="18" t="str">
-        <f t="shared" ref="F3:F34" si="1">"/" &amp; D3</f>
+        <f t="shared" ref="F3:F35" si="1">"/" &amp; D3</f>
         <v>/boot</v>
       </c>
       <c r="G3" s="18" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H3" s="19" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C4" s="19" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D4" s="20" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E4" s="18" t="str">
         <f t="shared" si="0"/>
@@ -1306,24 +1316,24 @@
         <v>/boot_asd_done</v>
       </c>
       <c r="G4" s="18" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H4" s="19" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="18" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C5" s="19" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E5" s="18" t="str">
         <f>IF($D5="Da definire",$D5,_xlfn.CONCAT($D5,".blade.php"))</f>
@@ -1334,24 +1344,24 @@
         <v>/boot_socio</v>
       </c>
       <c r="G5" s="18" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H5" s="19" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D6" s="20" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E6" s="18" t="str">
         <f t="shared" si="0"/>
@@ -1362,24 +1372,24 @@
         <v>/boot_finished</v>
       </c>
       <c r="G6" s="18" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H6" s="19" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="18" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D7" s="20" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E7" s="18" t="str">
         <f t="shared" si="0"/>
@@ -1390,25 +1400,25 @@
         <v>/login</v>
       </c>
       <c r="G7" s="18" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H7" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="I7" s="12"/>
+    </row>
+    <row r="8" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="I7" s="12"/>
-    </row>
-    <row r="8" spans="1:9" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="18" t="s">
-        <v>54</v>
-      </c>
       <c r="B8" s="18" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C8" s="19" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D8" s="20" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E8" s="18" t="str">
         <f t="shared" si="0"/>
@@ -1419,25 +1429,25 @@
         <v>/login_done</v>
       </c>
       <c r="G8" s="18" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H8" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="I8" s="12"/>
+    </row>
+    <row r="9" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="I8" s="12"/>
-    </row>
-    <row r="9" spans="1:9" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="18" t="s">
-        <v>56</v>
-      </c>
       <c r="B9" s="18" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C9" s="19" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D9" s="20" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E9" s="18" t="str">
         <f t="shared" si="0"/>
@@ -1448,25 +1458,25 @@
         <v>/login_failure</v>
       </c>
       <c r="G9" s="18" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H9" s="19" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I9" s="12"/>
     </row>
-    <row r="10" spans="1:9" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="18" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C10" s="19" t="s">
         <v>9</v>
       </c>
       <c r="D10" s="20" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E10" s="18" t="str">
         <f t="shared" si="0"/>
@@ -1477,24 +1487,24 @@
         <v>/our_team</v>
       </c>
       <c r="G10" s="18" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H10" s="19" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="18" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B11" s="18" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C11" s="19" t="s">
         <v>10</v>
       </c>
       <c r="D11" s="20" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E11" s="18" t="str">
         <f t="shared" si="0"/>
@@ -1505,24 +1515,24 @@
         <v>/contacts</v>
       </c>
       <c r="G11" s="18" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H11" s="19" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="B12" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="C12" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="B12" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="C12" s="19" t="s">
-        <v>64</v>
-      </c>
       <c r="D12" s="20" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E12" s="18" t="str">
         <f t="shared" si="0"/>
@@ -1533,24 +1543,24 @@
         <v>/settings_account</v>
       </c>
       <c r="G12" s="18" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H12" s="19" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="28" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B13" s="28" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C13" s="24" t="s">
         <v>4</v>
       </c>
       <c r="D13" s="28" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E13" s="28" t="str">
         <f t="shared" si="0"/>
@@ -1561,24 +1571,24 @@
         <v>/homepage</v>
       </c>
       <c r="G13" s="28" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H13" s="24" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="19.899999999999999" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="19.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A14" s="26" t="s">
         <v>18</v>
       </c>
       <c r="B14" s="26" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C14" s="23" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D14" s="26" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E14" s="26" t="str">
         <f t="shared" si="0"/>
@@ -1589,24 +1599,24 @@
         <v>/managment</v>
       </c>
       <c r="G14" s="26" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H14" s="23" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="19.899999999999999" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="19.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A15" s="27" t="s">
         <v>19</v>
       </c>
       <c r="B15" s="27" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C15" s="21" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D15" s="27" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E15" s="27" t="str">
         <f t="shared" si="0"/>
@@ -1617,24 +1627,24 @@
         <v>/staff</v>
       </c>
       <c r="G15" s="27" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H15" s="21" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="19.899999999999999" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="19.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A16" s="25" t="s">
         <v>20</v>
       </c>
       <c r="B16" s="25" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C16" s="22" t="s">
         <v>12</v>
       </c>
       <c r="D16" s="25" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E16" s="25" t="str">
         <f t="shared" si="0"/>
@@ -1645,22 +1655,22 @@
         <v>/staff/collab-int</v>
       </c>
       <c r="G16" s="25" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H16" s="22"/>
     </row>
-    <row r="17" spans="1:8" ht="19.899999999999999" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="19.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A17" s="25" t="s">
         <v>21</v>
       </c>
       <c r="B17" s="25" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C17" s="22" t="s">
         <v>13</v>
       </c>
       <c r="D17" s="25" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E17" s="25" t="str">
         <f t="shared" si="0"/>
@@ -1671,22 +1681,22 @@
         <v>/staff/collab-ext</v>
       </c>
       <c r="G17" s="25" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H17" s="22"/>
     </row>
-    <row r="18" spans="1:8" ht="19.899999999999999" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="19.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A18" s="25" t="s">
         <v>22</v>
       </c>
       <c r="B18" s="25" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C18" s="22" t="s">
         <v>14</v>
       </c>
       <c r="D18" s="25" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E18" s="25" t="str">
         <f t="shared" si="0"/>
@@ -1697,22 +1707,22 @@
         <v>/staff/trainee</v>
       </c>
       <c r="G18" s="25" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H18" s="22"/>
     </row>
-    <row r="19" spans="1:8" ht="19.899999999999999" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="19.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A19" s="25" t="s">
         <v>23</v>
       </c>
       <c r="B19" s="25" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C19" s="22" t="s">
         <v>15</v>
       </c>
       <c r="D19" s="25" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E19" s="25" t="str">
         <f t="shared" si="0"/>
@@ -1723,22 +1733,22 @@
         <v>/staff/teacher</v>
       </c>
       <c r="G19" s="25" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H19" s="22"/>
     </row>
-    <row r="20" spans="1:8" ht="19.899999999999999" hidden="1" customHeight="1" outlineLevel="2" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="19.95" customHeight="1" outlineLevel="2" collapsed="1" x14ac:dyDescent="0.3">
       <c r="A20" s="27" t="s">
         <v>24</v>
       </c>
       <c r="B20" s="27" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C20" s="21" t="s">
         <v>11</v>
       </c>
       <c r="D20" s="27" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E20" s="27" t="str">
         <f t="shared" si="0"/>
@@ -1749,24 +1759,24 @@
         <v>/payments</v>
       </c>
       <c r="G20" s="27" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H20" s="21" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="19.899999999999999" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="19.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A21" s="25" t="s">
         <v>25</v>
       </c>
       <c r="B21" s="25" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C21" s="22" t="s">
         <v>16</v>
       </c>
       <c r="D21" s="25" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E21" s="25" t="str">
         <f t="shared" si="0"/>
@@ -1777,22 +1787,22 @@
         <v>/payments/outflow</v>
       </c>
       <c r="G21" s="25" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H21" s="22"/>
     </row>
-    <row r="22" spans="1:8" ht="19.899999999999999" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="19.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A22" s="25" t="s">
         <v>26</v>
       </c>
       <c r="B22" s="25" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C22" s="22" t="s">
         <v>17</v>
       </c>
       <c r="D22" s="25" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E22" s="25" t="str">
         <f t="shared" si="0"/>
@@ -1803,22 +1813,22 @@
         <v>/payments/earn</v>
       </c>
       <c r="G22" s="25" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H22" s="22"/>
     </row>
-    <row r="23" spans="1:8" ht="19.899999999999999" hidden="1" customHeight="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" ht="19.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A23" s="26" t="s">
         <v>27</v>
       </c>
       <c r="B23" s="26" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C23" s="23" t="s">
         <v>6</v>
       </c>
       <c r="D23" s="26" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E23" s="26" t="str">
         <f t="shared" si="0"/>
@@ -1829,24 +1839,24 @@
         <v>/secretariat</v>
       </c>
       <c r="G23" s="26" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H23" s="23" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="19.899999999999999" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="19.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A24" s="27" t="s">
         <v>28</v>
       </c>
       <c r="B24" s="27" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C24" s="21" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D24" s="27" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E24" s="27" t="str">
         <f t="shared" si="0"/>
@@ -1857,287 +1867,312 @@
         <v>/subscribers</v>
       </c>
       <c r="G24" s="27" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H24" s="21" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="19.899999999999999" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="19.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A25" s="25" t="s">
         <v>37</v>
       </c>
       <c r="B25" s="25" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C25" s="22" t="s">
-        <v>34</v>
+        <v>139</v>
       </c>
       <c r="D25" s="25" t="s">
-        <v>121</v>
+        <v>142</v>
       </c>
       <c r="E25" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>students.blade.php</v>
+        <v>founders.blade.php</v>
       </c>
       <c r="F25" s="25" t="str">
         <f>$F$24 &amp; "/" &amp; D25</f>
-        <v>/subscribers/students</v>
+        <v>/subscribers/founders</v>
       </c>
       <c r="G25" s="25" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H25" s="22"/>
     </row>
-    <row r="26" spans="1:8" ht="19.899999999999999" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" ht="19.95" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A26" s="25" t="s">
-        <v>38</v>
+        <v>140</v>
       </c>
       <c r="B26" s="25" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C26" s="22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D26" s="25" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E26" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>cards.blade.php</v>
+        <v>students.blade.php</v>
       </c>
       <c r="F26" s="25" t="str">
         <f>$F$24 &amp; "/" &amp; D26</f>
+        <v>/subscribers/students</v>
+      </c>
+      <c r="G26" s="25" t="s">
+        <v>128</v>
+      </c>
+      <c r="H26" s="22"/>
+    </row>
+    <row r="27" spans="1:8" ht="19.95" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.3">
+      <c r="A27" s="25" t="s">
+        <v>141</v>
+      </c>
+      <c r="B27" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="C27" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="D27" s="25" t="s">
+        <v>121</v>
+      </c>
+      <c r="E27" s="25" t="str">
+        <f t="shared" si="0"/>
+        <v>cards.blade.php</v>
+      </c>
+      <c r="F27" s="25" t="str">
+        <f>$F$24 &amp; "/" &amp; D27</f>
         <v>/subscribers/cards</v>
       </c>
-      <c r="G26" s="25" t="s">
-        <v>129</v>
-      </c>
-      <c r="H26" s="22"/>
-    </row>
-    <row r="27" spans="1:8" ht="19.899999999999999" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A27" s="27" t="s">
-        <v>39</v>
-      </c>
-      <c r="B27" s="27" t="s">
-        <v>68</v>
-      </c>
-      <c r="C27" s="21" t="s">
+      <c r="G27" s="25" t="s">
+        <v>128</v>
+      </c>
+      <c r="H27" s="22"/>
+    </row>
+    <row r="28" spans="1:8" ht="19.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
+      <c r="A28" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="B28" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="C28" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="D27" s="27" t="s">
-        <v>123</v>
-      </c>
-      <c r="E27" s="27" t="str">
+      <c r="D28" s="27" t="s">
+        <v>122</v>
+      </c>
+      <c r="E28" s="27" t="str">
         <f t="shared" si="0"/>
         <v>vendors.blade.php</v>
       </c>
-      <c r="F27" s="27" t="str">
+      <c r="F28" s="27" t="str">
         <f t="shared" si="1"/>
         <v>/vendors</v>
       </c>
-      <c r="G27" s="27" t="s">
-        <v>131</v>
-      </c>
-      <c r="H27" s="21"/>
-    </row>
-    <row r="28" spans="1:8" ht="19.899999999999999" hidden="1" customHeight="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="26" t="s">
-        <v>40</v>
-      </c>
-      <c r="B28" s="26" t="s">
-        <v>69</v>
-      </c>
-      <c r="C28" s="23" t="s">
+      <c r="G28" s="27" t="s">
+        <v>130</v>
+      </c>
+      <c r="H28" s="21"/>
+    </row>
+    <row r="29" spans="1:8" ht="19.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="26" t="s">
+        <v>39</v>
+      </c>
+      <c r="B29" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="C29" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="D28" s="26" t="s">
-        <v>106</v>
-      </c>
-      <c r="E28" s="26" t="str">
+      <c r="D29" s="26" t="s">
+        <v>105</v>
+      </c>
+      <c r="E29" s="26" t="str">
         <f t="shared" si="0"/>
         <v>mng_activity.blade.php</v>
       </c>
-      <c r="F28" s="26" t="str">
+      <c r="F29" s="26" t="str">
         <f t="shared" si="1"/>
         <v>/mng_activity</v>
       </c>
-      <c r="G28" s="26" t="s">
-        <v>107</v>
-      </c>
-      <c r="H28" s="23" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" ht="19.899999999999999" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A29" s="25" t="s">
+      <c r="G29" s="26" t="s">
+        <v>106</v>
+      </c>
+      <c r="H29" s="23" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="19.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
+      <c r="A30" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="B30" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="C30" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="D30" s="25" t="s">
+        <v>123</v>
+      </c>
+      <c r="E30" s="25" t="str">
+        <f t="shared" si="0"/>
+        <v>disciplines.blade.php</v>
+      </c>
+      <c r="F30" s="25" t="str">
+        <f>$F$29 &amp; "/" &amp; D30</f>
+        <v>/mng_activity/disciplines</v>
+      </c>
+      <c r="G30" s="25" t="s">
+        <v>131</v>
+      </c>
+      <c r="H30" s="22"/>
+    </row>
+    <row r="31" spans="1:8" ht="19.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
+      <c r="A31" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="B29" s="25" t="s">
-        <v>68</v>
-      </c>
-      <c r="C29" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="D29" s="25" t="s">
+      <c r="B31" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="C31" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="D31" s="25" t="s">
         <v>124</v>
       </c>
-      <c r="E29" s="25" t="str">
-        <f t="shared" si="0"/>
-        <v>disciplines.blade.php</v>
-      </c>
-      <c r="F29" s="25" t="str">
-        <f>$F$28 &amp; "/" &amp; D29</f>
-        <v>/mng_activity/disciplines</v>
-      </c>
-      <c r="G29" s="25" t="s">
-        <v>132</v>
-      </c>
-      <c r="H29" s="22"/>
-    </row>
-    <row r="30" spans="1:8" ht="19.899999999999999" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A30" s="25" t="s">
-        <v>42</v>
-      </c>
-      <c r="B30" s="25" t="s">
-        <v>68</v>
-      </c>
-      <c r="C30" s="22" t="s">
-        <v>30</v>
-      </c>
-      <c r="D30" s="25" t="s">
-        <v>125</v>
-      </c>
-      <c r="E30" s="25" t="str">
+      <c r="E31" s="25" t="str">
         <f t="shared" si="0"/>
         <v>courses.blade.php</v>
       </c>
-      <c r="F30" s="25" t="str">
-        <f t="shared" ref="F30:F33" si="3">$F$28 &amp; "/" &amp; D30</f>
+      <c r="F31" s="25" t="str">
+        <f t="shared" ref="F31:F34" si="3">$F$29 &amp; "/" &amp; D31</f>
         <v>/mng_activity/courses</v>
       </c>
-      <c r="G30" s="25" t="s">
-        <v>132</v>
-      </c>
-      <c r="H30" s="22"/>
-    </row>
-    <row r="31" spans="1:8" ht="19.899999999999999" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A31" s="25" t="s">
-        <v>44</v>
-      </c>
-      <c r="B31" s="25" t="s">
-        <v>68</v>
-      </c>
-      <c r="C31" s="22" t="s">
+      <c r="G31" s="25" t="s">
+        <v>131</v>
+      </c>
+      <c r="H31" s="22"/>
+    </row>
+    <row r="32" spans="1:8" ht="19.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
+      <c r="A32" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="B32" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="C32" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="D31" s="25" t="s">
-        <v>127</v>
-      </c>
-      <c r="E31" s="25" t="str">
+      <c r="D32" s="25" t="s">
+        <v>126</v>
+      </c>
+      <c r="E32" s="25" t="str">
         <f t="shared" si="0"/>
         <v>packages.blade.php</v>
       </c>
-      <c r="F31" s="25" t="str">
+      <c r="F32" s="25" t="str">
         <f t="shared" si="3"/>
         <v>/mng_activity/packages</v>
       </c>
-      <c r="G31" s="25" t="s">
-        <v>132</v>
-      </c>
-      <c r="H31" s="22"/>
-    </row>
-    <row r="32" spans="1:8" ht="19.899999999999999" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A32" s="25" t="s">
-        <v>43</v>
-      </c>
-      <c r="B32" s="25" t="s">
-        <v>68</v>
-      </c>
-      <c r="C32" s="22" t="s">
+      <c r="G32" s="25" t="s">
+        <v>131</v>
+      </c>
+      <c r="H32" s="22"/>
+    </row>
+    <row r="33" spans="1:8" ht="19.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
+      <c r="A33" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="B33" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="C33" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="D32" s="25" t="s">
-        <v>126</v>
-      </c>
-      <c r="E32" s="25" t="str">
+      <c r="D33" s="25" t="s">
+        <v>125</v>
+      </c>
+      <c r="E33" s="25" t="str">
         <f t="shared" si="0"/>
         <v>rooms.blade.php</v>
       </c>
-      <c r="F32" s="25" t="str">
+      <c r="F33" s="25" t="str">
         <f t="shared" si="3"/>
         <v>/mng_activity/rooms</v>
       </c>
-      <c r="G32" s="25" t="s">
-        <v>132</v>
-      </c>
-      <c r="H32" s="22"/>
-    </row>
-    <row r="33" spans="1:8" ht="19.899999999999999" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A33" s="25" t="s">
-        <v>45</v>
-      </c>
-      <c r="B33" s="25" t="s">
-        <v>68</v>
-      </c>
-      <c r="C33" s="22" t="s">
+      <c r="G33" s="25" t="s">
+        <v>131</v>
+      </c>
+      <c r="H33" s="22"/>
+    </row>
+    <row r="34" spans="1:8" ht="19.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
+      <c r="A34" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="B34" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="C34" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="D33" s="25" t="s">
-        <v>128</v>
-      </c>
-      <c r="E33" s="25" t="str">
+      <c r="D34" s="25" t="s">
+        <v>127</v>
+      </c>
+      <c r="E34" s="25" t="str">
         <f t="shared" si="0"/>
         <v>scheduling.blade.php</v>
       </c>
-      <c r="F33" s="25" t="str">
+      <c r="F34" s="25" t="str">
         <f t="shared" si="3"/>
         <v>/mng_activity/scheduling</v>
       </c>
-      <c r="G33" s="25" t="s">
-        <v>132</v>
-      </c>
-      <c r="H33" s="22"/>
-    </row>
-    <row r="34" spans="1:8" ht="19.899999999999999" hidden="1" customHeight="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="26" t="s">
-        <v>46</v>
-      </c>
-      <c r="B34" s="26" t="s">
-        <v>68</v>
-      </c>
-      <c r="C34" s="23" t="s">
+      <c r="G34" s="25" t="s">
+        <v>131</v>
+      </c>
+      <c r="H34" s="22"/>
+    </row>
+    <row r="35" spans="1:8" ht="19.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="B35" s="26" t="s">
+        <v>67</v>
+      </c>
+      <c r="C35" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="D34" s="26" t="s">
-        <v>109</v>
-      </c>
-      <c r="E34" s="26" t="str">
+      <c r="D35" s="26" t="s">
+        <v>108</v>
+      </c>
+      <c r="E35" s="26" t="str">
         <f t="shared" si="0"/>
         <v>report_stats.blade.php</v>
       </c>
-      <c r="F34" s="26" t="str">
+      <c r="F35" s="26" t="str">
         <f t="shared" si="1"/>
         <v>/report_stats</v>
       </c>
-      <c r="G34" s="26" t="s">
-        <v>107</v>
-      </c>
-      <c r="H34" s="23" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" collapsed="1" x14ac:dyDescent="0.25"/>
+      <c r="G35" s="26" t="s">
+        <v>106</v>
+      </c>
+      <c r="H35" s="23" t="s">
+        <v>109</v>
+      </c>
+    </row>
   </sheetData>
   <dataConsolidate/>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F36" xr:uid="{C7F42672-59D8-4A95-9804-4B94DD14E8F6}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F37" xr:uid="{C7F42672-59D8-4A95-9804-4B94DD14E8F6}">
       <formula1>RefView_route</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B7:B34 B2:B6" xr:uid="{F340BA2D-9D43-4A9F-86F9-B281B429D2E7}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B2:B35" xr:uid="{F340BA2D-9D43-4A9F-86F9-B281B429D2E7}">
       <formula1>RefTipo</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G7:G34 G2:G6" xr:uid="{DFF187B0-2821-4C72-B394-0420A8E90996}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G35" xr:uid="{DFF187B0-2821-4C72-B394-0420A8E90996}">
       <formula1>RefController_nome</formula1>
     </dataValidation>
   </dataValidations>
@@ -2160,105 +2195,105 @@
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="6" width="25.140625" customWidth="1"/>
-    <col min="7" max="7" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="6" width="25.109375" customWidth="1"/>
+    <col min="7" max="7" width="24.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="19" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D1" t="s">
         <v>74</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E2" s="5"/>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B3" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="E1" t="s">
-        <v>78</v>
-      </c>
-      <c r="F1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="2" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="D2" t="s">
-        <v>81</v>
-      </c>
-      <c r="E2" s="5"/>
-    </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B3" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>76</v>
-      </c>
       <c r="E3" s="5"/>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B4" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D4" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="E4" s="5"/>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B5" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D5" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B6" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D6" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B7" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="D7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B8" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="E4" s="5"/>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B5" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="D5" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B6" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="D8" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B7" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="D7" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B8" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="D8" t="s">
+    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="D9" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="D9" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B15" s="17"/>
       <c r="C15" s="16"/>
       <c r="D15" s="16"/>
       <c r="E15" s="16"/>
     </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B16" s="9"/>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
@@ -2266,7 +2301,7 @@
       <c r="F16" s="10"/>
       <c r="G16" s="8"/>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B17" s="9"/>
       <c r="C17" s="6"/>
       <c r="D17" s="7"/>
@@ -2274,7 +2309,7 @@
       <c r="F17" s="10"/>
       <c r="G17" s="8"/>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B18" s="9"/>
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
@@ -2282,7 +2317,7 @@
       <c r="F18" s="10"/>
       <c r="G18" s="8"/>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B19" s="9"/>
       <c r="C19" s="6"/>
       <c r="D19" s="7"/>
@@ -2290,7 +2325,7 @@
       <c r="F19" s="10"/>
       <c r="G19" s="8"/>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B20" s="9"/>
       <c r="C20" s="6"/>
       <c r="D20" s="7"/>
@@ -2298,7 +2333,7 @@
       <c r="F20" s="10"/>
       <c r="G20" s="8"/>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B21" s="9"/>
       <c r="C21" s="6"/>
       <c r="D21" s="7"/>
@@ -2306,7 +2341,7 @@
       <c r="F21" s="10"/>
       <c r="G21" s="8"/>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B22" s="9"/>
       <c r="C22" s="6"/>
       <c r="D22" s="7"/>
@@ -2314,7 +2349,7 @@
       <c r="F22" s="10"/>
       <c r="G22" s="8"/>
     </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B23" s="9"/>
       <c r="C23" s="6"/>
       <c r="D23" s="7"/>
@@ -2322,7 +2357,7 @@
       <c r="F23" s="10"/>
       <c r="G23" s="8"/>
     </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B24" s="9"/>
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
@@ -2330,7 +2365,7 @@
       <c r="F24" s="10"/>
       <c r="G24" s="8"/>
     </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B25" s="9"/>
       <c r="C25" s="6"/>
       <c r="D25" s="7"/>
@@ -2338,7 +2373,7 @@
       <c r="F25" s="10"/>
       <c r="G25" s="8"/>
     </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B26" s="9"/>
       <c r="C26" s="6"/>
       <c r="D26" s="7"/>
@@ -2346,7 +2381,7 @@
       <c r="F26" s="10"/>
       <c r="G26" s="8"/>
     </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B27" s="9"/>
       <c r="C27" s="6"/>
       <c r="D27" s="7"/>
@@ -2354,13 +2389,13 @@
       <c r="F27" s="10"/>
       <c r="G27" s="8"/>
     </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:7" x14ac:dyDescent="0.3">
       <c r="D28" s="7"/>
       <c r="E28" s="10"/>
       <c r="F28" s="10"/>
     </row>
   </sheetData>
-  <sortState ref="D13:D29">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="D13:D29">
     <sortCondition ref="D13"/>
   </sortState>
   <dataConsolidate/>

</xml_diff>

<commit_message>
Aggiunto il middleware per il redirect alla welcome
- Inserito una rotta di redirect alla welcome con avviso
-  Aggiunto il middleware per filtro alle pagine boot e login
- Rinominato il controller MainControll a BootController
</commit_message>
<xml_diff>
--- a/Documentazioni/Codifica pagine sito.xlsx
+++ b/Documentazioni/Codifica pagine sito.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
   <workbookPr filterPrivacy="1" codeName="Questa_cartella_di_lavoro"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5DF7088-6006-4D9F-82D6-4D19D411D0CA}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E02D93B-CCED-4A51-BBD7-78BE7A4A4789}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -12,7 +12,7 @@
     <sheet name="Foglio utile" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Main!$A$1:$H$35</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Main!$A$1:$H$37</definedName>
     <definedName name="RefController_nome">Controller[Lista Controller]</definedName>
     <definedName name="RefTipo">Tipo[]</definedName>
   </definedNames>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="147">
   <si>
     <t>Nome gabbia logica</t>
   </si>
@@ -283,9 +283,6 @@
     <t>contacts</t>
   </si>
   <si>
-    <t>our_team</t>
-  </si>
-  <si>
     <t>Benvenuto</t>
   </si>
   <si>
@@ -298,9 +295,6 @@
     <t>Registrazione ASD effettuata</t>
   </si>
   <si>
-    <t>login_done</t>
-  </si>
-  <si>
     <t>homepage</t>
   </si>
   <si>
@@ -316,24 +310,12 @@
     <t>Registrazione finita</t>
   </si>
   <si>
-    <t>boot_socio</t>
-  </si>
-  <si>
-    <t>boot_finished</t>
-  </si>
-  <si>
-    <t>login_failure</t>
-  </si>
-  <si>
     <t>Redirect</t>
   </si>
   <si>
     <t>Login effettuato</t>
   </si>
   <si>
-    <t>settings_account</t>
-  </si>
-  <si>
     <t>Amministrazione</t>
   </si>
   <si>
@@ -445,9 +427,6 @@
     <t>Messaggio di registrazione riuscita per il socio fondatore</t>
   </si>
   <si>
-    <t>boot_asd_done</t>
-  </si>
-  <si>
     <t>A025</t>
   </si>
   <si>
@@ -461,6 +440,39 @@
   </si>
   <si>
     <t>founders</t>
+  </si>
+  <si>
+    <t>BootController</t>
+  </si>
+  <si>
+    <t>boot-asd-done</t>
+  </si>
+  <si>
+    <t>boot-socio</t>
+  </si>
+  <si>
+    <t>boot-finished</t>
+  </si>
+  <si>
+    <t>login-done</t>
+  </si>
+  <si>
+    <t>our-team</t>
+  </si>
+  <si>
+    <t>settings-account</t>
+  </si>
+  <si>
+    <t>login-failure</t>
+  </si>
+  <si>
+    <t>A001</t>
+  </si>
+  <si>
+    <t>Redirect a A000</t>
+  </si>
+  <si>
+    <t>Redirect a A000, con avviso di effettuare la registrazione prima</t>
   </si>
 </sst>
 </file>
@@ -881,8 +893,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{905F6574-56C3-4E36-86AD-16F4E970F9D2}" name="Tabella4" displayName="Tabella4" ref="A1:H35" dataDxfId="16">
-  <autoFilter ref="A1:H35" xr:uid="{34684D11-7ACD-45A4-AA96-0CE6C7239D98}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{905F6574-56C3-4E36-86AD-16F4E970F9D2}" name="Tabella4" displayName="Tabella4" ref="A1:H37" dataDxfId="16">
+  <autoFilter ref="A1:H37" xr:uid="{34684D11-7ACD-45A4-AA96-0CE6C7239D98}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{E7D98D43-EB7B-46CE-B0B0-C555D83773A6}" name="Codice gabbia logica" dataDxfId="15" totalsRowDxfId="14"/>
     <tableColumn id="2" xr3:uid="{DB39DBBD-231C-4393-B53A-31DA54EF2B6B}" name="Tipo" dataDxfId="13" totalsRowDxfId="12"/>
@@ -1190,10 +1202,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Foglio2"/>
-  <dimension ref="A1:I35"/>
+  <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D20" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H26" sqref="H25:H26"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" outlineLevelRow="3" x14ac:dyDescent="0.3"/>
@@ -1223,7 +1235,7 @@
         <v>0</v>
       </c>
       <c r="D1" s="13" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E1" s="13" t="s">
         <v>78</v>
@@ -1246,13 +1258,13 @@
         <v>67</v>
       </c>
       <c r="C2" s="19" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D2" s="20" t="s">
         <v>65</v>
       </c>
       <c r="E2" s="18" t="str">
-        <f t="shared" ref="E2:E35" si="0">IF($D2="Da definire",$D2,_xlfn.CONCAT($D2,".blade.php"))</f>
+        <f t="shared" ref="E2:E37" si="0">IF($D2="Da definire",$D2,_xlfn.CONCAT($D2,".blade.php"))</f>
         <v>welcome.blade.php</v>
       </c>
       <c r="F2" s="18" t="str">
@@ -1260,919 +1272,964 @@
         <v>/welcome</v>
       </c>
       <c r="G2" s="18" t="s">
-        <v>75</v>
+        <v>136</v>
       </c>
       <c r="H2" s="19" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="18" t="s">
-        <v>48</v>
-      </c>
+        <v>126</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="19.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="18"/>
       <c r="B3" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="C3" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="20" t="s">
-        <v>79</v>
-      </c>
-      <c r="E3" s="18" t="str">
-        <f t="shared" si="0"/>
-        <v>boot.blade.php</v>
-      </c>
+        <v>92</v>
+      </c>
+      <c r="C3" s="19"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="18"/>
       <c r="F3" s="18" t="str">
-        <f t="shared" ref="F3:F35" si="1">"/" &amp; D3</f>
-        <v>/boot</v>
+        <f>"/" &amp; D3</f>
+        <v>/</v>
       </c>
       <c r="G3" s="18" t="s">
-        <v>75</v>
+        <v>136</v>
       </c>
       <c r="H3" s="19" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="19.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
-        <v>57</v>
+        <v>144</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="C4" s="19" t="s">
-        <v>87</v>
-      </c>
+        <v>92</v>
+      </c>
+      <c r="C4" s="19"/>
       <c r="D4" s="20" t="s">
-        <v>137</v>
+        <v>65</v>
       </c>
       <c r="E4" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>boot_asd_done.blade.php</v>
+        <v>welcome.blade.php</v>
       </c>
       <c r="F4" s="18" t="str">
-        <f t="shared" si="1"/>
-        <v>/boot_asd_done</v>
+        <f>"/" &amp; D4 &amp; "/redirect"</f>
+        <v>/welcome/redirect</v>
       </c>
       <c r="G4" s="18" t="s">
-        <v>75</v>
+        <v>136</v>
       </c>
       <c r="H4" s="19" t="s">
-        <v>134</v>
+        <v>146</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="18" t="s">
-        <v>138</v>
+        <v>48</v>
       </c>
       <c r="B5" s="18" t="s">
         <v>67</v>
       </c>
       <c r="C5" s="19" t="s">
-        <v>92</v>
+        <v>3</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>94</v>
+        <v>79</v>
       </c>
       <c r="E5" s="18" t="str">
-        <f>IF($D5="Da definire",$D5,_xlfn.CONCAT($D5,".blade.php"))</f>
-        <v>boot_socio.blade.php</v>
+        <f t="shared" si="0"/>
+        <v>boot.blade.php</v>
       </c>
       <c r="F5" s="18" t="str">
-        <f>"/" &amp; D5</f>
-        <v>/boot_socio</v>
+        <f t="shared" ref="F5:F37" si="1">"/" &amp; D5</f>
+        <v>/boot</v>
       </c>
       <c r="G5" s="18" t="s">
-        <v>75</v>
+        <v>136</v>
       </c>
       <c r="H5" s="19" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="18" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="B6" s="18" t="s">
         <v>67</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="D6" s="20" t="s">
-        <v>95</v>
+        <v>137</v>
       </c>
       <c r="E6" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>boot_finished.blade.php</v>
+        <v>boot-asd-done.blade.php</v>
       </c>
       <c r="F6" s="18" t="str">
         <f t="shared" si="1"/>
-        <v>/boot_finished</v>
+        <v>/boot-asd-done</v>
       </c>
       <c r="G6" s="18" t="s">
-        <v>75</v>
+        <v>136</v>
       </c>
       <c r="H6" s="19" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="B7" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="C7" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="D7" s="20" t="s">
+        <v>138</v>
+      </c>
+      <c r="E7" s="18" t="str">
+        <f>IF($D7="Da definire",$D7,_xlfn.CONCAT($D7,".blade.php"))</f>
+        <v>boot-socio.blade.php</v>
+      </c>
+      <c r="F7" s="18" t="str">
+        <f>"/" &amp; D7</f>
+        <v>/boot-socio</v>
+      </c>
+      <c r="G7" s="18" t="s">
+        <v>136</v>
+      </c>
+      <c r="H7" s="19" t="s">
+        <v>129</v>
+      </c>
+      <c r="I7" s="12"/>
+    </row>
+    <row r="8" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="B8" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="C8" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="D8" s="20" t="s">
+        <v>139</v>
+      </c>
+      <c r="E8" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>boot-finished.blade.php</v>
+      </c>
+      <c r="F8" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v>/boot-finished</v>
+      </c>
+      <c r="G8" s="18" t="s">
+        <v>136</v>
+      </c>
+      <c r="H8" s="19" t="s">
+        <v>130</v>
+      </c>
+      <c r="I8" s="12"/>
+    </row>
+    <row r="9" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="B7" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="C7" s="19" t="s">
-        <v>86</v>
-      </c>
-      <c r="D7" s="20" t="s">
+      <c r="B9" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="C9" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="E7" s="18" t="str">
+      <c r="D9" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="E9" s="18" t="str">
         <f t="shared" si="0"/>
         <v>login.blade.php</v>
       </c>
-      <c r="F7" s="18" t="str">
+      <c r="F9" s="18" t="str">
         <f t="shared" si="1"/>
         <v>/login</v>
       </c>
-      <c r="G7" s="18" t="s">
-        <v>75</v>
-      </c>
-      <c r="H7" s="19" t="s">
+      <c r="G9" s="18" t="s">
+        <v>136</v>
+      </c>
+      <c r="H9" s="19" t="s">
         <v>52</v>
-      </c>
-      <c r="I7" s="12"/>
-    </row>
-    <row r="8" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="18" t="s">
-        <v>53</v>
-      </c>
-      <c r="B8" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="C8" s="19" t="s">
-        <v>98</v>
-      </c>
-      <c r="D8" s="20" t="s">
-        <v>88</v>
-      </c>
-      <c r="E8" s="18" t="str">
-        <f t="shared" si="0"/>
-        <v>login_done.blade.php</v>
-      </c>
-      <c r="F8" s="18" t="str">
-        <f t="shared" si="1"/>
-        <v>/login_done</v>
-      </c>
-      <c r="G8" s="18" t="s">
-        <v>75</v>
-      </c>
-      <c r="H8" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="I8" s="12"/>
-    </row>
-    <row r="9" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="B9" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="C9" s="19" t="s">
-        <v>91</v>
-      </c>
-      <c r="D9" s="20" t="s">
-        <v>96</v>
-      </c>
-      <c r="E9" s="18" t="str">
-        <f t="shared" si="0"/>
-        <v>login_failure.blade.php</v>
-      </c>
-      <c r="F9" s="18" t="str">
-        <f t="shared" si="1"/>
-        <v>/login_failure</v>
-      </c>
-      <c r="G9" s="18" t="s">
-        <v>75</v>
-      </c>
-      <c r="H9" s="19" t="s">
-        <v>56</v>
       </c>
       <c r="I9" s="12"/>
     </row>
     <row r="10" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="18" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B10" s="18" t="s">
         <v>67</v>
       </c>
       <c r="C10" s="19" t="s">
-        <v>9</v>
+        <v>93</v>
       </c>
       <c r="D10" s="20" t="s">
-        <v>83</v>
+        <v>140</v>
       </c>
       <c r="E10" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>our_team.blade.php</v>
+        <v>login-done.blade.php</v>
       </c>
       <c r="F10" s="18" t="str">
         <f t="shared" si="1"/>
-        <v>/our_team</v>
+        <v>/login-done</v>
       </c>
       <c r="G10" s="18" t="s">
-        <v>75</v>
+        <v>136</v>
       </c>
       <c r="H10" s="19" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="18" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="B11" s="18" t="s">
         <v>67</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>10</v>
+        <v>89</v>
       </c>
       <c r="D11" s="20" t="s">
-        <v>82</v>
+        <v>143</v>
       </c>
       <c r="E11" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>contacts.blade.php</v>
+        <v>login-failure.blade.php</v>
       </c>
       <c r="F11" s="18" t="str">
         <f t="shared" si="1"/>
-        <v>/contacts</v>
+        <v>/login-failure</v>
       </c>
       <c r="G11" s="18" t="s">
-        <v>75</v>
+        <v>136</v>
       </c>
       <c r="H11" s="19" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="18" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B12" s="18" t="s">
         <v>67</v>
       </c>
       <c r="C12" s="19" t="s">
-        <v>63</v>
+        <v>9</v>
       </c>
       <c r="D12" s="20" t="s">
-        <v>99</v>
+        <v>141</v>
       </c>
       <c r="E12" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>settings_account.blade.php</v>
+        <v>our-team.blade.php</v>
       </c>
       <c r="F12" s="18" t="str">
         <f t="shared" si="1"/>
-        <v>/settings_account</v>
+        <v>/our-team</v>
       </c>
       <c r="G12" s="18" t="s">
-        <v>75</v>
+        <v>136</v>
       </c>
       <c r="H12" s="19" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="B13" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="C13" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="E13" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>contacts.blade.php</v>
+      </c>
+      <c r="F13" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v>/contacts</v>
+      </c>
+      <c r="G13" s="18" t="s">
+        <v>136</v>
+      </c>
+      <c r="H13" s="19" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="19.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="B14" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="C14" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="D14" s="20" t="s">
+        <v>142</v>
+      </c>
+      <c r="E14" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>settings-account.blade.php</v>
+      </c>
+      <c r="F14" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v>/settings-account</v>
+      </c>
+      <c r="G14" s="18" t="s">
+        <v>136</v>
+      </c>
+      <c r="H14" s="19" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="28" t="s">
+    <row r="15" spans="1:9" ht="19.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
+      <c r="A15" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="B13" s="28" t="s">
-        <v>67</v>
-      </c>
-      <c r="C13" s="24" t="s">
+      <c r="B15" s="28" t="s">
+        <v>67</v>
+      </c>
+      <c r="C15" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="D13" s="28" t="s">
-        <v>89</v>
-      </c>
-      <c r="E13" s="28" t="str">
+      <c r="D15" s="28" t="s">
+        <v>87</v>
+      </c>
+      <c r="E15" s="28" t="str">
         <f t="shared" si="0"/>
         <v>homepage.blade.php</v>
       </c>
-      <c r="F13" s="28" t="str">
+      <c r="F15" s="28" t="str">
         <f t="shared" si="1"/>
         <v>/homepage</v>
       </c>
-      <c r="G13" s="28" t="s">
+      <c r="G15" s="28" t="s">
         <v>75</v>
       </c>
-      <c r="H13" s="24" t="s">
+      <c r="H15" s="24" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="19.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="26" t="s">
+    <row r="16" spans="1:9" ht="19.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
+      <c r="A16" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="26" t="s">
+      <c r="B16" s="26" t="s">
         <v>68</v>
       </c>
-      <c r="C14" s="23" t="s">
-        <v>100</v>
-      </c>
-      <c r="D14" s="26" t="s">
-        <v>103</v>
-      </c>
-      <c r="E14" s="26" t="str">
+      <c r="C16" s="23" t="s">
+        <v>94</v>
+      </c>
+      <c r="D16" s="26" t="s">
+        <v>97</v>
+      </c>
+      <c r="E16" s="26" t="str">
         <f t="shared" si="0"/>
         <v>managment.blade.php</v>
       </c>
-      <c r="F14" s="26" t="str">
+      <c r="F16" s="26" t="str">
         <f t="shared" si="1"/>
         <v>/managment</v>
       </c>
-      <c r="G14" s="26" t="s">
-        <v>106</v>
-      </c>
-      <c r="H14" s="23" t="s">
+      <c r="G16" s="26" t="s">
+        <v>100</v>
+      </c>
+      <c r="H16" s="23" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="19.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
-      <c r="A15" s="27" t="s">
+    <row r="17" spans="1:8" ht="19.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
+      <c r="A17" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="27" t="s">
-        <v>107</v>
-      </c>
-      <c r="C15" s="21" t="s">
+      <c r="B17" s="27" t="s">
         <v>101</v>
       </c>
-      <c r="D15" s="27" t="s">
-        <v>110</v>
-      </c>
-      <c r="E15" s="27" t="str">
+      <c r="C17" s="21" t="s">
+        <v>95</v>
+      </c>
+      <c r="D17" s="27" t="s">
+        <v>104</v>
+      </c>
+      <c r="E17" s="27" t="str">
         <f t="shared" si="0"/>
         <v>staff.blade.php</v>
       </c>
-      <c r="F15" s="27" t="str">
+      <c r="F17" s="27" t="str">
         <f t="shared" si="1"/>
         <v>/staff</v>
       </c>
-      <c r="G15" s="27" t="s">
-        <v>111</v>
-      </c>
-      <c r="H15" s="21" t="s">
+      <c r="G17" s="27" t="s">
+        <v>105</v>
+      </c>
+      <c r="H17" s="21" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" ht="19.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
-      <c r="A16" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="B16" s="25" t="s">
-        <v>67</v>
-      </c>
-      <c r="C16" s="22" t="s">
-        <v>12</v>
-      </c>
-      <c r="D16" s="25" t="s">
-        <v>112</v>
-      </c>
-      <c r="E16" s="25" t="str">
-        <f t="shared" si="0"/>
-        <v>collab-int.blade.php</v>
-      </c>
-      <c r="F16" s="25" t="str">
-        <f>$F$15 &amp; "/" &amp; D16</f>
-        <v>/staff/collab-int</v>
-      </c>
-      <c r="G16" s="25" t="s">
-        <v>111</v>
-      </c>
-      <c r="H16" s="22"/>
-    </row>
-    <row r="17" spans="1:8" ht="19.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
-      <c r="A17" s="25" t="s">
-        <v>21</v>
-      </c>
-      <c r="B17" s="25" t="s">
-        <v>67</v>
-      </c>
-      <c r="C17" s="22" t="s">
-        <v>13</v>
-      </c>
-      <c r="D17" s="25" t="s">
-        <v>113</v>
-      </c>
-      <c r="E17" s="25" t="str">
-        <f t="shared" si="0"/>
-        <v>collab-ext.blade.php</v>
-      </c>
-      <c r="F17" s="25" t="str">
-        <f t="shared" ref="F17:F18" si="2">$F$15 &amp; "/" &amp; D17</f>
-        <v>/staff/collab-ext</v>
-      </c>
-      <c r="G17" s="25" t="s">
-        <v>111</v>
-      </c>
-      <c r="H17" s="22"/>
     </row>
     <row r="18" spans="1:8" ht="19.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A18" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="C18" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="D18" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="E18" s="25" t="str">
+        <f t="shared" si="0"/>
+        <v>collab-int.blade.php</v>
+      </c>
+      <c r="F18" s="25" t="str">
+        <f>$F$17 &amp; "/" &amp; D18</f>
+        <v>/staff/collab-int</v>
+      </c>
+      <c r="G18" s="25" t="s">
+        <v>105</v>
+      </c>
+      <c r="H18" s="22"/>
+    </row>
+    <row r="19" spans="1:8" ht="19.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
+      <c r="A19" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="C19" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="D19" s="25" t="s">
+        <v>107</v>
+      </c>
+      <c r="E19" s="25" t="str">
+        <f t="shared" si="0"/>
+        <v>collab-ext.blade.php</v>
+      </c>
+      <c r="F19" s="25" t="str">
+        <f t="shared" ref="F19:F20" si="2">$F$17 &amp; "/" &amp; D19</f>
+        <v>/staff/collab-ext</v>
+      </c>
+      <c r="G19" s="25" t="s">
+        <v>105</v>
+      </c>
+      <c r="H19" s="22"/>
+    </row>
+    <row r="20" spans="1:8" ht="19.95" customHeight="1" outlineLevel="2" collapsed="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="B18" s="25" t="s">
-        <v>67</v>
-      </c>
-      <c r="C18" s="22" t="s">
+      <c r="B20" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="C20" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="D18" s="25" t="s">
-        <v>114</v>
-      </c>
-      <c r="E18" s="25" t="str">
+      <c r="D20" s="25" t="s">
+        <v>108</v>
+      </c>
+      <c r="E20" s="25" t="str">
         <f t="shared" si="0"/>
         <v>trainee.blade.php</v>
       </c>
-      <c r="F18" s="25" t="str">
+      <c r="F20" s="25" t="str">
         <f t="shared" si="2"/>
         <v>/staff/trainee</v>
       </c>
-      <c r="G18" s="25" t="s">
-        <v>111</v>
-      </c>
-      <c r="H18" s="22"/>
-    </row>
-    <row r="19" spans="1:8" ht="19.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
-      <c r="A19" s="25" t="s">
+      <c r="G20" s="25" t="s">
+        <v>105</v>
+      </c>
+      <c r="H20" s="22"/>
+    </row>
+    <row r="21" spans="1:8" ht="19.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
+      <c r="A21" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="B19" s="25" t="s">
-        <v>67</v>
-      </c>
-      <c r="C19" s="22" t="s">
+      <c r="B21" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="C21" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="D19" s="25" t="s">
-        <v>115</v>
-      </c>
-      <c r="E19" s="25" t="str">
+      <c r="D21" s="25" t="s">
+        <v>109</v>
+      </c>
+      <c r="E21" s="25" t="str">
         <f t="shared" si="0"/>
         <v>teacher.blade.php</v>
       </c>
-      <c r="F19" s="25" t="str">
-        <f>$F$15 &amp; "/" &amp; D19</f>
+      <c r="F21" s="25" t="str">
+        <f>$F$17 &amp; "/" &amp; D21</f>
         <v>/staff/teacher</v>
       </c>
-      <c r="G19" s="25" t="s">
-        <v>111</v>
-      </c>
-      <c r="H19" s="22"/>
-    </row>
-    <row r="20" spans="1:8" ht="19.95" customHeight="1" outlineLevel="2" collapsed="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="27" t="s">
+      <c r="G21" s="25" t="s">
+        <v>105</v>
+      </c>
+      <c r="H21" s="22"/>
+    </row>
+    <row r="22" spans="1:8" ht="19.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
+      <c r="A22" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="B20" s="27" t="s">
-        <v>107</v>
-      </c>
-      <c r="C20" s="21" t="s">
+      <c r="B22" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="C22" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="D20" s="27" t="s">
-        <v>118</v>
-      </c>
-      <c r="E20" s="27" t="str">
+      <c r="D22" s="27" t="s">
+        <v>112</v>
+      </c>
+      <c r="E22" s="27" t="str">
         <f t="shared" si="0"/>
         <v>payments.blade.php</v>
       </c>
-      <c r="F20" s="27" t="str">
+      <c r="F22" s="27" t="str">
         <f t="shared" si="1"/>
         <v>/payments</v>
       </c>
-      <c r="G20" s="27" t="s">
-        <v>129</v>
-      </c>
-      <c r="H20" s="21" t="s">
+      <c r="G22" s="27" t="s">
+        <v>123</v>
+      </c>
+      <c r="H22" s="21" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="19.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
-      <c r="A21" s="25" t="s">
+    <row r="23" spans="1:8" ht="19.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="B21" s="25" t="s">
-        <v>67</v>
-      </c>
-      <c r="C21" s="22" t="s">
+      <c r="B23" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="C23" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="D21" s="25" t="s">
-        <v>117</v>
-      </c>
-      <c r="E21" s="25" t="str">
+      <c r="D23" s="25" t="s">
+        <v>111</v>
+      </c>
+      <c r="E23" s="25" t="str">
         <f t="shared" si="0"/>
         <v>outflow.blade.php</v>
       </c>
-      <c r="F21" s="25" t="str">
-        <f>$F$20 &amp; "/" &amp; D21</f>
+      <c r="F23" s="25" t="str">
+        <f>$F$22 &amp; "/" &amp; D23</f>
         <v>/payments/outflow</v>
       </c>
-      <c r="G21" s="25" t="s">
-        <v>129</v>
-      </c>
-      <c r="H21" s="22"/>
-    </row>
-    <row r="22" spans="1:8" ht="19.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
-      <c r="A22" s="25" t="s">
+      <c r="G23" s="25" t="s">
+        <v>123</v>
+      </c>
+      <c r="H23" s="22"/>
+    </row>
+    <row r="24" spans="1:8" ht="19.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
+      <c r="A24" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="B22" s="25" t="s">
-        <v>67</v>
-      </c>
-      <c r="C22" s="22" t="s">
+      <c r="B24" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="C24" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="D22" s="25" t="s">
-        <v>116</v>
-      </c>
-      <c r="E22" s="25" t="str">
+      <c r="D24" s="25" t="s">
+        <v>110</v>
+      </c>
+      <c r="E24" s="25" t="str">
         <f t="shared" si="0"/>
         <v>earn.blade.php</v>
       </c>
-      <c r="F22" s="25" t="str">
-        <f>$F$20 &amp; "/" &amp; D22</f>
+      <c r="F24" s="25" t="str">
+        <f>$F$22 &amp; "/" &amp; D24</f>
         <v>/payments/earn</v>
       </c>
-      <c r="G22" s="25" t="s">
-        <v>129</v>
-      </c>
-      <c r="H22" s="22"/>
-    </row>
-    <row r="23" spans="1:8" ht="19.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="26" t="s">
+      <c r="G24" s="25" t="s">
+        <v>123</v>
+      </c>
+      <c r="H24" s="22"/>
+    </row>
+    <row r="25" spans="1:8" ht="19.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
+      <c r="A25" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="B23" s="26" t="s">
+      <c r="B25" s="26" t="s">
         <v>68</v>
       </c>
-      <c r="C23" s="23" t="s">
+      <c r="C25" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="D23" s="26" t="s">
-        <v>104</v>
-      </c>
-      <c r="E23" s="26" t="str">
+      <c r="D25" s="26" t="s">
+        <v>98</v>
+      </c>
+      <c r="E25" s="26" t="str">
         <f t="shared" si="0"/>
         <v>secretariat.blade.php</v>
       </c>
-      <c r="F23" s="26" t="str">
+      <c r="F25" s="26" t="str">
         <f t="shared" si="1"/>
         <v>/secretariat</v>
       </c>
-      <c r="G23" s="26" t="s">
-        <v>106</v>
-      </c>
-      <c r="H23" s="23" t="s">
+      <c r="G25" s="26" t="s">
+        <v>100</v>
+      </c>
+      <c r="H25" s="23" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="19.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
-      <c r="A24" s="27" t="s">
+    <row r="26" spans="1:8" ht="19.95" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.3">
+      <c r="A26" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="B24" s="27" t="s">
-        <v>107</v>
-      </c>
-      <c r="C24" s="21" t="s">
-        <v>102</v>
-      </c>
-      <c r="D24" s="27" t="s">
-        <v>119</v>
-      </c>
-      <c r="E24" s="27" t="str">
+      <c r="B26" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="C26" s="21" t="s">
+        <v>96</v>
+      </c>
+      <c r="D26" s="27" t="s">
+        <v>113</v>
+      </c>
+      <c r="E26" s="27" t="str">
         <f t="shared" si="0"/>
         <v>subscribers.blade.php</v>
       </c>
-      <c r="F24" s="27" t="str">
+      <c r="F26" s="27" t="str">
         <f t="shared" si="1"/>
         <v>/subscribers</v>
       </c>
-      <c r="G24" s="27" t="s">
-        <v>128</v>
-      </c>
-      <c r="H24" s="21" t="s">
+      <c r="G26" s="27" t="s">
+        <v>122</v>
+      </c>
+      <c r="H26" s="21" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" ht="19.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
-      <c r="A25" s="25" t="s">
-        <v>37</v>
-      </c>
-      <c r="B25" s="25" t="s">
-        <v>67</v>
-      </c>
-      <c r="C25" s="22" t="s">
-        <v>139</v>
-      </c>
-      <c r="D25" s="25" t="s">
-        <v>142</v>
-      </c>
-      <c r="E25" s="25" t="str">
-        <f t="shared" si="0"/>
-        <v>founders.blade.php</v>
-      </c>
-      <c r="F25" s="25" t="str">
-        <f>$F$24 &amp; "/" &amp; D25</f>
-        <v>/subscribers/founders</v>
-      </c>
-      <c r="G25" s="25" t="s">
-        <v>128</v>
-      </c>
-      <c r="H25" s="22"/>
-    </row>
-    <row r="26" spans="1:8" ht="19.95" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.3">
-      <c r="A26" s="25" t="s">
-        <v>140</v>
-      </c>
-      <c r="B26" s="25" t="s">
-        <v>67</v>
-      </c>
-      <c r="C26" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="D26" s="25" t="s">
-        <v>120</v>
-      </c>
-      <c r="E26" s="25" t="str">
-        <f t="shared" si="0"/>
-        <v>students.blade.php</v>
-      </c>
-      <c r="F26" s="25" t="str">
-        <f>$F$24 &amp; "/" &amp; D26</f>
-        <v>/subscribers/students</v>
-      </c>
-      <c r="G26" s="25" t="s">
-        <v>128</v>
-      </c>
-      <c r="H26" s="22"/>
     </row>
     <row r="27" spans="1:8" ht="19.95" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A27" s="25" t="s">
-        <v>141</v>
+        <v>37</v>
       </c>
       <c r="B27" s="25" t="s">
         <v>67</v>
       </c>
       <c r="C27" s="22" t="s">
+        <v>132</v>
+      </c>
+      <c r="D27" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="E27" s="25" t="str">
+        <f t="shared" si="0"/>
+        <v>founders.blade.php</v>
+      </c>
+      <c r="F27" s="25" t="str">
+        <f>$F$26 &amp; "/" &amp; D27</f>
+        <v>/subscribers/founders</v>
+      </c>
+      <c r="G27" s="25" t="s">
+        <v>122</v>
+      </c>
+      <c r="H27" s="22"/>
+    </row>
+    <row r="28" spans="1:8" ht="19.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
+      <c r="A28" s="25" t="s">
+        <v>133</v>
+      </c>
+      <c r="B28" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="C28" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="D28" s="25" t="s">
+        <v>114</v>
+      </c>
+      <c r="E28" s="25" t="str">
+        <f t="shared" si="0"/>
+        <v>students.blade.php</v>
+      </c>
+      <c r="F28" s="25" t="str">
+        <f>$F$26 &amp; "/" &amp; D28</f>
+        <v>/subscribers/students</v>
+      </c>
+      <c r="G28" s="25" t="s">
+        <v>122</v>
+      </c>
+      <c r="H28" s="22"/>
+    </row>
+    <row r="29" spans="1:8" ht="19.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="25" t="s">
+        <v>134</v>
+      </c>
+      <c r="B29" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="C29" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="D27" s="25" t="s">
-        <v>121</v>
-      </c>
-      <c r="E27" s="25" t="str">
+      <c r="D29" s="25" t="s">
+        <v>115</v>
+      </c>
+      <c r="E29" s="25" t="str">
         <f t="shared" si="0"/>
         <v>cards.blade.php</v>
       </c>
-      <c r="F27" s="25" t="str">
-        <f>$F$24 &amp; "/" &amp; D27</f>
+      <c r="F29" s="25" t="str">
+        <f>$F$26 &amp; "/" &amp; D29</f>
         <v>/subscribers/cards</v>
       </c>
-      <c r="G27" s="25" t="s">
-        <v>128</v>
-      </c>
-      <c r="H27" s="22"/>
-    </row>
-    <row r="28" spans="1:8" ht="19.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
-      <c r="A28" s="27" t="s">
+      <c r="G29" s="25" t="s">
+        <v>122</v>
+      </c>
+      <c r="H29" s="22"/>
+    </row>
+    <row r="30" spans="1:8" ht="19.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
+      <c r="A30" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="B28" s="27" t="s">
-        <v>67</v>
-      </c>
-      <c r="C28" s="21" t="s">
+      <c r="B30" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="C30" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="D28" s="27" t="s">
-        <v>122</v>
-      </c>
-      <c r="E28" s="27" t="str">
+      <c r="D30" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="E30" s="27" t="str">
         <f t="shared" si="0"/>
         <v>vendors.blade.php</v>
       </c>
-      <c r="F28" s="27" t="str">
+      <c r="F30" s="27" t="str">
         <f t="shared" si="1"/>
         <v>/vendors</v>
       </c>
-      <c r="G28" s="27" t="s">
-        <v>130</v>
-      </c>
-      <c r="H28" s="21"/>
-    </row>
-    <row r="29" spans="1:8" ht="19.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="26" t="s">
+      <c r="G30" s="27" t="s">
+        <v>124</v>
+      </c>
+      <c r="H30" s="21"/>
+    </row>
+    <row r="31" spans="1:8" ht="19.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
+      <c r="A31" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="B29" s="26" t="s">
+      <c r="B31" s="26" t="s">
         <v>68</v>
       </c>
-      <c r="C29" s="23" t="s">
+      <c r="C31" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="D29" s="26" t="s">
-        <v>105</v>
-      </c>
-      <c r="E29" s="26" t="str">
+      <c r="D31" s="26" t="s">
+        <v>99</v>
+      </c>
+      <c r="E31" s="26" t="str">
         <f t="shared" si="0"/>
         <v>mng_activity.blade.php</v>
       </c>
-      <c r="F29" s="26" t="str">
+      <c r="F31" s="26" t="str">
         <f t="shared" si="1"/>
         <v>/mng_activity</v>
       </c>
-      <c r="G29" s="26" t="s">
-        <v>106</v>
-      </c>
-      <c r="H29" s="23" t="s">
+      <c r="G31" s="26" t="s">
+        <v>100</v>
+      </c>
+      <c r="H31" s="23" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" ht="19.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
-      <c r="A30" s="25" t="s">
-        <v>40</v>
-      </c>
-      <c r="B30" s="25" t="s">
-        <v>67</v>
-      </c>
-      <c r="C30" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="D30" s="25" t="s">
-        <v>123</v>
-      </c>
-      <c r="E30" s="25" t="str">
-        <f t="shared" si="0"/>
-        <v>disciplines.blade.php</v>
-      </c>
-      <c r="F30" s="25" t="str">
-        <f>$F$29 &amp; "/" &amp; D30</f>
-        <v>/mng_activity/disciplines</v>
-      </c>
-      <c r="G30" s="25" t="s">
-        <v>131</v>
-      </c>
-      <c r="H30" s="22"/>
-    </row>
-    <row r="31" spans="1:8" ht="19.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
-      <c r="A31" s="25" t="s">
-        <v>41</v>
-      </c>
-      <c r="B31" s="25" t="s">
-        <v>67</v>
-      </c>
-      <c r="C31" s="22" t="s">
-        <v>30</v>
-      </c>
-      <c r="D31" s="25" t="s">
-        <v>124</v>
-      </c>
-      <c r="E31" s="25" t="str">
-        <f t="shared" si="0"/>
-        <v>courses.blade.php</v>
-      </c>
-      <c r="F31" s="25" t="str">
-        <f t="shared" ref="F31:F34" si="3">$F$29 &amp; "/" &amp; D31</f>
-        <v>/mng_activity/courses</v>
-      </c>
-      <c r="G31" s="25" t="s">
-        <v>131</v>
-      </c>
-      <c r="H31" s="22"/>
     </row>
     <row r="32" spans="1:8" ht="19.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A32" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="B32" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="C32" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="D32" s="25" t="s">
+        <v>117</v>
+      </c>
+      <c r="E32" s="25" t="str">
+        <f t="shared" si="0"/>
+        <v>disciplines.blade.php</v>
+      </c>
+      <c r="F32" s="25" t="str">
+        <f>$F$31 &amp; "/" &amp; D32</f>
+        <v>/mng_activity/disciplines</v>
+      </c>
+      <c r="G32" s="25" t="s">
+        <v>125</v>
+      </c>
+      <c r="H32" s="22"/>
+    </row>
+    <row r="33" spans="1:8" ht="19.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
+      <c r="A33" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="B33" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="C33" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="D33" s="25" t="s">
+        <v>118</v>
+      </c>
+      <c r="E33" s="25" t="str">
+        <f t="shared" si="0"/>
+        <v>courses.blade.php</v>
+      </c>
+      <c r="F33" s="25" t="str">
+        <f t="shared" ref="F33:F36" si="3">$F$31 &amp; "/" &amp; D33</f>
+        <v>/mng_activity/courses</v>
+      </c>
+      <c r="G33" s="25" t="s">
+        <v>125</v>
+      </c>
+      <c r="H33" s="22"/>
+    </row>
+    <row r="34" spans="1:8" ht="19.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
+      <c r="A34" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="B32" s="25" t="s">
-        <v>67</v>
-      </c>
-      <c r="C32" s="22" t="s">
+      <c r="B34" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="C34" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="D32" s="25" t="s">
-        <v>126</v>
-      </c>
-      <c r="E32" s="25" t="str">
+      <c r="D34" s="25" t="s">
+        <v>120</v>
+      </c>
+      <c r="E34" s="25" t="str">
         <f t="shared" si="0"/>
         <v>packages.blade.php</v>
       </c>
-      <c r="F32" s="25" t="str">
+      <c r="F34" s="25" t="str">
         <f t="shared" si="3"/>
         <v>/mng_activity/packages</v>
       </c>
-      <c r="G32" s="25" t="s">
-        <v>131</v>
-      </c>
-      <c r="H32" s="22"/>
-    </row>
-    <row r="33" spans="1:8" ht="19.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
-      <c r="A33" s="25" t="s">
+      <c r="G34" s="25" t="s">
+        <v>125</v>
+      </c>
+      <c r="H34" s="22"/>
+    </row>
+    <row r="35" spans="1:8" ht="19.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="B33" s="25" t="s">
-        <v>67</v>
-      </c>
-      <c r="C33" s="22" t="s">
+      <c r="B35" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="C35" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="D33" s="25" t="s">
-        <v>125</v>
-      </c>
-      <c r="E33" s="25" t="str">
+      <c r="D35" s="25" t="s">
+        <v>119</v>
+      </c>
+      <c r="E35" s="25" t="str">
         <f t="shared" si="0"/>
         <v>rooms.blade.php</v>
       </c>
-      <c r="F33" s="25" t="str">
+      <c r="F35" s="25" t="str">
         <f t="shared" si="3"/>
         <v>/mng_activity/rooms</v>
       </c>
-      <c r="G33" s="25" t="s">
-        <v>131</v>
-      </c>
-      <c r="H33" s="22"/>
-    </row>
-    <row r="34" spans="1:8" ht="19.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
-      <c r="A34" s="25" t="s">
+      <c r="G35" s="25" t="s">
+        <v>125</v>
+      </c>
+      <c r="H35" s="22"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A36" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="B34" s="25" t="s">
-        <v>67</v>
-      </c>
-      <c r="C34" s="22" t="s">
+      <c r="B36" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="C36" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="D34" s="25" t="s">
-        <v>127</v>
-      </c>
-      <c r="E34" s="25" t="str">
+      <c r="D36" s="25" t="s">
+        <v>121</v>
+      </c>
+      <c r="E36" s="25" t="str">
         <f t="shared" si="0"/>
         <v>scheduling.blade.php</v>
       </c>
-      <c r="F34" s="25" t="str">
+      <c r="F36" s="25" t="str">
         <f t="shared" si="3"/>
         <v>/mng_activity/scheduling</v>
       </c>
-      <c r="G34" s="25" t="s">
-        <v>131</v>
-      </c>
-      <c r="H34" s="22"/>
-    </row>
-    <row r="35" spans="1:8" ht="19.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="26" t="s">
+      <c r="G36" s="25" t="s">
+        <v>125</v>
+      </c>
+      <c r="H36" s="22"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A37" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="B35" s="26" t="s">
-        <v>67</v>
-      </c>
-      <c r="C35" s="23" t="s">
+      <c r="B37" s="26" t="s">
+        <v>67</v>
+      </c>
+      <c r="C37" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="D35" s="26" t="s">
-        <v>108</v>
-      </c>
-      <c r="E35" s="26" t="str">
+      <c r="D37" s="26" t="s">
+        <v>102</v>
+      </c>
+      <c r="E37" s="26" t="str">
         <f t="shared" si="0"/>
         <v>report_stats.blade.php</v>
       </c>
-      <c r="F35" s="26" t="str">
+      <c r="F37" s="26" t="str">
         <f t="shared" si="1"/>
         <v>/report_stats</v>
       </c>
-      <c r="G35" s="26" t="s">
-        <v>106</v>
-      </c>
-      <c r="H35" s="23" t="s">
-        <v>109</v>
+      <c r="G37" s="26" t="s">
+        <v>100</v>
+      </c>
+      <c r="H37" s="23" t="s">
+        <v>103</v>
       </c>
     </row>
   </sheetData>
   <dataConsolidate/>
-  <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F37" xr:uid="{C7F42672-59D8-4A95-9804-4B94DD14E8F6}">
+  <dataValidations disablePrompts="1" count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F39" xr:uid="{C7F42672-59D8-4A95-9804-4B94DD14E8F6}">
       <formula1>RefView_route</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B2:B35" xr:uid="{F340BA2D-9D43-4A9F-86F9-B281B429D2E7}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B2:B37" xr:uid="{F340BA2D-9D43-4A9F-86F9-B281B429D2E7}">
       <formula1>RefTipo</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G35" xr:uid="{DFF187B0-2821-4C72-B394-0420A8E90996}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G37" xr:uid="{DFF187B0-2821-4C72-B394-0420A8E90996}">
       <formula1>RefController_nome</formula1>
     </dataValidation>
   </dataValidations>
@@ -2192,7 +2249,7 @@
   <dimension ref="B1:G28"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2233,7 +2290,7 @@
         <v>70</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>75</v>
+        <v>136</v>
       </c>
       <c r="E3" s="5"/>
     </row>
@@ -2242,7 +2299,7 @@
         <v>69</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="E4" s="5"/>
     </row>
@@ -2251,7 +2308,7 @@
         <v>68</v>
       </c>
       <c r="D5" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.3">
@@ -2259,28 +2316,28 @@
         <v>67</v>
       </c>
       <c r="D6" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B7" s="4" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="D7" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B8" s="4" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="D8" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.3">
       <c r="D9" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Creata la sidenav proceduralemente
Bisogna solo modificare gli include per modificare i link ed i testi
</commit_message>
<xml_diff>
--- a/Documentazioni/Codifica pagine sito.xlsx
+++ b/Documentazioni/Codifica pagine sito.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr filterPrivacy="1" codeName="Questa_cartella_di_lavoro"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E02D93B-CCED-4A51-BBD7-78BE7A4A4789}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{917D0437-7F98-4427-B86B-4ED63DD762CF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,6 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -916,7 +915,7 @@
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{45120F09-8607-4F6A-A989-7184307236A1}" name="Tipo" displayName="Tipo" ref="B1:B8" totalsRowShown="0" headerRowDxfId="2" tableBorderDxfId="1">
   <autoFilter ref="B1:B8" xr:uid="{B0803B6A-3448-4A89-AC43-1127F3DBD833}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:B8">
+  <sortState ref="B2:B8">
     <sortCondition ref="B1:B8"/>
   </sortState>
   <tableColumns count="1">
@@ -1204,27 +1203,27 @@
   <sheetPr codeName="Foglio2"/>
   <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" outlineLevelRow="3" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" outlineLevelRow="2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.5546875" style="14" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.5703125" style="14" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13" style="12" customWidth="1"/>
-    <col min="3" max="3" width="35.5546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.33203125" style="15" customWidth="1"/>
-    <col min="5" max="5" width="24.44140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="29.33203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" style="15" customWidth="1"/>
+    <col min="5" max="5" width="24.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.28515625" style="13" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17" style="13" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="89.6640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="28.6640625" style="13" customWidth="1"/>
-    <col min="10" max="11" width="8.88671875" style="13"/>
+    <col min="8" max="8" width="89.7109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="28.7109375" style="13" customWidth="1"/>
+    <col min="10" max="11" width="8.85546875" style="13"/>
     <col min="12" max="12" width="19" style="13" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="8.88671875" style="13"/>
+    <col min="13" max="16384" width="8.85546875" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>1</v>
       </c>
@@ -1250,7 +1249,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>47</v>
       </c>
@@ -1278,7 +1277,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="19.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="19.899999999999999" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A3" s="18"/>
       <c r="B3" s="18" t="s">
         <v>92</v>
@@ -1297,7 +1296,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="19.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="19.899999999999999" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
         <v>144</v>
       </c>
@@ -1323,7 +1322,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
         <v>48</v>
       </c>
@@ -1351,7 +1350,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
         <v>57</v>
       </c>
@@ -1379,7 +1378,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
         <v>131</v>
       </c>
@@ -1408,7 +1407,7 @@
       </c>
       <c r="I7" s="12"/>
     </row>
-    <row r="8" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
         <v>49</v>
       </c>
@@ -1437,7 +1436,7 @@
       </c>
       <c r="I8" s="12"/>
     </row>
-    <row r="9" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
         <v>51</v>
       </c>
@@ -1466,7 +1465,7 @@
       </c>
       <c r="I9" s="12"/>
     </row>
-    <row r="10" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
         <v>53</v>
       </c>
@@ -1494,7 +1493,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="18" t="s">
         <v>55</v>
       </c>
@@ -1522,7 +1521,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
         <v>58</v>
       </c>
@@ -1550,7 +1549,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
         <v>61</v>
       </c>
@@ -1578,7 +1577,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="19.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="18" t="s">
         <v>62</v>
       </c>
@@ -1606,7 +1605,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="19.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="28" t="s">
         <v>46</v>
       </c>
@@ -1634,7 +1633,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="19.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="26" t="s">
         <v>18</v>
       </c>
@@ -1662,7 +1661,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="19.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" ht="19.899999999999999" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A17" s="27" t="s">
         <v>19</v>
       </c>
@@ -1690,7 +1689,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="19.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" ht="19.899999999999999" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A18" s="25" t="s">
         <v>20</v>
       </c>
@@ -1716,7 +1715,7 @@
       </c>
       <c r="H18" s="22"/>
     </row>
-    <row r="19" spans="1:8" ht="19.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" ht="19.899999999999999" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A19" s="25" t="s">
         <v>21</v>
       </c>
@@ -1742,7 +1741,7 @@
       </c>
       <c r="H19" s="22"/>
     </row>
-    <row r="20" spans="1:8" ht="19.95" customHeight="1" outlineLevel="2" collapsed="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" ht="19.899999999999999" hidden="1" customHeight="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A20" s="25" t="s">
         <v>22</v>
       </c>
@@ -1768,7 +1767,7 @@
       </c>
       <c r="H20" s="22"/>
     </row>
-    <row r="21" spans="1:8" ht="19.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" ht="19.899999999999999" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A21" s="25" t="s">
         <v>23</v>
       </c>
@@ -1794,7 +1793,7 @@
       </c>
       <c r="H21" s="22"/>
     </row>
-    <row r="22" spans="1:8" ht="19.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" ht="19.899999999999999" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A22" s="27" t="s">
         <v>24</v>
       </c>
@@ -1822,7 +1821,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="19.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" ht="19.899999999999999" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A23" s="25" t="s">
         <v>25</v>
       </c>
@@ -1848,7 +1847,7 @@
       </c>
       <c r="H23" s="22"/>
     </row>
-    <row r="24" spans="1:8" ht="19.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" ht="19.899999999999999" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A24" s="25" t="s">
         <v>26</v>
       </c>
@@ -1874,7 +1873,7 @@
       </c>
       <c r="H24" s="22"/>
     </row>
-    <row r="25" spans="1:8" ht="19.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" ht="19.899999999999999" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A25" s="26" t="s">
         <v>27</v>
       </c>
@@ -1902,7 +1901,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="19.95" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" ht="19.899999999999999" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A26" s="27" t="s">
         <v>28</v>
       </c>
@@ -1930,7 +1929,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="19.95" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" ht="19.899999999999999" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A27" s="25" t="s">
         <v>37</v>
       </c>
@@ -1956,7 +1955,7 @@
       </c>
       <c r="H27" s="22"/>
     </row>
-    <row r="28" spans="1:8" ht="19.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" ht="19.899999999999999" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A28" s="25" t="s">
         <v>133</v>
       </c>
@@ -1982,7 +1981,7 @@
       </c>
       <c r="H28" s="22"/>
     </row>
-    <row r="29" spans="1:8" ht="19.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" ht="19.899999999999999" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A29" s="25" t="s">
         <v>134</v>
       </c>
@@ -2008,7 +2007,7 @@
       </c>
       <c r="H29" s="22"/>
     </row>
-    <row r="30" spans="1:8" ht="19.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" ht="19.899999999999999" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A30" s="27" t="s">
         <v>38</v>
       </c>
@@ -2034,7 +2033,7 @@
       </c>
       <c r="H30" s="21"/>
     </row>
-    <row r="31" spans="1:8" ht="19.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="26" t="s">
         <v>39</v>
       </c>
@@ -2062,7 +2061,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="19.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" ht="19.899999999999999" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A32" s="25" t="s">
         <v>40</v>
       </c>
@@ -2088,7 +2087,7 @@
       </c>
       <c r="H32" s="22"/>
     </row>
-    <row r="33" spans="1:8" ht="19.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" ht="19.899999999999999" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A33" s="25" t="s">
         <v>41</v>
       </c>
@@ -2114,7 +2113,7 @@
       </c>
       <c r="H33" s="22"/>
     </row>
-    <row r="34" spans="1:8" ht="19.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" ht="19.899999999999999" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A34" s="25" t="s">
         <v>43</v>
       </c>
@@ -2140,7 +2139,7 @@
       </c>
       <c r="H34" s="22"/>
     </row>
-    <row r="35" spans="1:8" ht="19.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" ht="19.899999999999999" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A35" s="25" t="s">
         <v>42</v>
       </c>
@@ -2166,7 +2165,7 @@
       </c>
       <c r="H35" s="22"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A36" s="25" t="s">
         <v>44</v>
       </c>
@@ -2192,7 +2191,7 @@
       </c>
       <c r="H36" s="22"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="26" t="s">
         <v>45</v>
       </c>
@@ -2252,17 +2251,17 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="6" width="25.109375" customWidth="1"/>
-    <col min="7" max="7" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="6" width="25.140625" customWidth="1"/>
+    <col min="7" max="7" width="24.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="19" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>73</v>
       </c>
@@ -2276,7 +2275,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="3" t="s">
         <v>71</v>
       </c>
@@ -2285,7 +2284,7 @@
       </c>
       <c r="E2" s="5"/>
     </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>70</v>
       </c>
@@ -2294,7 +2293,7 @@
       </c>
       <c r="E3" s="5"/>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>69</v>
       </c>
@@ -2303,7 +2302,7 @@
       </c>
       <c r="E4" s="5"/>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>68</v>
       </c>
@@ -2311,7 +2310,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
         <v>67</v>
       </c>
@@ -2319,7 +2318,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
         <v>92</v>
       </c>
@@ -2327,7 +2326,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="s">
         <v>101</v>
       </c>
@@ -2335,22 +2334,22 @@
         <v>124</v>
       </c>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D9" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B15" s="17"/>
       <c r="C15" s="16"/>
       <c r="D15" s="16"/>
       <c r="E15" s="16"/>
     </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B16" s="9"/>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
@@ -2358,7 +2357,7 @@
       <c r="F16" s="10"/>
       <c r="G16" s="8"/>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="9"/>
       <c r="C17" s="6"/>
       <c r="D17" s="7"/>
@@ -2366,7 +2365,7 @@
       <c r="F17" s="10"/>
       <c r="G17" s="8"/>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="9"/>
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
@@ -2374,7 +2373,7 @@
       <c r="F18" s="10"/>
       <c r="G18" s="8"/>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="9"/>
       <c r="C19" s="6"/>
       <c r="D19" s="7"/>
@@ -2382,7 +2381,7 @@
       <c r="F19" s="10"/>
       <c r="G19" s="8"/>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="9"/>
       <c r="C20" s="6"/>
       <c r="D20" s="7"/>
@@ -2390,7 +2389,7 @@
       <c r="F20" s="10"/>
       <c r="G20" s="8"/>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="9"/>
       <c r="C21" s="6"/>
       <c r="D21" s="7"/>
@@ -2398,7 +2397,7 @@
       <c r="F21" s="10"/>
       <c r="G21" s="8"/>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="9"/>
       <c r="C22" s="6"/>
       <c r="D22" s="7"/>
@@ -2406,7 +2405,7 @@
       <c r="F22" s="10"/>
       <c r="G22" s="8"/>
     </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" s="9"/>
       <c r="C23" s="6"/>
       <c r="D23" s="7"/>
@@ -2414,7 +2413,7 @@
       <c r="F23" s="10"/>
       <c r="G23" s="8"/>
     </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" s="9"/>
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
@@ -2422,7 +2421,7 @@
       <c r="F24" s="10"/>
       <c r="G24" s="8"/>
     </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" s="9"/>
       <c r="C25" s="6"/>
       <c r="D25" s="7"/>
@@ -2430,7 +2429,7 @@
       <c r="F25" s="10"/>
       <c r="G25" s="8"/>
     </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" s="9"/>
       <c r="C26" s="6"/>
       <c r="D26" s="7"/>
@@ -2438,7 +2437,7 @@
       <c r="F26" s="10"/>
       <c r="G26" s="8"/>
     </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" s="9"/>
       <c r="C27" s="6"/>
       <c r="D27" s="7"/>
@@ -2446,13 +2445,13 @@
       <c r="F27" s="10"/>
       <c r="G27" s="8"/>
     </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D28" s="7"/>
       <c r="E28" s="10"/>
       <c r="F28" s="10"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="D13:D29">
+  <sortState ref="D13:D29">
     <sortCondition ref="D13"/>
   </sortState>
   <dataConsolidate/>

</xml_diff>

<commit_message>
Finito le CRUD di discipline
</commit_message>
<xml_diff>
--- a/Documentazioni/Codifica pagine sito.xlsx
+++ b/Documentazioni/Codifica pagine sito.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr filterPrivacy="1" codeName="Questa_cartella_di_lavoro"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88F4AD76-E681-4E3D-BA29-5EA4BBC66464}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99AE5DD0-C38C-4FA7-86F8-EB1ED213E938}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -12,7 +12,7 @@
     <sheet name="Foglio utile" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Main!$A$1:$H$37</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Main!$A$1:$H$42</definedName>
     <definedName name="RefController_nome">Controller[Lista Controller]</definedName>
     <definedName name="RefTipo">Tipo[]</definedName>
   </definedNames>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="155">
   <si>
     <t>Nome gabbia logica</t>
   </si>
@@ -231,9 +231,6 @@
     <t>Link</t>
   </si>
   <si>
-    <t>Azione veloce</t>
-  </si>
-  <si>
     <t>Da definire</t>
   </si>
   <si>
@@ -463,6 +460,42 @@
   </si>
   <si>
     <t>CourseController</t>
+  </si>
+  <si>
+    <t>disciplines-create</t>
+  </si>
+  <si>
+    <t>DisciplineController</t>
+  </si>
+  <si>
+    <t>M311</t>
+  </si>
+  <si>
+    <t>Azione</t>
+  </si>
+  <si>
+    <t>disciplines-edit</t>
+  </si>
+  <si>
+    <t>disciplines-delete</t>
+  </si>
+  <si>
+    <t>M312</t>
+  </si>
+  <si>
+    <t>M313</t>
+  </si>
+  <si>
+    <t>discipline-store</t>
+  </si>
+  <si>
+    <t>M314</t>
+  </si>
+  <si>
+    <t>disciplines-update</t>
+  </si>
+  <si>
+    <t>M315</t>
   </si>
 </sst>
 </file>
@@ -665,30 +698,6 @@
   </cellStyles>
   <dxfs count="18">
     <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="medium">
           <color indexed="64"/>
@@ -861,6 +870,30 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -892,34 +925,34 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{905F6574-56C3-4E36-86AD-16F4E970F9D2}" name="Tabella4" displayName="Tabella4" ref="A1:H37" dataDxfId="17">
-  <autoFilter ref="A1:H37" xr:uid="{34684D11-7ACD-45A4-AA96-0CE6C7239D98}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{905F6574-56C3-4E36-86AD-16F4E970F9D2}" name="Tabella4" displayName="Tabella4" ref="A1:H42" dataDxfId="17">
+  <autoFilter ref="A1:H42" xr:uid="{34684D11-7ACD-45A4-AA96-0CE6C7239D98}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{E7D98D43-EB7B-46CE-B0B0-C555D83773A6}" name="Codice gabbia logica" dataDxfId="16" totalsRowDxfId="15"/>
-    <tableColumn id="8" xr3:uid="{CAF26B0C-D3E2-4A71-A7C5-519E983C334C}" name="Rotta" dataDxfId="0" totalsRowDxfId="1">
+    <tableColumn id="8" xr3:uid="{CAF26B0C-D3E2-4A71-A7C5-519E983C334C}" name="Rotta" dataDxfId="14" totalsRowDxfId="13">
       <calculatedColumnFormula>"/" &amp; E2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{DB39DBBD-231C-4393-B53A-31DA54EF2B6B}" name="Tipo" dataDxfId="14" totalsRowDxfId="13"/>
-    <tableColumn id="3" xr3:uid="{267C913B-0C60-4A11-8D31-6129F6A6699A}" name="Nome gabbia logica" dataDxfId="12" totalsRowDxfId="11"/>
-    <tableColumn id="5" xr3:uid="{251AE08F-697F-47EC-9FB6-7CEF1CCB916E}" name="view" dataDxfId="10" totalsRowDxfId="9"/>
-    <tableColumn id="6" xr3:uid="{E87D751D-6B30-48F2-95B8-E2DCF4172ECA}" name="Nome file" dataDxfId="8">
+    <tableColumn id="2" xr3:uid="{DB39DBBD-231C-4393-B53A-31DA54EF2B6B}" name="Tipo" dataDxfId="12" totalsRowDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{267C913B-0C60-4A11-8D31-6129F6A6699A}" name="Nome gabbia logica" dataDxfId="10" totalsRowDxfId="9"/>
+    <tableColumn id="5" xr3:uid="{251AE08F-697F-47EC-9FB6-7CEF1CCB916E}" name="view" dataDxfId="8" totalsRowDxfId="7"/>
+    <tableColumn id="6" xr3:uid="{E87D751D-6B30-48F2-95B8-E2DCF4172ECA}" name="Nome file" dataDxfId="6">
       <calculatedColumnFormula>IF($E2="Da definire",$E2,_xlfn.CONCAT($E2,".blade.php"))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{C8498EB6-2C5F-47B9-B993-99AA78B7EEAA}" name="Controller" dataDxfId="7"/>
-    <tableColumn id="10" xr3:uid="{E6E3AEA2-F019-429B-B8B1-54C1BCAF6687}" name="Commento" dataDxfId="6" totalsRowDxfId="5"/>
+    <tableColumn id="9" xr3:uid="{C8498EB6-2C5F-47B9-B993-99AA78B7EEAA}" name="Controller" dataDxfId="5"/>
+    <tableColumn id="10" xr3:uid="{E6E3AEA2-F019-429B-B8B1-54C1BCAF6687}" name="Commento" dataDxfId="4" totalsRowDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium12" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{45120F09-8607-4F6A-A989-7184307236A1}" name="Tipo" displayName="Tipo" ref="B1:B8" totalsRowShown="0" headerRowDxfId="4" tableBorderDxfId="3">
-  <autoFilter ref="B1:B8" xr:uid="{B0803B6A-3448-4A89-AC43-1127F3DBD833}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{45120F09-8607-4F6A-A989-7184307236A1}" name="Tipo" displayName="Tipo" ref="B1:B9" totalsRowShown="0" headerRowDxfId="2" tableBorderDxfId="1">
+  <autoFilter ref="B1:B9" xr:uid="{B0803B6A-3448-4A89-AC43-1127F3DBD833}"/>
   <sortState ref="B2:B8">
     <sortCondition ref="B1:B8"/>
   </sortState>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{95A47413-48BC-4507-BE9E-0DFA740DC4DC}" name="Tipi di pagina" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{95A47413-48BC-4507-BE9E-0DFA740DC4DC}" name="Tipi di pagina" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1201,19 +1234,19 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Foglio2"/>
-  <dimension ref="A1:I37"/>
+  <dimension ref="A1:I42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" outlineLevelRow="2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.5703125" style="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.42578125" style="13" customWidth="1"/>
+    <col min="2" max="2" width="27.140625" style="13" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13" style="12" customWidth="1"/>
     <col min="4" max="4" width="35.5703125" style="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.28515625" style="15" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" style="15" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="24.42578125" style="13" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="88.42578125" style="13" bestFit="1" customWidth="1"/>
@@ -1229,7 +1262,7 @@
         <v>1</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C1" s="12" t="s">
         <v>62</v>
@@ -1238,13 +1271,13 @@
         <v>0</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F1" s="13" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G1" s="13" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H1" s="11" t="s">
         <v>2</v>
@@ -1263,20 +1296,20 @@
         <v>63</v>
       </c>
       <c r="D2" s="19" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E2" s="20" t="s">
         <v>61</v>
       </c>
       <c r="F2" s="18" t="str">
-        <f t="shared" ref="F2:F37" si="0">IF($E2="Da definire",$E2,_xlfn.CONCAT($E2,".blade.php"))</f>
+        <f t="shared" ref="F2:F42" si="0">IF($E2="Da definire",$E2,_xlfn.CONCAT($E2,".blade.php"))</f>
         <v>welcome.blade.php</v>
       </c>
       <c r="G2" s="18" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H2" s="19" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="I2" s="13"/>
     </row>
@@ -1287,29 +1320,29 @@
         <v>/</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D3" s="19"/>
       <c r="E3" s="20"/>
       <c r="F3" s="18"/>
       <c r="G3" s="18" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H3" s="19" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I3" s="13"/>
     </row>
     <row r="4" spans="1:9" ht="19.899999999999999" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B4" s="18" t="str">
         <f>"/" &amp; E4 &amp; "/redirect"</f>
         <v>/welcome/redirect</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D4" s="19"/>
       <c r="E4" s="20" t="s">
@@ -1320,10 +1353,10 @@
         <v>welcome.blade.php</v>
       </c>
       <c r="G4" s="18" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H4" s="19" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="I4" s="13"/>
     </row>
@@ -1332,7 +1365,7 @@
         <v>44</v>
       </c>
       <c r="B5" s="18" t="str">
-        <f>"/" &amp; E5</f>
+        <f t="shared" ref="B5:B17" si="1">"/" &amp; E5</f>
         <v>/boot</v>
       </c>
       <c r="C5" s="18" t="s">
@@ -1342,17 +1375,17 @@
         <v>3</v>
       </c>
       <c r="E5" s="20" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F5" s="18" t="str">
         <f t="shared" si="0"/>
         <v>boot.blade.php</v>
       </c>
       <c r="G5" s="18" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H5" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="I5" s="13"/>
     </row>
@@ -1361,56 +1394,56 @@
         <v>53</v>
       </c>
       <c r="B6" s="18" t="str">
-        <f>"/" &amp; E6</f>
+        <f t="shared" si="1"/>
         <v>/boot-asd-done</v>
       </c>
       <c r="C6" s="18" t="s">
         <v>63</v>
       </c>
       <c r="D6" s="19" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E6" s="20" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F6" s="18" t="str">
         <f t="shared" si="0"/>
         <v>boot-asd-done.blade.php</v>
       </c>
       <c r="G6" s="18" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H6" s="19" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="I6" s="13"/>
     </row>
     <row r="7" spans="1:9" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B7" s="18" t="str">
-        <f>"/" &amp; E7</f>
+        <f t="shared" si="1"/>
         <v>/boot-socio</v>
       </c>
       <c r="C7" s="18" t="s">
         <v>63</v>
       </c>
       <c r="D7" s="19" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E7" s="20" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F7" s="18" t="str">
         <f>IF($E7="Da definire",$E7,_xlfn.CONCAT($E7,".blade.php"))</f>
         <v>boot-socio.blade.php</v>
       </c>
       <c r="G7" s="18" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H7" s="19" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I7" s="12"/>
     </row>
@@ -1419,27 +1452,27 @@
         <v>45</v>
       </c>
       <c r="B8" s="18" t="str">
-        <f>"/" &amp; E8</f>
+        <f t="shared" si="1"/>
         <v>/boot-finished</v>
       </c>
       <c r="C8" s="18" t="s">
         <v>63</v>
       </c>
       <c r="D8" s="19" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E8" s="20" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F8" s="18" t="str">
         <f t="shared" si="0"/>
         <v>boot-finished.blade.php</v>
       </c>
       <c r="G8" s="18" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H8" s="19" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I8" s="12"/>
     </row>
@@ -1448,24 +1481,24 @@
         <v>47</v>
       </c>
       <c r="B9" s="18" t="str">
-        <f>"/" &amp; E9</f>
+        <f t="shared" si="1"/>
         <v>/login</v>
       </c>
       <c r="C9" s="18" t="s">
         <v>63</v>
       </c>
       <c r="D9" s="19" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E9" s="20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F9" s="18" t="str">
         <f t="shared" si="0"/>
         <v>login.blade.php</v>
       </c>
       <c r="G9" s="18" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H9" s="19" t="s">
         <v>48</v>
@@ -1477,24 +1510,24 @@
         <v>49</v>
       </c>
       <c r="B10" s="18" t="str">
-        <f>"/" &amp; E10</f>
+        <f t="shared" si="1"/>
         <v>/login-done</v>
       </c>
       <c r="C10" s="18" t="s">
         <v>63</v>
       </c>
       <c r="D10" s="19" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E10" s="20" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F10" s="18" t="str">
         <f t="shared" si="0"/>
         <v>login-done.blade.php</v>
       </c>
       <c r="G10" s="18" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H10" s="19" t="s">
         <v>50</v>
@@ -1506,24 +1539,24 @@
         <v>51</v>
       </c>
       <c r="B11" s="18" t="str">
-        <f>"/" &amp; E11</f>
+        <f t="shared" si="1"/>
         <v>/login-failure</v>
       </c>
       <c r="C11" s="18" t="s">
         <v>63</v>
       </c>
       <c r="D11" s="19" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E11" s="20" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F11" s="18" t="str">
         <f t="shared" si="0"/>
         <v>login-failure.blade.php</v>
       </c>
       <c r="G11" s="18" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H11" s="19" t="s">
         <v>52</v>
@@ -1535,7 +1568,7 @@
         <v>54</v>
       </c>
       <c r="B12" s="18" t="str">
-        <f>"/" &amp; E12</f>
+        <f t="shared" si="1"/>
         <v>/our-team</v>
       </c>
       <c r="C12" s="18" t="s">
@@ -1545,14 +1578,14 @@
         <v>9</v>
       </c>
       <c r="E12" s="20" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F12" s="18" t="str">
         <f t="shared" si="0"/>
         <v>our-team.blade.php</v>
       </c>
       <c r="G12" s="18" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H12" s="19" t="s">
         <v>55</v>
@@ -1564,7 +1597,7 @@
         <v>57</v>
       </c>
       <c r="B13" s="18" t="str">
-        <f>"/" &amp; E13</f>
+        <f t="shared" si="1"/>
         <v>/contacts</v>
       </c>
       <c r="C13" s="18" t="s">
@@ -1574,14 +1607,14 @@
         <v>10</v>
       </c>
       <c r="E13" s="20" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F13" s="18" t="str">
         <f t="shared" si="0"/>
         <v>contacts.blade.php</v>
       </c>
       <c r="G13" s="18" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H13" s="19" t="s">
         <v>56</v>
@@ -1593,7 +1626,7 @@
         <v>58</v>
       </c>
       <c r="B14" s="18" t="str">
-        <f>"/" &amp; E14</f>
+        <f t="shared" si="1"/>
         <v>/settings-account</v>
       </c>
       <c r="C14" s="18" t="s">
@@ -1603,14 +1636,14 @@
         <v>59</v>
       </c>
       <c r="E14" s="20" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F14" s="18" t="str">
         <f t="shared" si="0"/>
         <v>settings-account.blade.php</v>
       </c>
       <c r="G14" s="18" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H14" s="19" t="s">
         <v>60</v>
@@ -1622,7 +1655,7 @@
         <v>42</v>
       </c>
       <c r="B15" s="28" t="str">
-        <f>"/" &amp; E15</f>
+        <f t="shared" si="1"/>
         <v>/homepage</v>
       </c>
       <c r="C15" s="28" t="s">
@@ -1632,14 +1665,14 @@
         <v>4</v>
       </c>
       <c r="E15" s="28" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F15" s="28" t="str">
         <f t="shared" si="0"/>
         <v>homepage.blade.php</v>
       </c>
       <c r="G15" s="28" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H15" s="24" t="s">
         <v>5</v>
@@ -1649,24 +1682,24 @@
     <row r="16" spans="1:9" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="26"/>
       <c r="B16" s="26" t="str">
-        <f>"/" &amp; E16</f>
+        <f t="shared" si="1"/>
         <v>/managment</v>
       </c>
       <c r="C16" s="26" t="s">
         <v>64</v>
       </c>
       <c r="D16" s="23" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E16" s="26" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F16" s="26" t="str">
         <f t="shared" si="0"/>
         <v>managment.blade.php</v>
       </c>
       <c r="G16" s="26" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H16" s="23" t="s">
         <v>46</v>
@@ -1678,24 +1711,24 @@
         <v>18</v>
       </c>
       <c r="B17" s="27" t="str">
-        <f>"/" &amp; E17</f>
+        <f t="shared" si="1"/>
         <v>/staff</v>
       </c>
       <c r="C17" s="27" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D17" s="21" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E17" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="F17" s="27" t="str">
+        <f t="shared" si="0"/>
+        <v>staff.blade.php</v>
+      </c>
+      <c r="G17" s="27" t="s">
         <v>100</v>
-      </c>
-      <c r="F17" s="27" t="str">
-        <f t="shared" si="0"/>
-        <v>staff.blade.php</v>
-      </c>
-      <c r="G17" s="27" t="s">
-        <v>101</v>
       </c>
       <c r="H17" s="21" t="s">
         <v>46</v>
@@ -1717,14 +1750,14 @@
         <v>12</v>
       </c>
       <c r="E18" s="25" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F18" s="25" t="str">
         <f t="shared" si="0"/>
         <v>collab-int.blade.php</v>
       </c>
       <c r="G18" s="25" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H18" s="22"/>
       <c r="I18" s="13"/>
@@ -1744,14 +1777,14 @@
         <v>13</v>
       </c>
       <c r="E19" s="25" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F19" s="25" t="str">
         <f t="shared" si="0"/>
         <v>collab-ext.blade.php</v>
       </c>
       <c r="G19" s="25" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H19" s="22"/>
       <c r="I19" s="13"/>
@@ -1771,14 +1804,14 @@
         <v>14</v>
       </c>
       <c r="E20" s="25" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F20" s="25" t="str">
         <f t="shared" si="0"/>
         <v>trainee.blade.php</v>
       </c>
       <c r="G20" s="25" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H20" s="22"/>
       <c r="I20" s="13"/>
@@ -1798,14 +1831,14 @@
         <v>15</v>
       </c>
       <c r="E21" s="25" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F21" s="25" t="str">
         <f t="shared" si="0"/>
         <v>teacher.blade.php</v>
       </c>
       <c r="G21" s="25" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H21" s="22"/>
       <c r="I21" s="13"/>
@@ -1819,20 +1852,20 @@
         <v>/payments</v>
       </c>
       <c r="C22" s="27" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D22" s="21" t="s">
         <v>11</v>
       </c>
       <c r="E22" s="27" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F22" s="27" t="str">
         <f t="shared" si="0"/>
         <v>payments.blade.php</v>
       </c>
       <c r="G22" s="27" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H22" s="21" t="s">
         <v>46</v>
@@ -1854,14 +1887,14 @@
         <v>16</v>
       </c>
       <c r="E23" s="25" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F23" s="25" t="str">
         <f t="shared" si="0"/>
         <v>outflow.blade.php</v>
       </c>
       <c r="G23" s="25" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H23" s="22"/>
       <c r="I23" s="13"/>
@@ -1881,14 +1914,14 @@
         <v>17</v>
       </c>
       <c r="E24" s="25" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F24" s="25" t="str">
         <f t="shared" si="0"/>
         <v>earn.blade.php</v>
       </c>
       <c r="G24" s="25" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H24" s="22"/>
       <c r="I24" s="13"/>
@@ -1906,14 +1939,14 @@
         <v>6</v>
       </c>
       <c r="E25" s="26" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F25" s="26" t="str">
         <f t="shared" si="0"/>
         <v>secretariat.blade.php</v>
       </c>
       <c r="G25" s="26" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H25" s="23" t="s">
         <v>46</v>
@@ -1929,20 +1962,20 @@
         <v>/subscribers</v>
       </c>
       <c r="C26" s="27" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D26" s="21" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E26" s="27" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F26" s="27" t="str">
         <f t="shared" si="0"/>
         <v>subscribers.blade.php</v>
       </c>
       <c r="G26" s="27" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H26" s="21" t="s">
         <v>46</v>
@@ -1961,24 +1994,24 @@
         <v>63</v>
       </c>
       <c r="D27" s="22" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E27" s="25" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F27" s="25" t="str">
         <f t="shared" si="0"/>
         <v>founders.blade.php</v>
       </c>
       <c r="G27" s="25" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H27" s="22"/>
       <c r="I27" s="13"/>
     </row>
     <row r="28" spans="1:9" ht="19.899999999999999" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A28" s="25" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B28" s="25" t="str">
         <f>$B$26 &amp; "/" &amp; E28</f>
@@ -1991,21 +2024,21 @@
         <v>32</v>
       </c>
       <c r="E28" s="25" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F28" s="25" t="str">
         <f t="shared" si="0"/>
         <v>students.blade.php</v>
       </c>
       <c r="G28" s="25" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H28" s="22"/>
       <c r="I28" s="13"/>
     </row>
     <row r="29" spans="1:9" ht="19.899999999999999" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A29" s="25" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B29" s="25" t="str">
         <f>$B$26 &amp; "/" &amp; E29</f>
@@ -2018,14 +2051,14 @@
         <v>33</v>
       </c>
       <c r="E29" s="25" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F29" s="25" t="str">
         <f t="shared" si="0"/>
         <v>cards.blade.php</v>
       </c>
       <c r="G29" s="25" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H29" s="22"/>
       <c r="I29" s="13"/>
@@ -2045,14 +2078,14 @@
         <v>34</v>
       </c>
       <c r="E30" s="27" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F30" s="27" t="str">
         <f t="shared" si="0"/>
         <v>vendors.blade.php</v>
       </c>
       <c r="G30" s="27" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H30" s="21"/>
       <c r="I30" s="13"/>
@@ -2070,14 +2103,14 @@
         <v>7</v>
       </c>
       <c r="E31" s="26" t="s">
+        <v>94</v>
+      </c>
+      <c r="F31" s="26" t="str">
+        <f t="shared" si="0"/>
+        <v>mng_activity.blade.php</v>
+      </c>
+      <c r="G31" s="26" t="s">
         <v>95</v>
-      </c>
-      <c r="F31" s="26" t="str">
-        <f t="shared" si="0"/>
-        <v>mng_activity.blade.php</v>
-      </c>
-      <c r="G31" s="26" t="s">
-        <v>96</v>
       </c>
       <c r="H31" s="23" t="s">
         <v>46</v>
@@ -2099,163 +2132,282 @@
         <v>27</v>
       </c>
       <c r="E32" s="25" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F32" s="25" t="str">
         <f t="shared" si="0"/>
         <v>disciplines.blade.php</v>
       </c>
       <c r="G32" s="25" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H32" s="22"/>
       <c r="I32" s="13"/>
     </row>
-    <row r="33" spans="1:9" ht="19.899999999999999" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" ht="19.899999999999999" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A33" s="25" t="s">
-        <v>38</v>
+        <v>145</v>
       </c>
       <c r="B33" s="25" t="str">
-        <f>$B$31 &amp; "/" &amp; E33</f>
-        <v>/mng_activity/courses</v>
+        <f t="shared" ref="B33:B41" si="2">$B$31 &amp; "/" &amp; E33</f>
+        <v>/mng_activity/disciplines-create</v>
       </c>
       <c r="C33" s="25" t="s">
-        <v>63</v>
-      </c>
-      <c r="D33" s="22" t="s">
-        <v>28</v>
-      </c>
+        <v>146</v>
+      </c>
+      <c r="D33" s="22"/>
       <c r="E33" s="25" t="s">
-        <v>114</v>
+        <v>143</v>
       </c>
       <c r="F33" s="25" t="str">
-        <f t="shared" si="0"/>
-        <v>courses.blade.php</v>
+        <f>IF($E33="Da definire",$E33,_xlfn.CONCAT($E33,".blade.php"))</f>
+        <v>disciplines-create.blade.php</v>
       </c>
       <c r="G33" s="25" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="H33" s="22"/>
       <c r="I33" s="13"/>
     </row>
-    <row r="34" spans="1:9" ht="19.899999999999999" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" ht="19.899999999999999" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A34" s="25" t="s">
-        <v>40</v>
+        <v>149</v>
       </c>
       <c r="B34" s="25" t="str">
-        <f>$B$31 &amp; "/" &amp; E34</f>
-        <v>/mng_activity/packages</v>
+        <f t="shared" si="2"/>
+        <v>/mng_activity/discipline-store</v>
       </c>
       <c r="C34" s="25" t="s">
-        <v>63</v>
-      </c>
-      <c r="D34" s="22" t="s">
-        <v>29</v>
-      </c>
+        <v>76</v>
+      </c>
+      <c r="D34" s="22"/>
       <c r="E34" s="25" t="s">
-        <v>116</v>
-      </c>
-      <c r="F34" s="25" t="str">
-        <f t="shared" si="0"/>
-        <v>packages.blade.php</v>
-      </c>
+        <v>151</v>
+      </c>
+      <c r="F34" s="25"/>
       <c r="G34" s="25" t="s">
-        <v>121</v>
+        <v>144</v>
       </c>
       <c r="H34" s="22"/>
       <c r="I34" s="13"/>
     </row>
-    <row r="35" spans="1:9" ht="19.899999999999999" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" ht="19.899999999999999" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A35" s="25" t="s">
-        <v>39</v>
+        <v>150</v>
       </c>
       <c r="B35" s="25" t="str">
-        <f>$B$31 &amp; "/" &amp; E35</f>
-        <v>/mng_activity/rooms</v>
+        <f t="shared" si="2"/>
+        <v>/mng_activity/disciplines-edit</v>
       </c>
       <c r="C35" s="25" t="s">
-        <v>63</v>
-      </c>
-      <c r="D35" s="22" t="s">
-        <v>30</v>
-      </c>
+        <v>146</v>
+      </c>
+      <c r="D35" s="22"/>
       <c r="E35" s="25" t="s">
-        <v>115</v>
+        <v>147</v>
       </c>
       <c r="F35" s="25" t="str">
-        <f t="shared" si="0"/>
-        <v>rooms.blade.php</v>
+        <f>IF($E35="Da definire",$E35,_xlfn.CONCAT($E35,".blade.php"))</f>
+        <v>disciplines-edit.blade.php</v>
       </c>
       <c r="G35" s="25" t="s">
-        <v>121</v>
+        <v>144</v>
       </c>
       <c r="H35" s="22"/>
       <c r="I35" s="13"/>
     </row>
-    <row r="36" spans="1:9" ht="25.5" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" ht="19.899999999999999" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A36" s="25" t="s">
-        <v>41</v>
+        <v>152</v>
       </c>
       <c r="B36" s="25" t="str">
-        <f>$B$31 &amp; "/" &amp; E36</f>
-        <v>/mng_activity/scheduling</v>
+        <f t="shared" si="2"/>
+        <v>/mng_activity/disciplines-update</v>
       </c>
       <c r="C36" s="25" t="s">
-        <v>63</v>
-      </c>
-      <c r="D36" s="22" t="s">
-        <v>31</v>
-      </c>
+        <v>76</v>
+      </c>
+      <c r="D36" s="22"/>
       <c r="E36" s="25" t="s">
-        <v>117</v>
-      </c>
-      <c r="F36" s="25" t="str">
-        <f t="shared" si="0"/>
-        <v>scheduling.blade.php</v>
-      </c>
+        <v>153</v>
+      </c>
+      <c r="F36" s="25"/>
       <c r="G36" s="25" t="s">
-        <v>121</v>
+        <v>144</v>
       </c>
       <c r="H36" s="22"/>
       <c r="I36" s="13"/>
     </row>
-    <row r="37" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="26"/>
-      <c r="B37" s="26" t="str">
-        <f>"/" &amp; E37</f>
+    <row r="37" spans="1:9" ht="19.899999999999999" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="A37" s="25" t="s">
+        <v>154</v>
+      </c>
+      <c r="B37" s="25" t="str">
+        <f t="shared" si="2"/>
+        <v>/mng_activity/disciplines-delete</v>
+      </c>
+      <c r="C37" s="25" t="s">
+        <v>146</v>
+      </c>
+      <c r="D37" s="22"/>
+      <c r="E37" s="25" t="s">
+        <v>148</v>
+      </c>
+      <c r="F37" s="25" t="str">
+        <f>IF($E37="Da definire",$E37,_xlfn.CONCAT($E37,".blade.php"))</f>
+        <v>disciplines-delete.blade.php</v>
+      </c>
+      <c r="G37" s="25" t="s">
+        <v>144</v>
+      </c>
+      <c r="H37" s="22"/>
+      <c r="I37" s="13"/>
+    </row>
+    <row r="38" spans="1:9" ht="19.899999999999999" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="B38" s="25" t="str">
+        <f t="shared" si="2"/>
+        <v>/mng_activity/courses</v>
+      </c>
+      <c r="C38" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="D38" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="E38" s="25" t="s">
+        <v>113</v>
+      </c>
+      <c r="F38" s="25" t="str">
+        <f t="shared" si="0"/>
+        <v>courses.blade.php</v>
+      </c>
+      <c r="G38" s="25" t="s">
+        <v>142</v>
+      </c>
+      <c r="H38" s="22"/>
+      <c r="I38" s="13"/>
+    </row>
+    <row r="39" spans="1:9" ht="19.899999999999999" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="B39" s="25" t="str">
+        <f t="shared" si="2"/>
+        <v>/mng_activity/packages</v>
+      </c>
+      <c r="C39" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="D39" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="E39" s="25" t="s">
+        <v>115</v>
+      </c>
+      <c r="F39" s="25" t="str">
+        <f t="shared" si="0"/>
+        <v>packages.blade.php</v>
+      </c>
+      <c r="G39" s="25" t="s">
+        <v>120</v>
+      </c>
+      <c r="H39" s="22"/>
+      <c r="I39" s="13"/>
+    </row>
+    <row r="40" spans="1:9" ht="19.899999999999999" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="B40" s="25" t="str">
+        <f t="shared" si="2"/>
+        <v>/mng_activity/rooms</v>
+      </c>
+      <c r="C40" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="D40" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="E40" s="25" t="s">
+        <v>114</v>
+      </c>
+      <c r="F40" s="25" t="str">
+        <f t="shared" si="0"/>
+        <v>rooms.blade.php</v>
+      </c>
+      <c r="G40" s="25" t="s">
+        <v>120</v>
+      </c>
+      <c r="H40" s="22"/>
+      <c r="I40" s="13"/>
+    </row>
+    <row r="41" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="B41" s="25" t="str">
+        <f t="shared" si="2"/>
+        <v>/mng_activity/scheduling</v>
+      </c>
+      <c r="C41" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="D41" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="E41" s="25" t="s">
+        <v>116</v>
+      </c>
+      <c r="F41" s="25" t="str">
+        <f t="shared" si="0"/>
+        <v>scheduling.blade.php</v>
+      </c>
+      <c r="G41" s="25" t="s">
+        <v>120</v>
+      </c>
+      <c r="H41" s="22"/>
+      <c r="I41" s="13"/>
+    </row>
+    <row r="42" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="26"/>
+      <c r="B42" s="26" t="str">
+        <f>"/" &amp; E42</f>
         <v>/report_stats</v>
       </c>
-      <c r="C37" s="26" t="s">
-        <v>63</v>
-      </c>
-      <c r="D37" s="23" t="s">
+      <c r="C42" s="26" t="s">
+        <v>63</v>
+      </c>
+      <c r="D42" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="E37" s="26" t="s">
+      <c r="E42" s="26" t="s">
+        <v>97</v>
+      </c>
+      <c r="F42" s="26" t="str">
+        <f t="shared" si="0"/>
+        <v>report_stats.blade.php</v>
+      </c>
+      <c r="G42" s="26" t="s">
+        <v>95</v>
+      </c>
+      <c r="H42" s="23" t="s">
         <v>98</v>
       </c>
-      <c r="F37" s="26" t="str">
-        <f t="shared" si="0"/>
-        <v>report_stats.blade.php</v>
-      </c>
-      <c r="G37" s="26" t="s">
-        <v>96</v>
-      </c>
-      <c r="H37" s="23" t="s">
-        <v>99</v>
-      </c>
-      <c r="I37" s="13"/>
+      <c r="I42" s="13"/>
     </row>
   </sheetData>
   <dataConsolidate/>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B39" xr:uid="{C7F42672-59D8-4A95-9804-4B94DD14E8F6}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B44" xr:uid="{C7F42672-59D8-4A95-9804-4B94DD14E8F6}">
       <formula1>RefView_route</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C37" xr:uid="{F340BA2D-9D43-4A9F-86F9-B281B429D2E7}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C42" xr:uid="{F340BA2D-9D43-4A9F-86F9-B281B429D2E7}">
       <formula1>RefTipo</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G37" xr:uid="{DFF187B0-2821-4C72-B394-0420A8E90996}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G42" xr:uid="{DFF187B0-2821-4C72-B394-0420A8E90996}">
       <formula1>RefController_nome</formula1>
     </dataValidation>
   </dataValidations>
@@ -2275,7 +2427,7 @@
   <dimension ref="B1:G28"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2290,33 +2442,33 @@
   <sheetData>
     <row r="1" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D1" t="s">
         <v>69</v>
       </c>
-      <c r="D1" t="s">
-        <v>70</v>
-      </c>
       <c r="E1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E2" s="5"/>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
-        <v>66</v>
+        <v>146</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E3" s="5"/>
     </row>
@@ -2325,7 +2477,7 @@
         <v>65</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E4" s="5"/>
     </row>
@@ -2334,7 +2486,7 @@
         <v>64</v>
       </c>
       <c r="D5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
@@ -2342,33 +2494,41 @@
         <v>63</v>
       </c>
       <c r="D6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D8" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B9" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="D9" t="s">
         <v>120</v>
-      </c>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="D9" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D10" t="s">
-        <v>143</v>
+        <v>142</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Create le CRUD per corsi
- Finita la creazione
- Da finire la modifica
</commit_message>
<xml_diff>
--- a/Documentazioni/Codifica pagine sito.xlsx
+++ b/Documentazioni/Codifica pagine sito.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr filterPrivacy="1" codeName="Questa_cartella_di_lavoro"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99AE5DD0-C38C-4FA7-86F8-EB1ED213E938}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D1B28B0-93FF-430F-BC21-E59DDF77F7E5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -12,7 +12,7 @@
     <sheet name="Foglio utile" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Main!$A$1:$H$42</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Main!$A$1:$H$47</definedName>
     <definedName name="RefController_nome">Controller[Lista Controller]</definedName>
     <definedName name="RefTipo">Tipo[]</definedName>
   </definedNames>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="165">
   <si>
     <t>Nome gabbia logica</t>
   </si>
@@ -496,6 +496,36 @@
   </si>
   <si>
     <t>M315</t>
+  </si>
+  <si>
+    <t>M321</t>
+  </si>
+  <si>
+    <t>M322</t>
+  </si>
+  <si>
+    <t>M323</t>
+  </si>
+  <si>
+    <t>M324</t>
+  </si>
+  <si>
+    <t>M325</t>
+  </si>
+  <si>
+    <t>courses-create</t>
+  </si>
+  <si>
+    <t>courses-store</t>
+  </si>
+  <si>
+    <t>courses-edit</t>
+  </si>
+  <si>
+    <t>courses-update</t>
+  </si>
+  <si>
+    <t>courses-delete</t>
   </si>
 </sst>
 </file>
@@ -925,8 +955,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{905F6574-56C3-4E36-86AD-16F4E970F9D2}" name="Tabella4" displayName="Tabella4" ref="A1:H42" dataDxfId="17">
-  <autoFilter ref="A1:H42" xr:uid="{34684D11-7ACD-45A4-AA96-0CE6C7239D98}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{905F6574-56C3-4E36-86AD-16F4E970F9D2}" name="Tabella4" displayName="Tabella4" ref="A1:H47" dataDxfId="17">
+  <autoFilter ref="A1:H47" xr:uid="{34684D11-7ACD-45A4-AA96-0CE6C7239D98}">
+    <filterColumn colId="6">
+      <filters>
+        <filter val="CourseController"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{E7D98D43-EB7B-46CE-B0B0-C555D83773A6}" name="Codice gabbia logica" dataDxfId="16" totalsRowDxfId="15"/>
     <tableColumn id="8" xr3:uid="{CAF26B0C-D3E2-4A71-A7C5-519E983C334C}" name="Rotta" dataDxfId="14" totalsRowDxfId="13">
@@ -1234,10 +1270,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Foglio2"/>
-  <dimension ref="A1:I42"/>
+  <dimension ref="A1:I47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G39" sqref="G38:G43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" outlineLevelRow="2" x14ac:dyDescent="0.25"/>
@@ -1284,7 +1320,7 @@
       </c>
       <c r="I1" s="13"/>
     </row>
-    <row r="2" spans="1:9" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="19.899999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>43</v>
       </c>
@@ -1302,7 +1338,7 @@
         <v>61</v>
       </c>
       <c r="F2" s="18" t="str">
-        <f t="shared" ref="F2:F42" si="0">IF($E2="Da definire",$E2,_xlfn.CONCAT($E2,".blade.php"))</f>
+        <f t="shared" ref="F2:F47" si="0">IF($E2="Da definire",$E2,_xlfn.CONCAT($E2,".blade.php"))</f>
         <v>welcome.blade.php</v>
       </c>
       <c r="G2" s="18" t="s">
@@ -1313,7 +1349,7 @@
       </c>
       <c r="I2" s="13"/>
     </row>
-    <row r="3" spans="1:9" ht="19.899999999999999" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="19.899999999999999" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A3" s="18"/>
       <c r="B3" s="18" t="str">
         <f>"/" &amp; E3</f>
@@ -1333,7 +1369,7 @@
       </c>
       <c r="I3" s="13"/>
     </row>
-    <row r="4" spans="1:9" ht="19.899999999999999" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="19.899999999999999" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
         <v>139</v>
       </c>
@@ -1360,7 +1396,7 @@
       </c>
       <c r="I4" s="13"/>
     </row>
-    <row r="5" spans="1:9" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="19.899999999999999" hidden="1" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
         <v>44</v>
       </c>
@@ -1389,7 +1425,7 @@
       </c>
       <c r="I5" s="13"/>
     </row>
-    <row r="6" spans="1:9" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="19.899999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
         <v>53</v>
       </c>
@@ -1418,7 +1454,7 @@
       </c>
       <c r="I6" s="13"/>
     </row>
-    <row r="7" spans="1:9" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="19.899999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
         <v>126</v>
       </c>
@@ -1447,7 +1483,7 @@
       </c>
       <c r="I7" s="12"/>
     </row>
-    <row r="8" spans="1:9" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="19.899999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
         <v>45</v>
       </c>
@@ -1476,7 +1512,7 @@
       </c>
       <c r="I8" s="12"/>
     </row>
-    <row r="9" spans="1:9" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="19.899999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
         <v>47</v>
       </c>
@@ -1505,7 +1541,7 @@
       </c>
       <c r="I9" s="12"/>
     </row>
-    <row r="10" spans="1:9" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="19.899999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
         <v>49</v>
       </c>
@@ -1534,7 +1570,7 @@
       </c>
       <c r="I10" s="13"/>
     </row>
-    <row r="11" spans="1:9" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="19.899999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="18" t="s">
         <v>51</v>
       </c>
@@ -1563,7 +1599,7 @@
       </c>
       <c r="I11" s="13"/>
     </row>
-    <row r="12" spans="1:9" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="19.899999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
         <v>54</v>
       </c>
@@ -1592,7 +1628,7 @@
       </c>
       <c r="I12" s="13"/>
     </row>
-    <row r="13" spans="1:9" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="19.899999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
         <v>57</v>
       </c>
@@ -1621,7 +1657,7 @@
       </c>
       <c r="I13" s="13"/>
     </row>
-    <row r="14" spans="1:9" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="19.899999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="18" t="s">
         <v>58</v>
       </c>
@@ -1650,7 +1686,7 @@
       </c>
       <c r="I14" s="13"/>
     </row>
-    <row r="15" spans="1:9" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="19.899999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="28" t="s">
         <v>42</v>
       </c>
@@ -1679,7 +1715,7 @@
       </c>
       <c r="I15" s="13"/>
     </row>
-    <row r="16" spans="1:9" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="19.899999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="26"/>
       <c r="B16" s="26" t="str">
         <f t="shared" si="1"/>
@@ -1706,7 +1742,7 @@
       </c>
       <c r="I16" s="13"/>
     </row>
-    <row r="17" spans="1:9" ht="19.899999999999999" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" ht="19.899999999999999" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A17" s="27" t="s">
         <v>18</v>
       </c>
@@ -1735,7 +1771,7 @@
       </c>
       <c r="I17" s="13"/>
     </row>
-    <row r="18" spans="1:9" ht="19.899999999999999" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" ht="19.899999999999999" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A18" s="25" t="s">
         <v>19</v>
       </c>
@@ -1762,7 +1798,7 @@
       <c r="H18" s="22"/>
       <c r="I18" s="13"/>
     </row>
-    <row r="19" spans="1:9" ht="19.899999999999999" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" ht="19.899999999999999" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A19" s="25" t="s">
         <v>20</v>
       </c>
@@ -1789,7 +1825,7 @@
       <c r="H19" s="22"/>
       <c r="I19" s="13"/>
     </row>
-    <row r="20" spans="1:9" ht="19.899999999999999" customHeight="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" ht="19.899999999999999" hidden="1" customHeight="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A20" s="25" t="s">
         <v>21</v>
       </c>
@@ -1816,7 +1852,7 @@
       <c r="H20" s="22"/>
       <c r="I20" s="13"/>
     </row>
-    <row r="21" spans="1:9" ht="19.899999999999999" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" ht="19.899999999999999" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A21" s="25" t="s">
         <v>22</v>
       </c>
@@ -1843,7 +1879,7 @@
       <c r="H21" s="22"/>
       <c r="I21" s="13"/>
     </row>
-    <row r="22" spans="1:9" ht="19.899999999999999" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" ht="19.899999999999999" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A22" s="27" t="s">
         <v>23</v>
       </c>
@@ -1872,7 +1908,7 @@
       </c>
       <c r="I22" s="13"/>
     </row>
-    <row r="23" spans="1:9" ht="19.899999999999999" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" ht="19.899999999999999" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A23" s="25" t="s">
         <v>24</v>
       </c>
@@ -1899,7 +1935,7 @@
       <c r="H23" s="22"/>
       <c r="I23" s="13"/>
     </row>
-    <row r="24" spans="1:9" ht="19.899999999999999" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" ht="19.899999999999999" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A24" s="25" t="s">
         <v>25</v>
       </c>
@@ -1926,7 +1962,7 @@
       <c r="H24" s="22"/>
       <c r="I24" s="13"/>
     </row>
-    <row r="25" spans="1:9" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" ht="19.899999999999999" hidden="1" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A25" s="26"/>
       <c r="B25" s="26" t="str">
         <f>"/" &amp; E25</f>
@@ -1953,7 +1989,7 @@
       </c>
       <c r="I25" s="13"/>
     </row>
-    <row r="26" spans="1:9" ht="19.899999999999999" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" ht="19.899999999999999" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A26" s="27" t="s">
         <v>26</v>
       </c>
@@ -1982,7 +2018,7 @@
       </c>
       <c r="I26" s="13"/>
     </row>
-    <row r="27" spans="1:9" ht="19.899999999999999" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" ht="19.899999999999999" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A27" s="25" t="s">
         <v>35</v>
       </c>
@@ -2009,7 +2045,7 @@
       <c r="H27" s="22"/>
       <c r="I27" s="13"/>
     </row>
-    <row r="28" spans="1:9" ht="19.899999999999999" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" ht="19.899999999999999" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A28" s="25" t="s">
         <v>128</v>
       </c>
@@ -2036,7 +2072,7 @@
       <c r="H28" s="22"/>
       <c r="I28" s="13"/>
     </row>
-    <row r="29" spans="1:9" ht="19.899999999999999" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" ht="19.899999999999999" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A29" s="25" t="s">
         <v>129</v>
       </c>
@@ -2063,7 +2099,7 @@
       <c r="H29" s="22"/>
       <c r="I29" s="13"/>
     </row>
-    <row r="30" spans="1:9" ht="19.899999999999999" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" ht="19.899999999999999" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A30" s="27" t="s">
         <v>36</v>
       </c>
@@ -2090,7 +2126,7 @@
       <c r="H30" s="21"/>
       <c r="I30" s="13"/>
     </row>
-    <row r="31" spans="1:9" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" ht="19.899999999999999" hidden="1" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A31" s="26"/>
       <c r="B31" s="26" t="str">
         <f>"/" &amp; E31</f>
@@ -2117,7 +2153,7 @@
       </c>
       <c r="I31" s="13"/>
     </row>
-    <row r="32" spans="1:9" ht="19.899999999999999" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" ht="19.899999999999999" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A32" s="25" t="s">
         <v>37</v>
       </c>
@@ -2128,7 +2164,7 @@
       <c r="C32" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="D32" s="22" t="s">
+      <c r="D32" s="25" t="s">
         <v>27</v>
       </c>
       <c r="E32" s="25" t="s">
@@ -2144,12 +2180,12 @@
       <c r="H32" s="22"/>
       <c r="I32" s="13"/>
     </row>
-    <row r="33" spans="1:9" ht="19.899999999999999" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" ht="19.899999999999999" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A33" s="25" t="s">
         <v>145</v>
       </c>
       <c r="B33" s="25" t="str">
-        <f t="shared" ref="B33:B41" si="2">$B$31 &amp; "/" &amp; E33</f>
+        <f t="shared" ref="B33:B46" si="2">$B$31 &amp; "/" &amp; E33</f>
         <v>/mng_activity/disciplines-create</v>
       </c>
       <c r="C33" s="25" t="s">
@@ -2169,7 +2205,7 @@
       <c r="H33" s="22"/>
       <c r="I33" s="13"/>
     </row>
-    <row r="34" spans="1:9" ht="19.899999999999999" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" ht="19.899999999999999" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A34" s="25" t="s">
         <v>149</v>
       </c>
@@ -2191,7 +2227,7 @@
       <c r="H34" s="22"/>
       <c r="I34" s="13"/>
     </row>
-    <row r="35" spans="1:9" ht="19.899999999999999" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" ht="19.899999999999999" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A35" s="25" t="s">
         <v>150</v>
       </c>
@@ -2216,7 +2252,7 @@
       <c r="H35" s="22"/>
       <c r="I35" s="13"/>
     </row>
-    <row r="36" spans="1:9" ht="19.899999999999999" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" ht="19.899999999999999" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A36" s="25" t="s">
         <v>152</v>
       </c>
@@ -2238,12 +2274,12 @@
       <c r="H36" s="22"/>
       <c r="I36" s="13"/>
     </row>
-    <row r="37" spans="1:9" ht="19.899999999999999" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" ht="19.899999999999999" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A37" s="25" t="s">
         <v>154</v>
       </c>
       <c r="B37" s="25" t="str">
-        <f t="shared" si="2"/>
+        <f>$B$31 &amp; "/" &amp; E37</f>
         <v>/mng_activity/disciplines-delete</v>
       </c>
       <c r="C37" s="25" t="s">
@@ -2263,7 +2299,7 @@
       <c r="H37" s="22"/>
       <c r="I37" s="13"/>
     </row>
-    <row r="38" spans="1:9" ht="19.899999999999999" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" ht="19.899999999999999" customHeight="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A38" s="25" t="s">
         <v>38</v>
       </c>
@@ -2274,7 +2310,7 @@
       <c r="C38" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="D38" s="22" t="s">
+      <c r="D38" s="25" t="s">
         <v>28</v>
       </c>
       <c r="E38" s="25" t="s">
@@ -2290,124 +2326,240 @@
       <c r="H38" s="22"/>
       <c r="I38" s="13"/>
     </row>
-    <row r="39" spans="1:9" ht="19.899999999999999" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" ht="19.899999999999999" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A39" s="25" t="s">
+        <v>155</v>
+      </c>
+      <c r="B39" s="25" t="str">
+        <f t="shared" ref="B39:B43" si="3">$B$31 &amp; "/" &amp; E39</f>
+        <v>/mng_activity/courses-create</v>
+      </c>
+      <c r="C39" s="25" t="s">
+        <v>146</v>
+      </c>
+      <c r="D39" s="22"/>
+      <c r="E39" s="25" t="s">
+        <v>160</v>
+      </c>
+      <c r="F39" s="25" t="str">
+        <f>IF($E39="Da definire",$E39,_xlfn.CONCAT($E39,".blade.php"))</f>
+        <v>courses-create.blade.php</v>
+      </c>
+      <c r="G39" s="25" t="s">
+        <v>142</v>
+      </c>
+      <c r="H39" s="22"/>
+      <c r="I39" s="13"/>
+    </row>
+    <row r="40" spans="1:9" ht="19.899999999999999" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="A40" s="25" t="s">
+        <v>156</v>
+      </c>
+      <c r="B40" s="25" t="str">
+        <f t="shared" si="3"/>
+        <v>/mng_activity/courses-store</v>
+      </c>
+      <c r="C40" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="D40" s="22"/>
+      <c r="E40" s="25" t="s">
+        <v>161</v>
+      </c>
+      <c r="F40" s="25"/>
+      <c r="G40" s="25" t="s">
+        <v>142</v>
+      </c>
+      <c r="H40" s="22"/>
+      <c r="I40" s="13"/>
+    </row>
+    <row r="41" spans="1:9" ht="19.899999999999999" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="A41" s="25" t="s">
+        <v>157</v>
+      </c>
+      <c r="B41" s="25" t="str">
+        <f t="shared" si="3"/>
+        <v>/mng_activity/courses-edit</v>
+      </c>
+      <c r="C41" s="25" t="s">
+        <v>146</v>
+      </c>
+      <c r="D41" s="22"/>
+      <c r="E41" s="25" t="s">
+        <v>162</v>
+      </c>
+      <c r="F41" s="25" t="str">
+        <f>IF($E41="Da definire",$E41,_xlfn.CONCAT($E41,".blade.php"))</f>
+        <v>courses-edit.blade.php</v>
+      </c>
+      <c r="G41" s="25" t="s">
+        <v>142</v>
+      </c>
+      <c r="H41" s="22"/>
+      <c r="I41" s="13"/>
+    </row>
+    <row r="42" spans="1:9" ht="19.899999999999999" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="A42" s="25" t="s">
+        <v>158</v>
+      </c>
+      <c r="B42" s="25" t="str">
+        <f t="shared" si="3"/>
+        <v>/mng_activity/courses-update</v>
+      </c>
+      <c r="C42" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="D42" s="22"/>
+      <c r="E42" s="25" t="s">
+        <v>163</v>
+      </c>
+      <c r="F42" s="25"/>
+      <c r="G42" s="25" t="s">
+        <v>142</v>
+      </c>
+      <c r="H42" s="22"/>
+      <c r="I42" s="13"/>
+    </row>
+    <row r="43" spans="1:9" ht="19.899999999999999" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="A43" s="25" t="s">
+        <v>159</v>
+      </c>
+      <c r="B43" s="25" t="str">
+        <f>$B$31 &amp; "/" &amp; E43</f>
+        <v>/mng_activity/courses-delete</v>
+      </c>
+      <c r="C43" s="25" t="s">
+        <v>146</v>
+      </c>
+      <c r="D43" s="22"/>
+      <c r="E43" s="25" t="s">
+        <v>164</v>
+      </c>
+      <c r="F43" s="25" t="str">
+        <f>IF($E43="Da definire",$E43,_xlfn.CONCAT($E43,".blade.php"))</f>
+        <v>courses-delete.blade.php</v>
+      </c>
+      <c r="G43" s="25" t="s">
+        <v>142</v>
+      </c>
+      <c r="H43" s="22"/>
+      <c r="I43" s="13"/>
+    </row>
+    <row r="44" spans="1:9" ht="19.899999999999999" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="B39" s="25" t="str">
+      <c r="B44" s="25" t="str">
         <f t="shared" si="2"/>
         <v>/mng_activity/packages</v>
       </c>
-      <c r="C39" s="25" t="s">
+      <c r="C44" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="D39" s="22" t="s">
+      <c r="D44" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="E39" s="25" t="s">
+      <c r="E44" s="25" t="s">
         <v>115</v>
       </c>
-      <c r="F39" s="25" t="str">
+      <c r="F44" s="25" t="str">
         <f t="shared" si="0"/>
         <v>packages.blade.php</v>
       </c>
-      <c r="G39" s="25" t="s">
+      <c r="G44" s="25" t="s">
         <v>120</v>
       </c>
-      <c r="H39" s="22"/>
-      <c r="I39" s="13"/>
-    </row>
-    <row r="40" spans="1:9" ht="19.899999999999999" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="25" t="s">
+      <c r="H44" s="22"/>
+      <c r="I44" s="13"/>
+    </row>
+    <row r="45" spans="1:9" ht="19.899999999999999" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="B40" s="25" t="str">
+      <c r="B45" s="25" t="str">
         <f t="shared" si="2"/>
         <v>/mng_activity/rooms</v>
       </c>
-      <c r="C40" s="25" t="s">
+      <c r="C45" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="D40" s="22" t="s">
+      <c r="D45" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="E40" s="25" t="s">
+      <c r="E45" s="25" t="s">
         <v>114</v>
       </c>
-      <c r="F40" s="25" t="str">
+      <c r="F45" s="25" t="str">
         <f t="shared" si="0"/>
         <v>rooms.blade.php</v>
       </c>
-      <c r="G40" s="25" t="s">
+      <c r="G45" s="25" t="s">
         <v>120</v>
       </c>
-      <c r="H40" s="22"/>
-      <c r="I40" s="13"/>
-    </row>
-    <row r="41" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="25" t="s">
+      <c r="H45" s="22"/>
+      <c r="I45" s="13"/>
+    </row>
+    <row r="46" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="B41" s="25" t="str">
+      <c r="B46" s="25" t="str">
         <f t="shared" si="2"/>
         <v>/mng_activity/scheduling</v>
       </c>
-      <c r="C41" s="25" t="s">
+      <c r="C46" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="D41" s="22" t="s">
+      <c r="D46" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="E41" s="25" t="s">
+      <c r="E46" s="25" t="s">
         <v>116</v>
       </c>
-      <c r="F41" s="25" t="str">
+      <c r="F46" s="25" t="str">
         <f t="shared" si="0"/>
         <v>scheduling.blade.php</v>
       </c>
-      <c r="G41" s="25" t="s">
+      <c r="G46" s="25" t="s">
         <v>120</v>
       </c>
-      <c r="H41" s="22"/>
-      <c r="I41" s="13"/>
-    </row>
-    <row r="42" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="26"/>
-      <c r="B42" s="26" t="str">
-        <f>"/" &amp; E42</f>
+      <c r="H46" s="22"/>
+      <c r="I46" s="13"/>
+    </row>
+    <row r="47" spans="1:9" ht="21" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="26"/>
+      <c r="B47" s="26" t="str">
+        <f>"/" &amp; E47</f>
         <v>/report_stats</v>
       </c>
-      <c r="C42" s="26" t="s">
+      <c r="C47" s="26" t="s">
         <v>63</v>
       </c>
-      <c r="D42" s="23" t="s">
+      <c r="D47" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="E42" s="26" t="s">
+      <c r="E47" s="26" t="s">
         <v>97</v>
       </c>
-      <c r="F42" s="26" t="str">
+      <c r="F47" s="26" t="str">
         <f t="shared" si="0"/>
         <v>report_stats.blade.php</v>
       </c>
-      <c r="G42" s="26" t="s">
+      <c r="G47" s="26" t="s">
         <v>95</v>
       </c>
-      <c r="H42" s="23" t="s">
+      <c r="H47" s="23" t="s">
         <v>98</v>
       </c>
-      <c r="I42" s="13"/>
+      <c r="I47" s="13"/>
     </row>
   </sheetData>
   <dataConsolidate/>
-  <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B44" xr:uid="{C7F42672-59D8-4A95-9804-4B94DD14E8F6}">
-      <formula1>RefView_route</formula1>
-    </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C42" xr:uid="{F340BA2D-9D43-4A9F-86F9-B281B429D2E7}">
+  <dataValidations count="2">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C47" xr:uid="{F340BA2D-9D43-4A9F-86F9-B281B429D2E7}">
       <formula1>RefTipo</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G42" xr:uid="{DFF187B0-2821-4C72-B394-0420A8E90996}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G47" xr:uid="{DFF187B0-2821-4C72-B394-0420A8E90996}">
       <formula1>RefController_nome</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Finito le CRUD di Corsi
- Messi i placeholder agli input form
- Settato il costo_orario come float
</commit_message>
<xml_diff>
--- a/Documentazioni/Codifica pagine sito.xlsx
+++ b/Documentazioni/Codifica pagine sito.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
   <workbookPr filterPrivacy="1" codeName="Questa_cartella_di_lavoro"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D1B28B0-93FF-430F-BC21-E59DDF77F7E5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2802ED81-8AA9-4CB5-B2EE-AE2DAA403E97}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -24,6 +24,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -984,7 +985,7 @@
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{45120F09-8607-4F6A-A989-7184307236A1}" name="Tipo" displayName="Tipo" ref="B1:B9" totalsRowShown="0" headerRowDxfId="2" tableBorderDxfId="1">
   <autoFilter ref="B1:B9" xr:uid="{B0803B6A-3448-4A89-AC43-1127F3DBD833}"/>
-  <sortState ref="B2:B8">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:B8">
     <sortCondition ref="B1:B8"/>
   </sortState>
   <tableColumns count="1">
@@ -1273,27 +1274,27 @@
   <dimension ref="A1:I47"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G39" sqref="G38:G43"/>
+      <selection activeCell="D55" sqref="D55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" outlineLevelRow="2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" outlineLevelRow="2" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.5703125" style="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.5546875" style="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.109375" style="13" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13" style="12" customWidth="1"/>
-    <col min="4" max="4" width="35.5703125" style="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" style="15" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.42578125" style="13" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="88.42578125" style="13" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="89.7109375" style="11" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="28.7109375" style="13" customWidth="1"/>
-    <col min="11" max="12" width="8.85546875" style="13"/>
+    <col min="4" max="4" width="35.5546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.33203125" style="15" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.44140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="88.44140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="89.6640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="28.6640625" style="13" customWidth="1"/>
+    <col min="11" max="12" width="8.88671875" style="13"/>
     <col min="13" max="13" width="19" style="13" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="8.85546875" style="13"/>
+    <col min="14" max="16384" width="8.88671875" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
         <v>1</v>
       </c>
@@ -1320,7 +1321,7 @@
       </c>
       <c r="I1" s="13"/>
     </row>
-    <row r="2" spans="1:9" ht="19.899999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="19.95" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
         <v>43</v>
       </c>
@@ -1349,7 +1350,7 @@
       </c>
       <c r="I2" s="13"/>
     </row>
-    <row r="3" spans="1:9" ht="19.899999999999999" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="19.95" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A3" s="18"/>
       <c r="B3" s="18" t="str">
         <f>"/" &amp; E3</f>
@@ -1369,7 +1370,7 @@
       </c>
       <c r="I3" s="13"/>
     </row>
-    <row r="4" spans="1:9" ht="19.899999999999999" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="19.95" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
         <v>139</v>
       </c>
@@ -1396,7 +1397,7 @@
       </c>
       <c r="I4" s="13"/>
     </row>
-    <row r="5" spans="1:9" ht="19.899999999999999" hidden="1" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="19.95" hidden="1" customHeight="1" collapsed="1" x14ac:dyDescent="0.3">
       <c r="A5" s="18" t="s">
         <v>44</v>
       </c>
@@ -1425,7 +1426,7 @@
       </c>
       <c r="I5" s="13"/>
     </row>
-    <row r="6" spans="1:9" ht="19.899999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="19.95" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="18" t="s">
         <v>53</v>
       </c>
@@ -1454,7 +1455,7 @@
       </c>
       <c r="I6" s="13"/>
     </row>
-    <row r="7" spans="1:9" ht="19.899999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="19.95" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="18" t="s">
         <v>126</v>
       </c>
@@ -1483,7 +1484,7 @@
       </c>
       <c r="I7" s="12"/>
     </row>
-    <row r="8" spans="1:9" ht="19.899999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="19.95" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="18" t="s">
         <v>45</v>
       </c>
@@ -1512,7 +1513,7 @@
       </c>
       <c r="I8" s="12"/>
     </row>
-    <row r="9" spans="1:9" ht="19.899999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="19.95" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="18" t="s">
         <v>47</v>
       </c>
@@ -1541,7 +1542,7 @@
       </c>
       <c r="I9" s="12"/>
     </row>
-    <row r="10" spans="1:9" ht="19.899999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="19.95" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="18" t="s">
         <v>49</v>
       </c>
@@ -1570,7 +1571,7 @@
       </c>
       <c r="I10" s="13"/>
     </row>
-    <row r="11" spans="1:9" ht="19.899999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="19.95" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="18" t="s">
         <v>51</v>
       </c>
@@ -1599,7 +1600,7 @@
       </c>
       <c r="I11" s="13"/>
     </row>
-    <row r="12" spans="1:9" ht="19.899999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="19.95" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="18" t="s">
         <v>54</v>
       </c>
@@ -1628,7 +1629,7 @@
       </c>
       <c r="I12" s="13"/>
     </row>
-    <row r="13" spans="1:9" ht="19.899999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="19.95" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="18" t="s">
         <v>57</v>
       </c>
@@ -1657,7 +1658,7 @@
       </c>
       <c r="I13" s="13"/>
     </row>
-    <row r="14" spans="1:9" ht="19.899999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="19.95" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="18" t="s">
         <v>58</v>
       </c>
@@ -1686,7 +1687,7 @@
       </c>
       <c r="I14" s="13"/>
     </row>
-    <row r="15" spans="1:9" ht="19.899999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="19.95" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="28" t="s">
         <v>42</v>
       </c>
@@ -1715,7 +1716,7 @@
       </c>
       <c r="I15" s="13"/>
     </row>
-    <row r="16" spans="1:9" ht="19.899999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="19.95" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="26"/>
       <c r="B16" s="26" t="str">
         <f t="shared" si="1"/>
@@ -1742,7 +1743,7 @@
       </c>
       <c r="I16" s="13"/>
     </row>
-    <row r="17" spans="1:9" ht="19.899999999999999" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" ht="19.95" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A17" s="27" t="s">
         <v>18</v>
       </c>
@@ -1771,7 +1772,7 @@
       </c>
       <c r="I17" s="13"/>
     </row>
-    <row r="18" spans="1:9" ht="19.899999999999999" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" ht="19.95" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A18" s="25" t="s">
         <v>19</v>
       </c>
@@ -1798,7 +1799,7 @@
       <c r="H18" s="22"/>
       <c r="I18" s="13"/>
     </row>
-    <row r="19" spans="1:9" ht="19.899999999999999" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" ht="19.95" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A19" s="25" t="s">
         <v>20</v>
       </c>
@@ -1825,7 +1826,7 @@
       <c r="H19" s="22"/>
       <c r="I19" s="13"/>
     </row>
-    <row r="20" spans="1:9" ht="19.899999999999999" hidden="1" customHeight="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" ht="19.95" hidden="1" customHeight="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.3">
       <c r="A20" s="25" t="s">
         <v>21</v>
       </c>
@@ -1852,7 +1853,7 @@
       <c r="H20" s="22"/>
       <c r="I20" s="13"/>
     </row>
-    <row r="21" spans="1:9" ht="19.899999999999999" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" ht="19.95" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A21" s="25" t="s">
         <v>22</v>
       </c>
@@ -1879,7 +1880,7 @@
       <c r="H21" s="22"/>
       <c r="I21" s="13"/>
     </row>
-    <row r="22" spans="1:9" ht="19.899999999999999" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" ht="19.95" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A22" s="27" t="s">
         <v>23</v>
       </c>
@@ -1908,7 +1909,7 @@
       </c>
       <c r="I22" s="13"/>
     </row>
-    <row r="23" spans="1:9" ht="19.899999999999999" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" ht="19.95" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A23" s="25" t="s">
         <v>24</v>
       </c>
@@ -1935,7 +1936,7 @@
       <c r="H23" s="22"/>
       <c r="I23" s="13"/>
     </row>
-    <row r="24" spans="1:9" ht="19.899999999999999" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" ht="19.95" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A24" s="25" t="s">
         <v>25</v>
       </c>
@@ -1962,7 +1963,7 @@
       <c r="H24" s="22"/>
       <c r="I24" s="13"/>
     </row>
-    <row r="25" spans="1:9" ht="19.899999999999999" hidden="1" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" ht="19.95" hidden="1" customHeight="1" collapsed="1" x14ac:dyDescent="0.3">
       <c r="A25" s="26"/>
       <c r="B25" s="26" t="str">
         <f>"/" &amp; E25</f>
@@ -1989,7 +1990,7 @@
       </c>
       <c r="I25" s="13"/>
     </row>
-    <row r="26" spans="1:9" ht="19.899999999999999" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" ht="19.95" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A26" s="27" t="s">
         <v>26</v>
       </c>
@@ -2018,7 +2019,7 @@
       </c>
       <c r="I26" s="13"/>
     </row>
-    <row r="27" spans="1:9" ht="19.899999999999999" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" ht="19.95" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A27" s="25" t="s">
         <v>35</v>
       </c>
@@ -2045,7 +2046,7 @@
       <c r="H27" s="22"/>
       <c r="I27" s="13"/>
     </row>
-    <row r="28" spans="1:9" ht="19.899999999999999" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" ht="19.95" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A28" s="25" t="s">
         <v>128</v>
       </c>
@@ -2072,7 +2073,7 @@
       <c r="H28" s="22"/>
       <c r="I28" s="13"/>
     </row>
-    <row r="29" spans="1:9" ht="19.899999999999999" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" ht="19.95" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A29" s="25" t="s">
         <v>129</v>
       </c>
@@ -2099,7 +2100,7 @@
       <c r="H29" s="22"/>
       <c r="I29" s="13"/>
     </row>
-    <row r="30" spans="1:9" ht="19.899999999999999" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" ht="19.95" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A30" s="27" t="s">
         <v>36</v>
       </c>
@@ -2126,7 +2127,7 @@
       <c r="H30" s="21"/>
       <c r="I30" s="13"/>
     </row>
-    <row r="31" spans="1:9" ht="19.899999999999999" hidden="1" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" ht="19.95" hidden="1" customHeight="1" collapsed="1" x14ac:dyDescent="0.3">
       <c r="A31" s="26"/>
       <c r="B31" s="26" t="str">
         <f>"/" &amp; E31</f>
@@ -2153,7 +2154,7 @@
       </c>
       <c r="I31" s="13"/>
     </row>
-    <row r="32" spans="1:9" ht="19.899999999999999" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" ht="19.95" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A32" s="25" t="s">
         <v>37</v>
       </c>
@@ -2175,12 +2176,12 @@
         <v>disciplines.blade.php</v>
       </c>
       <c r="G32" s="25" t="s">
-        <v>120</v>
+        <v>144</v>
       </c>
       <c r="H32" s="22"/>
       <c r="I32" s="13"/>
     </row>
-    <row r="33" spans="1:9" ht="19.899999999999999" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" ht="19.95" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A33" s="25" t="s">
         <v>145</v>
       </c>
@@ -2205,7 +2206,7 @@
       <c r="H33" s="22"/>
       <c r="I33" s="13"/>
     </row>
-    <row r="34" spans="1:9" ht="19.899999999999999" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" ht="19.95" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A34" s="25" t="s">
         <v>149</v>
       </c>
@@ -2227,7 +2228,7 @@
       <c r="H34" s="22"/>
       <c r="I34" s="13"/>
     </row>
-    <row r="35" spans="1:9" ht="19.899999999999999" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" ht="19.95" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A35" s="25" t="s">
         <v>150</v>
       </c>
@@ -2252,7 +2253,7 @@
       <c r="H35" s="22"/>
       <c r="I35" s="13"/>
     </row>
-    <row r="36" spans="1:9" ht="19.899999999999999" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" ht="19.95" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A36" s="25" t="s">
         <v>152</v>
       </c>
@@ -2274,7 +2275,7 @@
       <c r="H36" s="22"/>
       <c r="I36" s="13"/>
     </row>
-    <row r="37" spans="1:9" ht="19.899999999999999" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" ht="19.95" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A37" s="25" t="s">
         <v>154</v>
       </c>
@@ -2299,7 +2300,7 @@
       <c r="H37" s="22"/>
       <c r="I37" s="13"/>
     </row>
-    <row r="38" spans="1:9" ht="19.899999999999999" customHeight="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" ht="19.95" customHeight="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.3">
       <c r="A38" s="25" t="s">
         <v>38</v>
       </c>
@@ -2326,12 +2327,12 @@
       <c r="H38" s="22"/>
       <c r="I38" s="13"/>
     </row>
-    <row r="39" spans="1:9" ht="19.899999999999999" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" ht="19.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A39" s="25" t="s">
         <v>155</v>
       </c>
       <c r="B39" s="25" t="str">
-        <f t="shared" ref="B39:B43" si="3">$B$31 &amp; "/" &amp; E39</f>
+        <f t="shared" ref="B39:B42" si="3">$B$31 &amp; "/" &amp; E39</f>
         <v>/mng_activity/courses-create</v>
       </c>
       <c r="C39" s="25" t="s">
@@ -2351,7 +2352,7 @@
       <c r="H39" s="22"/>
       <c r="I39" s="13"/>
     </row>
-    <row r="40" spans="1:9" ht="19.899999999999999" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" ht="19.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A40" s="25" t="s">
         <v>156</v>
       </c>
@@ -2373,7 +2374,7 @@
       <c r="H40" s="22"/>
       <c r="I40" s="13"/>
     </row>
-    <row r="41" spans="1:9" ht="19.899999999999999" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" ht="19.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A41" s="25" t="s">
         <v>157</v>
       </c>
@@ -2398,7 +2399,7 @@
       <c r="H41" s="22"/>
       <c r="I41" s="13"/>
     </row>
-    <row r="42" spans="1:9" ht="19.899999999999999" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" ht="19.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A42" s="25" t="s">
         <v>158</v>
       </c>
@@ -2420,7 +2421,7 @@
       <c r="H42" s="22"/>
       <c r="I42" s="13"/>
     </row>
-    <row r="43" spans="1:9" ht="19.899999999999999" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" ht="19.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A43" s="25" t="s">
         <v>159</v>
       </c>
@@ -2445,7 +2446,7 @@
       <c r="H43" s="22"/>
       <c r="I43" s="13"/>
     </row>
-    <row r="44" spans="1:9" ht="19.899999999999999" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" ht="19.95" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A44" s="25" t="s">
         <v>40</v>
       </c>
@@ -2472,7 +2473,7 @@
       <c r="H44" s="22"/>
       <c r="I44" s="13"/>
     </row>
-    <row r="45" spans="1:9" ht="19.899999999999999" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" ht="19.95" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A45" s="25" t="s">
         <v>39</v>
       </c>
@@ -2499,7 +2500,7 @@
       <c r="H45" s="22"/>
       <c r="I45" s="13"/>
     </row>
-    <row r="46" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A46" s="25" t="s">
         <v>41</v>
       </c>
@@ -2526,7 +2527,7 @@
       <c r="H46" s="22"/>
       <c r="I46" s="13"/>
     </row>
-    <row r="47" spans="1:9" ht="21" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" ht="21" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="26"/>
       <c r="B47" s="26" t="str">
         <f>"/" &amp; E47</f>
@@ -2582,17 +2583,17 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="6" width="25.140625" customWidth="1"/>
-    <col min="7" max="7" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="6" width="25.109375" customWidth="1"/>
+    <col min="7" max="7" width="24.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="19" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>68</v>
       </c>
@@ -2606,7 +2607,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="3" t="s">
         <v>66</v>
       </c>
@@ -2615,7 +2616,7 @@
       </c>
       <c r="E2" s="5"/>
     </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B3" s="2" t="s">
         <v>146</v>
       </c>
@@ -2624,7 +2625,7 @@
       </c>
       <c r="E3" s="5"/>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B4" s="3" t="s">
         <v>65</v>
       </c>
@@ -2633,7 +2634,7 @@
       </c>
       <c r="E4" s="5"/>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
         <v>64</v>
       </c>
@@ -2641,7 +2642,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B6" s="4" t="s">
         <v>63</v>
       </c>
@@ -2649,7 +2650,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B7" s="4" t="s">
         <v>87</v>
       </c>
@@ -2657,7 +2658,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B8" s="4" t="s">
         <v>96</v>
       </c>
@@ -2665,7 +2666,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B9" s="4" t="s">
         <v>76</v>
       </c>
@@ -2673,27 +2674,27 @@
         <v>120</v>
       </c>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:7" x14ac:dyDescent="0.3">
       <c r="D10" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:7" x14ac:dyDescent="0.3">
       <c r="D11" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B15" s="17"/>
       <c r="C15" s="16"/>
       <c r="D15" s="16"/>
       <c r="E15" s="16"/>
     </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B16" s="9"/>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
@@ -2701,7 +2702,7 @@
       <c r="F16" s="10"/>
       <c r="G16" s="8"/>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B17" s="9"/>
       <c r="C17" s="6"/>
       <c r="D17" s="7"/>
@@ -2709,7 +2710,7 @@
       <c r="F17" s="10"/>
       <c r="G17" s="8"/>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B18" s="9"/>
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
@@ -2717,7 +2718,7 @@
       <c r="F18" s="10"/>
       <c r="G18" s="8"/>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B19" s="9"/>
       <c r="C19" s="6"/>
       <c r="D19" s="7"/>
@@ -2725,7 +2726,7 @@
       <c r="F19" s="10"/>
       <c r="G19" s="8"/>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B20" s="9"/>
       <c r="C20" s="6"/>
       <c r="D20" s="7"/>
@@ -2733,7 +2734,7 @@
       <c r="F20" s="10"/>
       <c r="G20" s="8"/>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B21" s="9"/>
       <c r="C21" s="6"/>
       <c r="D21" s="7"/>
@@ -2741,7 +2742,7 @@
       <c r="F21" s="10"/>
       <c r="G21" s="8"/>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B22" s="9"/>
       <c r="C22" s="6"/>
       <c r="D22" s="7"/>
@@ -2749,7 +2750,7 @@
       <c r="F22" s="10"/>
       <c r="G22" s="8"/>
     </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B23" s="9"/>
       <c r="C23" s="6"/>
       <c r="D23" s="7"/>
@@ -2757,7 +2758,7 @@
       <c r="F23" s="10"/>
       <c r="G23" s="8"/>
     </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B24" s="9"/>
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
@@ -2765,7 +2766,7 @@
       <c r="F24" s="10"/>
       <c r="G24" s="8"/>
     </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B25" s="9"/>
       <c r="C25" s="6"/>
       <c r="D25" s="7"/>
@@ -2773,7 +2774,7 @@
       <c r="F25" s="10"/>
       <c r="G25" s="8"/>
     </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B26" s="9"/>
       <c r="C26" s="6"/>
       <c r="D26" s="7"/>
@@ -2781,7 +2782,7 @@
       <c r="F26" s="10"/>
       <c r="G26" s="8"/>
     </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B27" s="9"/>
       <c r="C27" s="6"/>
       <c r="D27" s="7"/>
@@ -2789,13 +2790,13 @@
       <c r="F27" s="10"/>
       <c r="G27" s="8"/>
     </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:7" x14ac:dyDescent="0.3">
       <c r="D28" s="7"/>
       <c r="E28" s="10"/>
       <c r="F28" s="10"/>
     </row>
   </sheetData>
-  <sortState ref="D13:D29">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="D13:D29">
     <sortCondition ref="D13"/>
   </sortState>
   <dataConsolidate/>

</xml_diff>

<commit_message>
Da finire CRUD pacchetti
- Finita la crea e la show
- Da finire la modifica
</commit_message>
<xml_diff>
--- a/Documentazioni/Codifica pagine sito.xlsx
+++ b/Documentazioni/Codifica pagine sito.xlsx
@@ -3,16 +3,16 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
   <workbookPr filterPrivacy="1" codeName="Questa_cartella_di_lavoro"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2802ED81-8AA9-4CB5-B2EE-AE2DAA403E97}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2797863-2BE0-4C65-92DB-0FA2C3B6DA08}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="1500" yWindow="1500" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
     <sheet name="Foglio utile" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Main!$A$1:$H$47</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Main!$A$1:$H$53</definedName>
     <definedName name="RefController_nome">Controller[Lista Controller]</definedName>
     <definedName name="RefTipo">Tipo[]</definedName>
   </definedNames>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="162">
   <si>
     <t>Nome gabbia logica</t>
   </si>
@@ -463,9 +463,6 @@
     <t>CourseController</t>
   </si>
   <si>
-    <t>disciplines-create</t>
-  </si>
-  <si>
     <t>DisciplineController</t>
   </si>
   <si>
@@ -475,27 +472,15 @@
     <t>Azione</t>
   </si>
   <si>
-    <t>disciplines-edit</t>
-  </si>
-  <si>
-    <t>disciplines-delete</t>
-  </si>
-  <si>
     <t>M312</t>
   </si>
   <si>
     <t>M313</t>
   </si>
   <si>
-    <t>discipline-store</t>
-  </si>
-  <si>
     <t>M314</t>
   </si>
   <si>
-    <t>disciplines-update</t>
-  </si>
-  <si>
     <t>M315</t>
   </si>
   <si>
@@ -514,19 +499,25 @@
     <t>M325</t>
   </si>
   <si>
-    <t>courses-create</t>
-  </si>
-  <si>
-    <t>courses-store</t>
-  </si>
-  <si>
-    <t>courses-edit</t>
-  </si>
-  <si>
-    <t>courses-update</t>
-  </si>
-  <si>
-    <t>courses-delete</t>
+    <t>PackageController</t>
+  </si>
+  <si>
+    <t>M331</t>
+  </si>
+  <si>
+    <t>M332</t>
+  </si>
+  <si>
+    <t>M333</t>
+  </si>
+  <si>
+    <t>M334</t>
+  </si>
+  <si>
+    <t>M335</t>
+  </si>
+  <si>
+    <t>M336</t>
   </si>
 </sst>
 </file>
@@ -956,14 +947,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{905F6574-56C3-4E36-86AD-16F4E970F9D2}" name="Tabella4" displayName="Tabella4" ref="A1:H47" dataDxfId="17">
-  <autoFilter ref="A1:H47" xr:uid="{34684D11-7ACD-45A4-AA96-0CE6C7239D98}">
-    <filterColumn colId="6">
-      <filters>
-        <filter val="CourseController"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{905F6574-56C3-4E36-86AD-16F4E970F9D2}" name="Tabella4" displayName="Tabella4" ref="A1:H53" dataDxfId="17">
+  <autoFilter ref="A1:H53" xr:uid="{34684D11-7ACD-45A4-AA96-0CE6C7239D98}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{E7D98D43-EB7B-46CE-B0B0-C555D83773A6}" name="Codice gabbia logica" dataDxfId="16" totalsRowDxfId="15"/>
     <tableColumn id="8" xr3:uid="{CAF26B0C-D3E2-4A71-A7C5-519E983C334C}" name="Rotta" dataDxfId="14" totalsRowDxfId="13">
@@ -1271,10 +1256,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Foglio2"/>
-  <dimension ref="A1:I47"/>
+  <dimension ref="A1:I53"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D55" sqref="D55"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D50" sqref="D50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" outlineLevelRow="2" x14ac:dyDescent="0.3"/>
@@ -1321,7 +1306,7 @@
       </c>
       <c r="I1" s="13"/>
     </row>
-    <row r="2" spans="1:9" ht="19.95" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
         <v>43</v>
       </c>
@@ -1339,7 +1324,7 @@
         <v>61</v>
       </c>
       <c r="F2" s="18" t="str">
-        <f t="shared" ref="F2:F47" si="0">IF($E2="Da definire",$E2,_xlfn.CONCAT($E2,".blade.php"))</f>
+        <f t="shared" ref="F2:F53" si="0">IF($E2="Da definire",$E2,_xlfn.CONCAT($E2,".blade.php"))</f>
         <v>welcome.blade.php</v>
       </c>
       <c r="G2" s="18" t="s">
@@ -1350,7 +1335,7 @@
       </c>
       <c r="I2" s="13"/>
     </row>
-    <row r="3" spans="1:9" ht="19.95" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="19.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A3" s="18"/>
       <c r="B3" s="18" t="str">
         <f>"/" &amp; E3</f>
@@ -1370,7 +1355,7 @@
       </c>
       <c r="I3" s="13"/>
     </row>
-    <row r="4" spans="1:9" ht="19.95" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="19.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
         <v>139</v>
       </c>
@@ -1397,7 +1382,7 @@
       </c>
       <c r="I4" s="13"/>
     </row>
-    <row r="5" spans="1:9" ht="19.95" hidden="1" customHeight="1" collapsed="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="18" t="s">
         <v>44</v>
       </c>
@@ -1426,7 +1411,7 @@
       </c>
       <c r="I5" s="13"/>
     </row>
-    <row r="6" spans="1:9" ht="19.95" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="18" t="s">
         <v>53</v>
       </c>
@@ -1455,7 +1440,7 @@
       </c>
       <c r="I6" s="13"/>
     </row>
-    <row r="7" spans="1:9" ht="19.95" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="18" t="s">
         <v>126</v>
       </c>
@@ -1484,7 +1469,7 @@
       </c>
       <c r="I7" s="12"/>
     </row>
-    <row r="8" spans="1:9" ht="19.95" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="18" t="s">
         <v>45</v>
       </c>
@@ -1513,7 +1498,7 @@
       </c>
       <c r="I8" s="12"/>
     </row>
-    <row r="9" spans="1:9" ht="19.95" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="18" t="s">
         <v>47</v>
       </c>
@@ -1542,7 +1527,7 @@
       </c>
       <c r="I9" s="12"/>
     </row>
-    <row r="10" spans="1:9" ht="19.95" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="18" t="s">
         <v>49</v>
       </c>
@@ -1571,7 +1556,7 @@
       </c>
       <c r="I10" s="13"/>
     </row>
-    <row r="11" spans="1:9" ht="19.95" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="18" t="s">
         <v>51</v>
       </c>
@@ -1600,7 +1585,7 @@
       </c>
       <c r="I11" s="13"/>
     </row>
-    <row r="12" spans="1:9" ht="19.95" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="18" t="s">
         <v>54</v>
       </c>
@@ -1629,7 +1614,7 @@
       </c>
       <c r="I12" s="13"/>
     </row>
-    <row r="13" spans="1:9" ht="19.95" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="18" t="s">
         <v>57</v>
       </c>
@@ -1658,7 +1643,7 @@
       </c>
       <c r="I13" s="13"/>
     </row>
-    <row r="14" spans="1:9" ht="19.95" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="18" t="s">
         <v>58</v>
       </c>
@@ -1687,7 +1672,7 @@
       </c>
       <c r="I14" s="13"/>
     </row>
-    <row r="15" spans="1:9" ht="19.95" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="28" t="s">
         <v>42</v>
       </c>
@@ -1716,7 +1701,7 @@
       </c>
       <c r="I15" s="13"/>
     </row>
-    <row r="16" spans="1:9" ht="19.95" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="26"/>
       <c r="B16" s="26" t="str">
         <f t="shared" si="1"/>
@@ -1743,7 +1728,7 @@
       </c>
       <c r="I16" s="13"/>
     </row>
-    <row r="17" spans="1:9" ht="19.95" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" ht="19.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A17" s="27" t="s">
         <v>18</v>
       </c>
@@ -1772,7 +1757,7 @@
       </c>
       <c r="I17" s="13"/>
     </row>
-    <row r="18" spans="1:9" ht="19.95" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" ht="19.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A18" s="25" t="s">
         <v>19</v>
       </c>
@@ -1799,7 +1784,7 @@
       <c r="H18" s="22"/>
       <c r="I18" s="13"/>
     </row>
-    <row r="19" spans="1:9" ht="19.95" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" ht="19.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A19" s="25" t="s">
         <v>20</v>
       </c>
@@ -1826,7 +1811,7 @@
       <c r="H19" s="22"/>
       <c r="I19" s="13"/>
     </row>
-    <row r="20" spans="1:9" ht="19.95" hidden="1" customHeight="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" ht="19.95" customHeight="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.3">
       <c r="A20" s="25" t="s">
         <v>21</v>
       </c>
@@ -1853,7 +1838,7 @@
       <c r="H20" s="22"/>
       <c r="I20" s="13"/>
     </row>
-    <row r="21" spans="1:9" ht="19.95" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" ht="19.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A21" s="25" t="s">
         <v>22</v>
       </c>
@@ -1880,7 +1865,7 @@
       <c r="H21" s="22"/>
       <c r="I21" s="13"/>
     </row>
-    <row r="22" spans="1:9" ht="19.95" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" ht="19.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A22" s="27" t="s">
         <v>23</v>
       </c>
@@ -1909,7 +1894,7 @@
       </c>
       <c r="I22" s="13"/>
     </row>
-    <row r="23" spans="1:9" ht="19.95" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" ht="19.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A23" s="25" t="s">
         <v>24</v>
       </c>
@@ -1936,7 +1921,7 @@
       <c r="H23" s="22"/>
       <c r="I23" s="13"/>
     </row>
-    <row r="24" spans="1:9" ht="19.95" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" ht="19.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A24" s="25" t="s">
         <v>25</v>
       </c>
@@ -1963,7 +1948,7 @@
       <c r="H24" s="22"/>
       <c r="I24" s="13"/>
     </row>
-    <row r="25" spans="1:9" ht="19.95" hidden="1" customHeight="1" collapsed="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="26"/>
       <c r="B25" s="26" t="str">
         <f>"/" &amp; E25</f>
@@ -1990,7 +1975,7 @@
       </c>
       <c r="I25" s="13"/>
     </row>
-    <row r="26" spans="1:9" ht="19.95" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" ht="19.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A26" s="27" t="s">
         <v>26</v>
       </c>
@@ -2019,7 +2004,7 @@
       </c>
       <c r="I26" s="13"/>
     </row>
-    <row r="27" spans="1:9" ht="19.95" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" ht="19.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A27" s="25" t="s">
         <v>35</v>
       </c>
@@ -2046,7 +2031,7 @@
       <c r="H27" s="22"/>
       <c r="I27" s="13"/>
     </row>
-    <row r="28" spans="1:9" ht="19.95" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" ht="19.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A28" s="25" t="s">
         <v>128</v>
       </c>
@@ -2073,7 +2058,7 @@
       <c r="H28" s="22"/>
       <c r="I28" s="13"/>
     </row>
-    <row r="29" spans="1:9" ht="19.95" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" ht="19.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A29" s="25" t="s">
         <v>129</v>
       </c>
@@ -2100,7 +2085,7 @@
       <c r="H29" s="22"/>
       <c r="I29" s="13"/>
     </row>
-    <row r="30" spans="1:9" ht="19.95" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" ht="19.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A30" s="27" t="s">
         <v>36</v>
       </c>
@@ -2127,7 +2112,7 @@
       <c r="H30" s="21"/>
       <c r="I30" s="13"/>
     </row>
-    <row r="31" spans="1:9" ht="19.95" hidden="1" customHeight="1" collapsed="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="26"/>
       <c r="B31" s="26" t="str">
         <f>"/" &amp; E31</f>
@@ -2154,7 +2139,7 @@
       </c>
       <c r="I31" s="13"/>
     </row>
-    <row r="32" spans="1:9" ht="19.95" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" ht="19.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A32" s="25" t="s">
         <v>37</v>
       </c>
@@ -2176,86 +2161,89 @@
         <v>disciplines.blade.php</v>
       </c>
       <c r="G32" s="25" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H32" s="22"/>
       <c r="I32" s="13"/>
     </row>
     <row r="33" spans="1:9" ht="19.95" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A33" s="25" t="s">
+        <v>144</v>
+      </c>
+      <c r="B33" s="25" t="str">
+        <f t="shared" ref="B33:B52" si="2">$B$31 &amp; "/" &amp; E33</f>
+        <v>/mng_activity/disciplines-create</v>
+      </c>
+      <c r="C33" s="25" t="s">
         <v>145</v>
       </c>
-      <c r="B33" s="25" t="str">
-        <f t="shared" ref="B33:B46" si="2">$B$31 &amp; "/" &amp; E33</f>
-        <v>/mng_activity/disciplines-create</v>
-      </c>
-      <c r="C33" s="25" t="s">
-        <v>146</v>
-      </c>
       <c r="D33" s="22"/>
-      <c r="E33" s="25" t="s">
-        <v>143</v>
+      <c r="E33" s="25" t="str">
+        <f>$E32 &amp; "-create"</f>
+        <v>disciplines-create</v>
       </c>
       <c r="F33" s="25" t="str">
         <f>IF($E33="Da definire",$E33,_xlfn.CONCAT($E33,".blade.php"))</f>
         <v>disciplines-create.blade.php</v>
       </c>
       <c r="G33" s="25" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H33" s="22"/>
       <c r="I33" s="13"/>
     </row>
     <row r="34" spans="1:9" ht="19.95" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A34" s="25" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B34" s="25" t="str">
         <f t="shared" si="2"/>
-        <v>/mng_activity/discipline-store</v>
+        <v>/mng_activity/disciplines-store</v>
       </c>
       <c r="C34" s="25" t="s">
         <v>76</v>
       </c>
       <c r="D34" s="22"/>
-      <c r="E34" s="25" t="s">
-        <v>151</v>
+      <c r="E34" s="25" t="str">
+        <f>$E32 &amp; "-store"</f>
+        <v>disciplines-store</v>
       </c>
       <c r="F34" s="25"/>
       <c r="G34" s="25" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H34" s="22"/>
       <c r="I34" s="13"/>
     </row>
     <row r="35" spans="1:9" ht="19.95" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A35" s="25" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B35" s="25" t="str">
         <f t="shared" si="2"/>
         <v>/mng_activity/disciplines-edit</v>
       </c>
       <c r="C35" s="25" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D35" s="22"/>
-      <c r="E35" s="25" t="s">
-        <v>147</v>
+      <c r="E35" s="25" t="str">
+        <f>$E32 &amp; "-edit"</f>
+        <v>disciplines-edit</v>
       </c>
       <c r="F35" s="25" t="str">
         <f>IF($E35="Da definire",$E35,_xlfn.CONCAT($E35,".blade.php"))</f>
         <v>disciplines-edit.blade.php</v>
       </c>
       <c r="G35" s="25" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H35" s="22"/>
       <c r="I35" s="13"/>
     </row>
     <row r="36" spans="1:9" ht="19.95" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A36" s="25" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="B36" s="25" t="str">
         <f t="shared" si="2"/>
@@ -2265,37 +2253,39 @@
         <v>76</v>
       </c>
       <c r="D36" s="22"/>
-      <c r="E36" s="25" t="s">
-        <v>153</v>
+      <c r="E36" s="25" t="str">
+        <f>$E32 &amp; "-update"</f>
+        <v>disciplines-update</v>
       </c>
       <c r="F36" s="25"/>
       <c r="G36" s="25" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H36" s="22"/>
       <c r="I36" s="13"/>
     </row>
     <row r="37" spans="1:9" ht="19.95" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A37" s="25" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="B37" s="25" t="str">
         <f>$B$31 &amp; "/" &amp; E37</f>
         <v>/mng_activity/disciplines-delete</v>
       </c>
       <c r="C37" s="25" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D37" s="22"/>
-      <c r="E37" s="25" t="s">
-        <v>148</v>
+      <c r="E37" s="25" t="str">
+        <f>$E32 &amp; "-delete"</f>
+        <v>disciplines-delete</v>
       </c>
       <c r="F37" s="25" t="str">
         <f>IF($E37="Da definire",$E37,_xlfn.CONCAT($E37,".blade.php"))</f>
         <v>disciplines-delete.blade.php</v>
       </c>
       <c r="G37" s="25" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H37" s="22"/>
       <c r="I37" s="13"/>
@@ -2327,20 +2317,21 @@
       <c r="H38" s="22"/>
       <c r="I38" s="13"/>
     </row>
-    <row r="39" spans="1:9" ht="19.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" ht="19.95" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A39" s="25" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="B39" s="25" t="str">
         <f t="shared" ref="B39:B42" si="3">$B$31 &amp; "/" &amp; E39</f>
         <v>/mng_activity/courses-create</v>
       </c>
       <c r="C39" s="25" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D39" s="22"/>
-      <c r="E39" s="25" t="s">
-        <v>160</v>
+      <c r="E39" s="25" t="str">
+        <f>$E38 &amp; "-create"</f>
+        <v>courses-create</v>
       </c>
       <c r="F39" s="25" t="str">
         <f>IF($E39="Da definire",$E39,_xlfn.CONCAT($E39,".blade.php"))</f>
@@ -2352,9 +2343,9 @@
       <c r="H39" s="22"/>
       <c r="I39" s="13"/>
     </row>
-    <row r="40" spans="1:9" ht="19.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" ht="19.95" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A40" s="25" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="B40" s="25" t="str">
         <f t="shared" si="3"/>
@@ -2364,8 +2355,9 @@
         <v>76</v>
       </c>
       <c r="D40" s="22"/>
-      <c r="E40" s="25" t="s">
-        <v>161</v>
+      <c r="E40" s="25" t="str">
+        <f>$E38 &amp; "-store"</f>
+        <v>courses-store</v>
       </c>
       <c r="F40" s="25"/>
       <c r="G40" s="25" t="s">
@@ -2374,20 +2366,21 @@
       <c r="H40" s="22"/>
       <c r="I40" s="13"/>
     </row>
-    <row r="41" spans="1:9" ht="19.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" ht="19.95" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A41" s="25" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="B41" s="25" t="str">
         <f t="shared" si="3"/>
         <v>/mng_activity/courses-edit</v>
       </c>
       <c r="C41" s="25" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D41" s="22"/>
-      <c r="E41" s="25" t="s">
-        <v>162</v>
+      <c r="E41" s="25" t="str">
+        <f>$E38 &amp; "-edit"</f>
+        <v>courses-edit</v>
       </c>
       <c r="F41" s="25" t="str">
         <f>IF($E41="Da definire",$E41,_xlfn.CONCAT($E41,".blade.php"))</f>
@@ -2399,9 +2392,9 @@
       <c r="H41" s="22"/>
       <c r="I41" s="13"/>
     </row>
-    <row r="42" spans="1:9" ht="19.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" ht="19.95" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A42" s="25" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="B42" s="25" t="str">
         <f t="shared" si="3"/>
@@ -2411,8 +2404,9 @@
         <v>76</v>
       </c>
       <c r="D42" s="22"/>
-      <c r="E42" s="25" t="s">
-        <v>163</v>
+      <c r="E42" s="25" t="str">
+        <f>$E38 &amp; "-update"</f>
+        <v>courses-update</v>
       </c>
       <c r="F42" s="25"/>
       <c r="G42" s="25" t="s">
@@ -2421,20 +2415,21 @@
       <c r="H42" s="22"/>
       <c r="I42" s="13"/>
     </row>
-    <row r="43" spans="1:9" ht="19.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" ht="19.95" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A43" s="25" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="B43" s="25" t="str">
         <f>$B$31 &amp; "/" &amp; E43</f>
         <v>/mng_activity/courses-delete</v>
       </c>
       <c r="C43" s="25" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D43" s="22"/>
-      <c r="E43" s="25" t="s">
-        <v>164</v>
+      <c r="E43" s="25" t="str">
+        <f>$E38 &amp; "-delete"</f>
+        <v>courses-delete</v>
       </c>
       <c r="F43" s="25" t="str">
         <f>IF($E43="Da definire",$E43,_xlfn.CONCAT($E43,".blade.php"))</f>
@@ -2446,7 +2441,7 @@
       <c r="H43" s="22"/>
       <c r="I43" s="13"/>
     </row>
-    <row r="44" spans="1:9" ht="19.95" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" ht="19.95" customHeight="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.3">
       <c r="A44" s="25" t="s">
         <v>40</v>
       </c>
@@ -2457,7 +2452,7 @@
       <c r="C44" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="D44" s="22" t="s">
+      <c r="D44" s="25" t="s">
         <v>29</v>
       </c>
       <c r="E44" s="25" t="s">
@@ -2468,99 +2463,249 @@
         <v>packages.blade.php</v>
       </c>
       <c r="G44" s="25" t="s">
-        <v>120</v>
+        <v>155</v>
       </c>
       <c r="H44" s="22"/>
       <c r="I44" s="13"/>
     </row>
-    <row r="45" spans="1:9" ht="19.95" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" ht="19.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A45" s="25" t="s">
+        <v>156</v>
+      </c>
+      <c r="B45" s="25" t="str">
+        <f t="shared" ref="B45:B48" si="4">$B$31 &amp; "/" &amp; E45</f>
+        <v>/mng_activity/packages-create</v>
+      </c>
+      <c r="C45" s="25" t="s">
+        <v>145</v>
+      </c>
+      <c r="D45" s="22"/>
+      <c r="E45" s="25" t="str">
+        <f>$E44 &amp; "-create"</f>
+        <v>packages-create</v>
+      </c>
+      <c r="F45" s="25" t="str">
+        <f>IF($E45="Da definire",$E45,_xlfn.CONCAT($E45,".blade.php"))</f>
+        <v>packages-create.blade.php</v>
+      </c>
+      <c r="G45" s="25" t="s">
+        <v>155</v>
+      </c>
+      <c r="H45" s="22"/>
+      <c r="I45" s="13"/>
+    </row>
+    <row r="46" spans="1:9" ht="19.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
+      <c r="A46" s="25" t="s">
+        <v>157</v>
+      </c>
+      <c r="B46" s="25" t="str">
+        <f t="shared" si="4"/>
+        <v>/mng_activity/packages-store</v>
+      </c>
+      <c r="C46" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="D46" s="22"/>
+      <c r="E46" s="25" t="str">
+        <f>$E44 &amp; "-store"</f>
+        <v>packages-store</v>
+      </c>
+      <c r="F46" s="25"/>
+      <c r="G46" s="25" t="s">
+        <v>155</v>
+      </c>
+      <c r="H46" s="22"/>
+      <c r="I46" s="13"/>
+    </row>
+    <row r="47" spans="1:9" ht="19.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
+      <c r="A47" s="25" t="s">
+        <v>158</v>
+      </c>
+      <c r="B47" s="25" t="str">
+        <f t="shared" si="4"/>
+        <v>/mng_activity/packages-edit</v>
+      </c>
+      <c r="C47" s="25" t="s">
+        <v>145</v>
+      </c>
+      <c r="D47" s="22"/>
+      <c r="E47" s="25" t="str">
+        <f>$E44 &amp; "-edit"</f>
+        <v>packages-edit</v>
+      </c>
+      <c r="F47" s="25" t="str">
+        <f>IF($E47="Da definire",$E47,_xlfn.CONCAT($E47,".blade.php"))</f>
+        <v>packages-edit.blade.php</v>
+      </c>
+      <c r="G47" s="25" t="s">
+        <v>155</v>
+      </c>
+      <c r="H47" s="22"/>
+      <c r="I47" s="13"/>
+    </row>
+    <row r="48" spans="1:9" ht="19.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
+      <c r="A48" s="25" t="s">
+        <v>159</v>
+      </c>
+      <c r="B48" s="25" t="str">
+        <f t="shared" si="4"/>
+        <v>/mng_activity/packages-update</v>
+      </c>
+      <c r="C48" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="D48" s="22"/>
+      <c r="E48" s="25" t="str">
+        <f>$E44 &amp; "-update"</f>
+        <v>packages-update</v>
+      </c>
+      <c r="F48" s="25"/>
+      <c r="G48" s="25" t="s">
+        <v>155</v>
+      </c>
+      <c r="H48" s="22"/>
+      <c r="I48" s="13"/>
+    </row>
+    <row r="49" spans="1:9" ht="19.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
+      <c r="A49" s="25" t="s">
+        <v>160</v>
+      </c>
+      <c r="B49" s="25" t="str">
+        <f>$B$31 &amp; "/" &amp; E49</f>
+        <v>/mng_activity/packages-delete</v>
+      </c>
+      <c r="C49" s="25" t="s">
+        <v>145</v>
+      </c>
+      <c r="D49" s="22"/>
+      <c r="E49" s="25" t="str">
+        <f>$E44 &amp; "-delete"</f>
+        <v>packages-delete</v>
+      </c>
+      <c r="F49" s="25" t="str">
+        <f>IF($E49="Da definire",$E49,_xlfn.CONCAT($E49,".blade.php"))</f>
+        <v>packages-delete.blade.php</v>
+      </c>
+      <c r="G49" s="25" t="s">
+        <v>155</v>
+      </c>
+      <c r="H49" s="22"/>
+      <c r="I49" s="13"/>
+    </row>
+    <row r="50" spans="1:9" ht="19.8" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
+      <c r="A50" s="25" t="s">
+        <v>161</v>
+      </c>
+      <c r="B50" s="25" t="str">
+        <f>$B$31 &amp; "/" &amp; E50</f>
+        <v>/mng_activity/packages-show</v>
+      </c>
+      <c r="C50" s="25" t="s">
+        <v>145</v>
+      </c>
+      <c r="D50" s="22"/>
+      <c r="E50" s="25" t="str">
+        <f>$E44 &amp; "-show"</f>
+        <v>packages-show</v>
+      </c>
+      <c r="F50" s="25" t="str">
+        <f>IF($E50="Da definire",$E50,_xlfn.CONCAT($E50,".blade.php"))</f>
+        <v>packages-show.blade.php</v>
+      </c>
+      <c r="G50" s="25" t="s">
+        <v>155</v>
+      </c>
+      <c r="H50" s="22"/>
+      <c r="I50" s="13"/>
+    </row>
+    <row r="51" spans="1:9" ht="19.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="B45" s="25" t="str">
+      <c r="B51" s="25" t="str">
         <f t="shared" si="2"/>
         <v>/mng_activity/rooms</v>
       </c>
-      <c r="C45" s="25" t="s">
+      <c r="C51" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="D45" s="22" t="s">
+      <c r="D51" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="E45" s="25" t="s">
+      <c r="E51" s="25" t="s">
         <v>114</v>
       </c>
-      <c r="F45" s="25" t="str">
+      <c r="F51" s="25" t="str">
         <f t="shared" si="0"/>
         <v>rooms.blade.php</v>
       </c>
-      <c r="G45" s="25" t="s">
+      <c r="G51" s="25" t="s">
         <v>120</v>
       </c>
-      <c r="H45" s="22"/>
-      <c r="I45" s="13"/>
-    </row>
-    <row r="46" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="25" t="s">
+      <c r="H51" s="22"/>
+      <c r="I51" s="13"/>
+    </row>
+    <row r="52" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="B46" s="25" t="str">
+      <c r="B52" s="25" t="str">
         <f t="shared" si="2"/>
         <v>/mng_activity/scheduling</v>
       </c>
-      <c r="C46" s="25" t="s">
+      <c r="C52" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="D46" s="22" t="s">
+      <c r="D52" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="E46" s="25" t="s">
+      <c r="E52" s="25" t="s">
         <v>116</v>
       </c>
-      <c r="F46" s="25" t="str">
+      <c r="F52" s="25" t="str">
         <f t="shared" si="0"/>
         <v>scheduling.blade.php</v>
       </c>
-      <c r="G46" s="25" t="s">
+      <c r="G52" s="25" t="s">
         <v>120</v>
       </c>
-      <c r="H46" s="22"/>
-      <c r="I46" s="13"/>
-    </row>
-    <row r="47" spans="1:9" ht="21" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="26"/>
-      <c r="B47" s="26" t="str">
-        <f>"/" &amp; E47</f>
+      <c r="H52" s="22"/>
+      <c r="I52" s="13"/>
+    </row>
+    <row r="53" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="26"/>
+      <c r="B53" s="26" t="str">
+        <f>"/" &amp; E53</f>
         <v>/report_stats</v>
       </c>
-      <c r="C47" s="26" t="s">
+      <c r="C53" s="26" t="s">
         <v>63</v>
       </c>
-      <c r="D47" s="23" t="s">
+      <c r="D53" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="E47" s="26" t="s">
+      <c r="E53" s="26" t="s">
         <v>97</v>
       </c>
-      <c r="F47" s="26" t="str">
+      <c r="F53" s="26" t="str">
         <f t="shared" si="0"/>
         <v>report_stats.blade.php</v>
       </c>
-      <c r="G47" s="26" t="s">
+      <c r="G53" s="26" t="s">
         <v>95</v>
       </c>
-      <c r="H47" s="23" t="s">
+      <c r="H53" s="23" t="s">
         <v>98</v>
       </c>
-      <c r="I47" s="13"/>
+      <c r="I53" s="13"/>
     </row>
   </sheetData>
   <dataConsolidate/>
   <dataValidations count="2">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C47" xr:uid="{F340BA2D-9D43-4A9F-86F9-B281B429D2E7}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C53" xr:uid="{F340BA2D-9D43-4A9F-86F9-B281B429D2E7}">
       <formula1>RefTipo</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G47" xr:uid="{DFF187B0-2821-4C72-B394-0420A8E90996}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G53" xr:uid="{DFF187B0-2821-4C72-B394-0420A8E90996}">
       <formula1>RefController_nome</formula1>
     </dataValidation>
   </dataValidations>
@@ -2580,7 +2725,7 @@
   <dimension ref="B1:G28"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2618,7 +2763,7 @@
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B3" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>131</v>
@@ -2681,7 +2826,12 @@
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.3">
       <c r="D11" t="s">
-        <v>144</v>
+        <v>143</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="D12" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Aggiunto la rotta show a discipline
</commit_message>
<xml_diff>
--- a/Documentazioni/Codifica pagine sito.xlsx
+++ b/Documentazioni/Codifica pagine sito.xlsx
@@ -1,18 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr filterPrivacy="1" codeName="Questa_cartella_di_lavoro"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2797863-2BE0-4C65-92DB-0FA2C3B6DA08}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D106A1C-CF76-4E72-A4AD-0240D5AB1303}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="1500" yWindow="1500" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1500" yWindow="1500" windowWidth="17280" windowHeight="8970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
     <sheet name="Foglio utile" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Main!$A$1:$H$53</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Main!$A$1:$H$61</definedName>
     <definedName name="RefController_nome">Controller[Lista Controller]</definedName>
     <definedName name="RefTipo">Tipo[]</definedName>
   </definedNames>
@@ -24,7 +24,6 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -32,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="171">
   <si>
     <t>Nome gabbia logica</t>
   </si>
@@ -518,6 +517,33 @@
   </si>
   <si>
     <t>M336</t>
+  </si>
+  <si>
+    <t>M341</t>
+  </si>
+  <si>
+    <t>M342</t>
+  </si>
+  <si>
+    <t>M343</t>
+  </si>
+  <si>
+    <t>M344</t>
+  </si>
+  <si>
+    <t>M345</t>
+  </si>
+  <si>
+    <t>M346</t>
+  </si>
+  <si>
+    <t>RoomController</t>
+  </si>
+  <si>
+    <t>M316</t>
+  </si>
+  <si>
+    <t>M326</t>
   </si>
 </sst>
 </file>
@@ -947,8 +973,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{905F6574-56C3-4E36-86AD-16F4E970F9D2}" name="Tabella4" displayName="Tabella4" ref="A1:H53" dataDxfId="17">
-  <autoFilter ref="A1:H53" xr:uid="{34684D11-7ACD-45A4-AA96-0CE6C7239D98}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{905F6574-56C3-4E36-86AD-16F4E970F9D2}" name="Tabella4" displayName="Tabella4" ref="A1:H61" dataDxfId="17">
+  <autoFilter ref="A1:H61" xr:uid="{34684D11-7ACD-45A4-AA96-0CE6C7239D98}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{E7D98D43-EB7B-46CE-B0B0-C555D83773A6}" name="Codice gabbia logica" dataDxfId="16" totalsRowDxfId="15"/>
     <tableColumn id="8" xr3:uid="{CAF26B0C-D3E2-4A71-A7C5-519E983C334C}" name="Rotta" dataDxfId="14" totalsRowDxfId="13">
@@ -970,7 +996,7 @@
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{45120F09-8607-4F6A-A989-7184307236A1}" name="Tipo" displayName="Tipo" ref="B1:B9" totalsRowShown="0" headerRowDxfId="2" tableBorderDxfId="1">
   <autoFilter ref="B1:B9" xr:uid="{B0803B6A-3448-4A89-AC43-1127F3DBD833}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:B8">
+  <sortState ref="B2:B8">
     <sortCondition ref="B1:B8"/>
   </sortState>
   <tableColumns count="1">
@@ -1256,30 +1282,30 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Foglio2"/>
-  <dimension ref="A1:I53"/>
+  <dimension ref="A1:I61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D50" sqref="D50"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G45" sqref="G45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" outlineLevelRow="2" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" outlineLevelRow="2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.5546875" style="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.5703125" style="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.140625" style="13" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13" style="12" customWidth="1"/>
-    <col min="4" max="4" width="35.5546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.33203125" style="15" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.44140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="88.44140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="89.6640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="28.6640625" style="13" customWidth="1"/>
-    <col min="11" max="12" width="8.88671875" style="13"/>
+    <col min="4" max="4" width="35.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.42578125" style="15" customWidth="1"/>
+    <col min="6" max="6" width="24.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="88.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="89.7109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="28.7109375" style="13" customWidth="1"/>
+    <col min="11" max="12" width="8.85546875" style="13"/>
     <col min="13" max="13" width="19" style="13" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="8.88671875" style="13"/>
+    <col min="14" max="16384" width="8.85546875" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>1</v>
       </c>
@@ -1306,7 +1332,7 @@
       </c>
       <c r="I1" s="13"/>
     </row>
-    <row r="2" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>43</v>
       </c>
@@ -1324,7 +1350,7 @@
         <v>61</v>
       </c>
       <c r="F2" s="18" t="str">
-        <f t="shared" ref="F2:F53" si="0">IF($E2="Da definire",$E2,_xlfn.CONCAT($E2,".blade.php"))</f>
+        <f t="shared" ref="F2:F61" si="0">IF($E2="Da definire",$E2,_xlfn.CONCAT($E2,".blade.php"))</f>
         <v>welcome.blade.php</v>
       </c>
       <c r="G2" s="18" t="s">
@@ -1335,7 +1361,7 @@
       </c>
       <c r="I2" s="13"/>
     </row>
-    <row r="3" spans="1:9" ht="19.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="19.899999999999999" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A3" s="18"/>
       <c r="B3" s="18" t="str">
         <f>"/" &amp; E3</f>
@@ -1355,7 +1381,7 @@
       </c>
       <c r="I3" s="13"/>
     </row>
-    <row r="4" spans="1:9" ht="19.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="19.899999999999999" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
         <v>139</v>
       </c>
@@ -1382,7 +1408,7 @@
       </c>
       <c r="I4" s="13"/>
     </row>
-    <row r="5" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
         <v>44</v>
       </c>
@@ -1411,7 +1437,7 @@
       </c>
       <c r="I5" s="13"/>
     </row>
-    <row r="6" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
         <v>53</v>
       </c>
@@ -1440,7 +1466,7 @@
       </c>
       <c r="I6" s="13"/>
     </row>
-    <row r="7" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
         <v>126</v>
       </c>
@@ -1469,7 +1495,7 @@
       </c>
       <c r="I7" s="12"/>
     </row>
-    <row r="8" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
         <v>45</v>
       </c>
@@ -1498,7 +1524,7 @@
       </c>
       <c r="I8" s="12"/>
     </row>
-    <row r="9" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
         <v>47</v>
       </c>
@@ -1527,7 +1553,7 @@
       </c>
       <c r="I9" s="12"/>
     </row>
-    <row r="10" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
         <v>49</v>
       </c>
@@ -1556,7 +1582,7 @@
       </c>
       <c r="I10" s="13"/>
     </row>
-    <row r="11" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="18" t="s">
         <v>51</v>
       </c>
@@ -1585,7 +1611,7 @@
       </c>
       <c r="I11" s="13"/>
     </row>
-    <row r="12" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
         <v>54</v>
       </c>
@@ -1614,7 +1640,7 @@
       </c>
       <c r="I12" s="13"/>
     </row>
-    <row r="13" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
         <v>57</v>
       </c>
@@ -1643,7 +1669,7 @@
       </c>
       <c r="I13" s="13"/>
     </row>
-    <row r="14" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="18" t="s">
         <v>58</v>
       </c>
@@ -1672,7 +1698,7 @@
       </c>
       <c r="I14" s="13"/>
     </row>
-    <row r="15" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="28" t="s">
         <v>42</v>
       </c>
@@ -1701,7 +1727,7 @@
       </c>
       <c r="I15" s="13"/>
     </row>
-    <row r="16" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="26"/>
       <c r="B16" s="26" t="str">
         <f t="shared" si="1"/>
@@ -1728,7 +1754,7 @@
       </c>
       <c r="I16" s="13"/>
     </row>
-    <row r="17" spans="1:9" ht="19.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" ht="19.899999999999999" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A17" s="27" t="s">
         <v>18</v>
       </c>
@@ -1757,7 +1783,7 @@
       </c>
       <c r="I17" s="13"/>
     </row>
-    <row r="18" spans="1:9" ht="19.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" ht="19.899999999999999" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A18" s="25" t="s">
         <v>19</v>
       </c>
@@ -1784,7 +1810,7 @@
       <c r="H18" s="22"/>
       <c r="I18" s="13"/>
     </row>
-    <row r="19" spans="1:9" ht="19.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" ht="19.899999999999999" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A19" s="25" t="s">
         <v>20</v>
       </c>
@@ -1811,7 +1837,7 @@
       <c r="H19" s="22"/>
       <c r="I19" s="13"/>
     </row>
-    <row r="20" spans="1:9" ht="19.95" customHeight="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" ht="19.899999999999999" customHeight="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A20" s="25" t="s">
         <v>21</v>
       </c>
@@ -1838,7 +1864,7 @@
       <c r="H20" s="22"/>
       <c r="I20" s="13"/>
     </row>
-    <row r="21" spans="1:9" ht="19.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" ht="19.899999999999999" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A21" s="25" t="s">
         <v>22</v>
       </c>
@@ -1865,7 +1891,7 @@
       <c r="H21" s="22"/>
       <c r="I21" s="13"/>
     </row>
-    <row r="22" spans="1:9" ht="19.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" ht="19.899999999999999" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A22" s="27" t="s">
         <v>23</v>
       </c>
@@ -1894,7 +1920,7 @@
       </c>
       <c r="I22" s="13"/>
     </row>
-    <row r="23" spans="1:9" ht="19.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" ht="19.899999999999999" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A23" s="25" t="s">
         <v>24</v>
       </c>
@@ -1921,7 +1947,7 @@
       <c r="H23" s="22"/>
       <c r="I23" s="13"/>
     </row>
-    <row r="24" spans="1:9" ht="19.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" ht="19.899999999999999" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A24" s="25" t="s">
         <v>25</v>
       </c>
@@ -1948,7 +1974,7 @@
       <c r="H24" s="22"/>
       <c r="I24" s="13"/>
     </row>
-    <row r="25" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="26"/>
       <c r="B25" s="26" t="str">
         <f>"/" &amp; E25</f>
@@ -1975,7 +2001,7 @@
       </c>
       <c r="I25" s="13"/>
     </row>
-    <row r="26" spans="1:9" ht="19.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" ht="19.899999999999999" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A26" s="27" t="s">
         <v>26</v>
       </c>
@@ -2004,7 +2030,7 @@
       </c>
       <c r="I26" s="13"/>
     </row>
-    <row r="27" spans="1:9" ht="19.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" ht="19.899999999999999" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A27" s="25" t="s">
         <v>35</v>
       </c>
@@ -2031,7 +2057,7 @@
       <c r="H27" s="22"/>
       <c r="I27" s="13"/>
     </row>
-    <row r="28" spans="1:9" ht="19.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" ht="19.899999999999999" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A28" s="25" t="s">
         <v>128</v>
       </c>
@@ -2058,7 +2084,7 @@
       <c r="H28" s="22"/>
       <c r="I28" s="13"/>
     </row>
-    <row r="29" spans="1:9" ht="19.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" ht="19.899999999999999" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A29" s="25" t="s">
         <v>129</v>
       </c>
@@ -2085,7 +2111,7 @@
       <c r="H29" s="22"/>
       <c r="I29" s="13"/>
     </row>
-    <row r="30" spans="1:9" ht="19.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" ht="19.899999999999999" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A30" s="27" t="s">
         <v>36</v>
       </c>
@@ -2112,7 +2138,7 @@
       <c r="H30" s="21"/>
       <c r="I30" s="13"/>
     </row>
-    <row r="31" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="26"/>
       <c r="B31" s="26" t="str">
         <f>"/" &amp; E31</f>
@@ -2139,7 +2165,7 @@
       </c>
       <c r="I31" s="13"/>
     </row>
-    <row r="32" spans="1:9" ht="19.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" ht="19.899999999999999" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A32" s="25" t="s">
         <v>37</v>
       </c>
@@ -2166,12 +2192,12 @@
       <c r="H32" s="22"/>
       <c r="I32" s="13"/>
     </row>
-    <row r="33" spans="1:9" ht="19.95" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" ht="19.899999999999999" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A33" s="25" t="s">
         <v>144</v>
       </c>
       <c r="B33" s="25" t="str">
-        <f t="shared" ref="B33:B52" si="2">$B$31 &amp; "/" &amp; E33</f>
+        <f t="shared" ref="B33:B60" si="2">$B$31 &amp; "/" &amp; E33</f>
         <v>/mng_activity/disciplines-create</v>
       </c>
       <c r="C33" s="25" t="s">
@@ -2192,7 +2218,7 @@
       <c r="H33" s="22"/>
       <c r="I33" s="13"/>
     </row>
-    <row r="34" spans="1:9" ht="19.95" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" ht="19.899999999999999" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A34" s="25" t="s">
         <v>146</v>
       </c>
@@ -2215,7 +2241,7 @@
       <c r="H34" s="22"/>
       <c r="I34" s="13"/>
     </row>
-    <row r="35" spans="1:9" ht="19.95" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" ht="19.899999999999999" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A35" s="25" t="s">
         <v>147</v>
       </c>
@@ -2241,7 +2267,7 @@
       <c r="H35" s="22"/>
       <c r="I35" s="13"/>
     </row>
-    <row r="36" spans="1:9" ht="19.95" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" ht="19.899999999999999" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A36" s="25" t="s">
         <v>148</v>
       </c>
@@ -2264,7 +2290,7 @@
       <c r="H36" s="22"/>
       <c r="I36" s="13"/>
     </row>
-    <row r="37" spans="1:9" ht="19.95" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" ht="19.899999999999999" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A37" s="25" t="s">
         <v>149</v>
       </c>
@@ -2290,274 +2316,277 @@
       <c r="H37" s="22"/>
       <c r="I37" s="13"/>
     </row>
-    <row r="38" spans="1:9" ht="19.95" customHeight="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" ht="19.899999999999999" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A38" s="25" t="s">
+        <v>169</v>
+      </c>
+      <c r="B38" s="25" t="str">
+        <f>$B$31 &amp; "/" &amp; E38</f>
+        <v>/mng_activity/disciplines-show</v>
+      </c>
+      <c r="C38" s="25" t="s">
+        <v>145</v>
+      </c>
+      <c r="D38" s="22"/>
+      <c r="E38" s="25" t="str">
+        <f>$E32 &amp; "-show"</f>
+        <v>disciplines-show</v>
+      </c>
+      <c r="F38" s="25" t="str">
+        <f>IF($E38="Da definire",$E38,_xlfn.CONCAT($E38,".blade.php"))</f>
+        <v>disciplines-show.blade.php</v>
+      </c>
+      <c r="G38" s="25" t="s">
+        <v>143</v>
+      </c>
+      <c r="H38" s="22"/>
+      <c r="I38" s="13"/>
+    </row>
+    <row r="39" spans="1:9" ht="19.899999999999999" customHeight="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="B38" s="25" t="str">
+      <c r="B39" s="25" t="str">
         <f t="shared" si="2"/>
         <v>/mng_activity/courses</v>
       </c>
-      <c r="C38" s="25" t="s">
+      <c r="C39" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="D38" s="25" t="s">
+      <c r="D39" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="E38" s="25" t="s">
+      <c r="E39" s="25" t="s">
         <v>113</v>
       </c>
-      <c r="F38" s="25" t="str">
+      <c r="F39" s="25" t="str">
         <f t="shared" si="0"/>
         <v>courses.blade.php</v>
       </c>
-      <c r="G38" s="25" t="s">
-        <v>142</v>
-      </c>
-      <c r="H38" s="22"/>
-      <c r="I38" s="13"/>
-    </row>
-    <row r="39" spans="1:9" ht="19.95" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
-      <c r="A39" s="25" t="s">
-        <v>150</v>
-      </c>
-      <c r="B39" s="25" t="str">
-        <f t="shared" ref="B39:B42" si="3">$B$31 &amp; "/" &amp; E39</f>
-        <v>/mng_activity/courses-create</v>
-      </c>
-      <c r="C39" s="25" t="s">
-        <v>145</v>
-      </c>
-      <c r="D39" s="22"/>
-      <c r="E39" s="25" t="str">
-        <f>$E38 &amp; "-create"</f>
-        <v>courses-create</v>
-      </c>
-      <c r="F39" s="25" t="str">
-        <f>IF($E39="Da definire",$E39,_xlfn.CONCAT($E39,".blade.php"))</f>
-        <v>courses-create.blade.php</v>
-      </c>
       <c r="G39" s="25" t="s">
         <v>142</v>
       </c>
       <c r="H39" s="22"/>
       <c r="I39" s="13"/>
     </row>
-    <row r="40" spans="1:9" ht="19.95" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" ht="19.899999999999999" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A40" s="25" t="s">
+        <v>150</v>
+      </c>
+      <c r="B40" s="25" t="str">
+        <f t="shared" ref="B40:B44" si="3">$B$31 &amp; "/" &amp; E40</f>
+        <v>/mng_activity/courses-create</v>
+      </c>
+      <c r="C40" s="25" t="s">
+        <v>145</v>
+      </c>
+      <c r="D40" s="22"/>
+      <c r="E40" s="25" t="str">
+        <f>$E39 &amp; "-create"</f>
+        <v>courses-create</v>
+      </c>
+      <c r="F40" s="25" t="str">
+        <f>IF($E40="Da definire",$E40,_xlfn.CONCAT($E40,".blade.php"))</f>
+        <v>courses-create.blade.php</v>
+      </c>
+      <c r="G40" s="25" t="s">
+        <v>142</v>
+      </c>
+      <c r="H40" s="22"/>
+      <c r="I40" s="13"/>
+    </row>
+    <row r="41" spans="1:9" ht="19.899999999999999" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="A41" s="25" t="s">
         <v>151</v>
       </c>
-      <c r="B40" s="25" t="str">
+      <c r="B41" s="25" t="str">
         <f t="shared" si="3"/>
         <v>/mng_activity/courses-store</v>
       </c>
-      <c r="C40" s="25" t="s">
+      <c r="C41" s="25" t="s">
         <v>76</v>
       </c>
-      <c r="D40" s="22"/>
-      <c r="E40" s="25" t="str">
-        <f>$E38 &amp; "-store"</f>
+      <c r="D41" s="22"/>
+      <c r="E41" s="25" t="str">
+        <f>$E39 &amp; "-store"</f>
         <v>courses-store</v>
       </c>
-      <c r="F40" s="25"/>
-      <c r="G40" s="25" t="s">
+      <c r="F41" s="25"/>
+      <c r="G41" s="25" t="s">
         <v>142</v>
       </c>
-      <c r="H40" s="22"/>
-      <c r="I40" s="13"/>
-    </row>
-    <row r="41" spans="1:9" ht="19.95" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
-      <c r="A41" s="25" t="s">
+      <c r="H41" s="22"/>
+      <c r="I41" s="13"/>
+    </row>
+    <row r="42" spans="1:9" ht="19.899999999999999" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="A42" s="25" t="s">
         <v>152</v>
       </c>
-      <c r="B41" s="25" t="str">
+      <c r="B42" s="25" t="str">
         <f t="shared" si="3"/>
         <v>/mng_activity/courses-edit</v>
       </c>
-      <c r="C41" s="25" t="s">
+      <c r="C42" s="25" t="s">
         <v>145</v>
       </c>
-      <c r="D41" s="22"/>
-      <c r="E41" s="25" t="str">
-        <f>$E38 &amp; "-edit"</f>
+      <c r="D42" s="22"/>
+      <c r="E42" s="25" t="str">
+        <f>$E39 &amp; "-edit"</f>
         <v>courses-edit</v>
       </c>
-      <c r="F41" s="25" t="str">
-        <f>IF($E41="Da definire",$E41,_xlfn.CONCAT($E41,".blade.php"))</f>
+      <c r="F42" s="25" t="str">
+        <f>IF($E42="Da definire",$E42,_xlfn.CONCAT($E42,".blade.php"))</f>
         <v>courses-edit.blade.php</v>
       </c>
-      <c r="G41" s="25" t="s">
+      <c r="G42" s="25" t="s">
         <v>142</v>
       </c>
-      <c r="H41" s="22"/>
-      <c r="I41" s="13"/>
-    </row>
-    <row r="42" spans="1:9" ht="19.95" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
-      <c r="A42" s="25" t="s">
+      <c r="H42" s="22"/>
+      <c r="I42" s="13"/>
+    </row>
+    <row r="43" spans="1:9" ht="19.899999999999999" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="A43" s="25" t="s">
         <v>153</v>
       </c>
-      <c r="B42" s="25" t="str">
+      <c r="B43" s="25" t="str">
         <f t="shared" si="3"/>
         <v>/mng_activity/courses-update</v>
       </c>
-      <c r="C42" s="25" t="s">
+      <c r="C43" s="25" t="s">
         <v>76</v>
-      </c>
-      <c r="D42" s="22"/>
-      <c r="E42" s="25" t="str">
-        <f>$E38 &amp; "-update"</f>
-        <v>courses-update</v>
-      </c>
-      <c r="F42" s="25"/>
-      <c r="G42" s="25" t="s">
-        <v>142</v>
-      </c>
-      <c r="H42" s="22"/>
-      <c r="I42" s="13"/>
-    </row>
-    <row r="43" spans="1:9" ht="19.95" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
-      <c r="A43" s="25" t="s">
-        <v>154</v>
-      </c>
-      <c r="B43" s="25" t="str">
-        <f>$B$31 &amp; "/" &amp; E43</f>
-        <v>/mng_activity/courses-delete</v>
-      </c>
-      <c r="C43" s="25" t="s">
-        <v>145</v>
       </c>
       <c r="D43" s="22"/>
       <c r="E43" s="25" t="str">
-        <f>$E38 &amp; "-delete"</f>
-        <v>courses-delete</v>
-      </c>
-      <c r="F43" s="25" t="str">
-        <f>IF($E43="Da definire",$E43,_xlfn.CONCAT($E43,".blade.php"))</f>
-        <v>courses-delete.blade.php</v>
-      </c>
+        <f>$E39 &amp; "-update"</f>
+        <v>courses-update</v>
+      </c>
+      <c r="F43" s="25"/>
       <c r="G43" s="25" t="s">
         <v>142</v>
       </c>
       <c r="H43" s="22"/>
       <c r="I43" s="13"/>
     </row>
-    <row r="44" spans="1:9" ht="19.95" customHeight="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" ht="19.899999999999999" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A44" s="25" t="s">
+        <v>154</v>
+      </c>
+      <c r="B44" s="25" t="str">
+        <f t="shared" si="3"/>
+        <v>/mng_activity/courses-delete</v>
+      </c>
+      <c r="C44" s="25" t="s">
+        <v>145</v>
+      </c>
+      <c r="D44" s="22"/>
+      <c r="E44" s="25" t="str">
+        <f>$E39 &amp; "-delete"</f>
+        <v>courses-delete</v>
+      </c>
+      <c r="F44" s="25" t="str">
+        <f>IF($E44="Da definire",$E44,_xlfn.CONCAT($E44,".blade.php"))</f>
+        <v>courses-delete.blade.php</v>
+      </c>
+      <c r="G44" s="25" t="s">
+        <v>142</v>
+      </c>
+      <c r="H44" s="22"/>
+      <c r="I44" s="13"/>
+    </row>
+    <row r="45" spans="1:9" ht="19.899999999999999" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="A45" s="25" t="s">
+        <v>170</v>
+      </c>
+      <c r="B45" s="25" t="str">
+        <f>$B$31 &amp; "/" &amp; E45</f>
+        <v>/mng_activity/courses-show</v>
+      </c>
+      <c r="C45" s="25" t="s">
+        <v>145</v>
+      </c>
+      <c r="D45" s="22"/>
+      <c r="E45" s="25" t="str">
+        <f>$E39 &amp; "-show"</f>
+        <v>courses-show</v>
+      </c>
+      <c r="F45" s="25" t="str">
+        <f>IF($E45="Da definire",$E45,_xlfn.CONCAT($E45,".blade.php"))</f>
+        <v>courses-show.blade.php</v>
+      </c>
+      <c r="G45" s="25" t="s">
+        <v>142</v>
+      </c>
+      <c r="H45" s="22"/>
+      <c r="I45" s="13"/>
+    </row>
+    <row r="46" spans="1:9" ht="19.899999999999999" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="B44" s="25" t="str">
+      <c r="B46" s="25" t="str">
         <f t="shared" si="2"/>
         <v>/mng_activity/packages</v>
       </c>
-      <c r="C44" s="25" t="s">
+      <c r="C46" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="D44" s="25" t="s">
+      <c r="D46" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="E44" s="25" t="s">
+      <c r="E46" s="25" t="s">
         <v>115</v>
       </c>
-      <c r="F44" s="25" t="str">
+      <c r="F46" s="25" t="str">
         <f t="shared" si="0"/>
         <v>packages.blade.php</v>
       </c>
-      <c r="G44" s="25" t="s">
+      <c r="G46" s="25" t="s">
         <v>155</v>
       </c>
-      <c r="H44" s="22"/>
-      <c r="I44" s="13"/>
-    </row>
-    <row r="45" spans="1:9" ht="19.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
-      <c r="A45" s="25" t="s">
+      <c r="H46" s="22"/>
+      <c r="I46" s="13"/>
+    </row>
+    <row r="47" spans="1:9" ht="19.899999999999999" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="A47" s="25" t="s">
         <v>156</v>
       </c>
-      <c r="B45" s="25" t="str">
-        <f t="shared" ref="B45:B48" si="4">$B$31 &amp; "/" &amp; E45</f>
+      <c r="B47" s="25" t="str">
+        <f t="shared" ref="B47:B50" si="4">$B$31 &amp; "/" &amp; E47</f>
         <v>/mng_activity/packages-create</v>
       </c>
-      <c r="C45" s="25" t="s">
+      <c r="C47" s="25" t="s">
         <v>145</v>
       </c>
-      <c r="D45" s="22"/>
-      <c r="E45" s="25" t="str">
-        <f>$E44 &amp; "-create"</f>
+      <c r="D47" s="22"/>
+      <c r="E47" s="25" t="str">
+        <f>$E46 &amp; "-create"</f>
         <v>packages-create</v>
       </c>
-      <c r="F45" s="25" t="str">
-        <f>IF($E45="Da definire",$E45,_xlfn.CONCAT($E45,".blade.php"))</f>
+      <c r="F47" s="25" t="str">
+        <f>IF($E47="Da definire",$E47,_xlfn.CONCAT($E47,".blade.php"))</f>
         <v>packages-create.blade.php</v>
       </c>
-      <c r="G45" s="25" t="s">
+      <c r="G47" s="25" t="s">
         <v>155</v>
       </c>
-      <c r="H45" s="22"/>
-      <c r="I45" s="13"/>
-    </row>
-    <row r="46" spans="1:9" ht="19.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
-      <c r="A46" s="25" t="s">
+      <c r="H47" s="22"/>
+      <c r="I47" s="13"/>
+    </row>
+    <row r="48" spans="1:9" ht="19.899999999999999" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="A48" s="25" t="s">
         <v>157</v>
       </c>
-      <c r="B46" s="25" t="str">
+      <c r="B48" s="25" t="str">
         <f t="shared" si="4"/>
         <v>/mng_activity/packages-store</v>
       </c>
-      <c r="C46" s="25" t="s">
-        <v>76</v>
-      </c>
-      <c r="D46" s="22"/>
-      <c r="E46" s="25" t="str">
-        <f>$E44 &amp; "-store"</f>
-        <v>packages-store</v>
-      </c>
-      <c r="F46" s="25"/>
-      <c r="G46" s="25" t="s">
-        <v>155</v>
-      </c>
-      <c r="H46" s="22"/>
-      <c r="I46" s="13"/>
-    </row>
-    <row r="47" spans="1:9" ht="19.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
-      <c r="A47" s="25" t="s">
-        <v>158</v>
-      </c>
-      <c r="B47" s="25" t="str">
-        <f t="shared" si="4"/>
-        <v>/mng_activity/packages-edit</v>
-      </c>
-      <c r="C47" s="25" t="s">
-        <v>145</v>
-      </c>
-      <c r="D47" s="22"/>
-      <c r="E47" s="25" t="str">
-        <f>$E44 &amp; "-edit"</f>
-        <v>packages-edit</v>
-      </c>
-      <c r="F47" s="25" t="str">
-        <f>IF($E47="Da definire",$E47,_xlfn.CONCAT($E47,".blade.php"))</f>
-        <v>packages-edit.blade.php</v>
-      </c>
-      <c r="G47" s="25" t="s">
-        <v>155</v>
-      </c>
-      <c r="H47" s="22"/>
-      <c r="I47" s="13"/>
-    </row>
-    <row r="48" spans="1:9" ht="19.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
-      <c r="A48" s="25" t="s">
-        <v>159</v>
-      </c>
-      <c r="B48" s="25" t="str">
-        <f t="shared" si="4"/>
-        <v>/mng_activity/packages-update</v>
-      </c>
       <c r="C48" s="25" t="s">
         <v>76</v>
       </c>
       <c r="D48" s="22"/>
       <c r="E48" s="25" t="str">
-        <f>$E44 &amp; "-update"</f>
-        <v>packages-update</v>
+        <f>$E46 &amp; "-store"</f>
+        <v>packages-store</v>
       </c>
       <c r="F48" s="25"/>
       <c r="G48" s="25" t="s">
@@ -2566,25 +2595,25 @@
       <c r="H48" s="22"/>
       <c r="I48" s="13"/>
     </row>
-    <row r="49" spans="1:9" ht="19.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:9" ht="19.899999999999999" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A49" s="25" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B49" s="25" t="str">
-        <f>$B$31 &amp; "/" &amp; E49</f>
-        <v>/mng_activity/packages-delete</v>
+        <f t="shared" si="4"/>
+        <v>/mng_activity/packages-edit</v>
       </c>
       <c r="C49" s="25" t="s">
         <v>145</v>
       </c>
       <c r="D49" s="22"/>
       <c r="E49" s="25" t="str">
-        <f>$E44 &amp; "-delete"</f>
-        <v>packages-delete</v>
+        <f>$E46 &amp; "-edit"</f>
+        <v>packages-edit</v>
       </c>
       <c r="F49" s="25" t="str">
         <f>IF($E49="Da definire",$E49,_xlfn.CONCAT($E49,".blade.php"))</f>
-        <v>packages-delete.blade.php</v>
+        <v>packages-edit.blade.php</v>
       </c>
       <c r="G49" s="25" t="s">
         <v>155</v>
@@ -2592,120 +2621,319 @@
       <c r="H49" s="22"/>
       <c r="I49" s="13"/>
     </row>
-    <row r="50" spans="1:9" ht="19.8" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:9" ht="19.899999999999999" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A50" s="25" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B50" s="25" t="str">
-        <f>$B$31 &amp; "/" &amp; E50</f>
-        <v>/mng_activity/packages-show</v>
+        <f t="shared" si="4"/>
+        <v>/mng_activity/packages-update</v>
       </c>
       <c r="C50" s="25" t="s">
-        <v>145</v>
+        <v>76</v>
       </c>
       <c r="D50" s="22"/>
       <c r="E50" s="25" t="str">
-        <f>$E44 &amp; "-show"</f>
-        <v>packages-show</v>
-      </c>
-      <c r="F50" s="25" t="str">
-        <f>IF($E50="Da definire",$E50,_xlfn.CONCAT($E50,".blade.php"))</f>
-        <v>packages-show.blade.php</v>
-      </c>
+        <f>$E46 &amp; "-update"</f>
+        <v>packages-update</v>
+      </c>
+      <c r="F50" s="25"/>
       <c r="G50" s="25" t="s">
         <v>155</v>
       </c>
       <c r="H50" s="22"/>
       <c r="I50" s="13"/>
     </row>
-    <row r="51" spans="1:9" ht="19.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:9" ht="19.899999999999999" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A51" s="25" t="s">
-        <v>39</v>
+        <v>160</v>
       </c>
       <c r="B51" s="25" t="str">
-        <f t="shared" si="2"/>
-        <v>/mng_activity/rooms</v>
+        <f>$B$31 &amp; "/" &amp; E51</f>
+        <v>/mng_activity/packages-delete</v>
       </c>
       <c r="C51" s="25" t="s">
-        <v>63</v>
-      </c>
-      <c r="D51" s="22" t="s">
-        <v>30</v>
-      </c>
-      <c r="E51" s="25" t="s">
-        <v>114</v>
+        <v>145</v>
+      </c>
+      <c r="D51" s="22"/>
+      <c r="E51" s="25" t="str">
+        <f>$E46 &amp; "-delete"</f>
+        <v>packages-delete</v>
       </c>
       <c r="F51" s="25" t="str">
-        <f t="shared" si="0"/>
-        <v>rooms.blade.php</v>
+        <f>IF($E51="Da definire",$E51,_xlfn.CONCAT($E51,".blade.php"))</f>
+        <v>packages-delete.blade.php</v>
       </c>
       <c r="G51" s="25" t="s">
-        <v>120</v>
+        <v>155</v>
       </c>
       <c r="H51" s="22"/>
       <c r="I51" s="13"/>
     </row>
-    <row r="52" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:9" ht="19.899999999999999" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A52" s="25" t="s">
+        <v>161</v>
+      </c>
+      <c r="B52" s="25" t="str">
+        <f>$B$31 &amp; "/" &amp; E52</f>
+        <v>/mng_activity/packages-show</v>
+      </c>
+      <c r="C52" s="25" t="s">
+        <v>145</v>
+      </c>
+      <c r="D52" s="22"/>
+      <c r="E52" s="25" t="str">
+        <f>$E46 &amp; "-show"</f>
+        <v>packages-show</v>
+      </c>
+      <c r="F52" s="25" t="str">
+        <f>IF($E52="Da definire",$E52,_xlfn.CONCAT($E52,".blade.php"))</f>
+        <v>packages-show.blade.php</v>
+      </c>
+      <c r="G52" s="25" t="s">
+        <v>155</v>
+      </c>
+      <c r="H52" s="22"/>
+      <c r="I52" s="13"/>
+    </row>
+    <row r="53" spans="1:9" ht="19.899999999999999" customHeight="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="B53" s="25" t="str">
+        <f>$B$31 &amp; "/" &amp; E53</f>
+        <v>/mng_activity/rooms</v>
+      </c>
+      <c r="C53" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="D53" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="E53" s="25" t="s">
+        <v>114</v>
+      </c>
+      <c r="F53" s="25" t="str">
+        <f>IF($E53="Da definire",$E53,_xlfn.CONCAT($E53,".blade.php"))</f>
+        <v>rooms.blade.php</v>
+      </c>
+      <c r="G53" s="25" t="s">
+        <v>168</v>
+      </c>
+      <c r="H53" s="22"/>
+      <c r="I53" s="13"/>
+    </row>
+    <row r="54" spans="1:9" ht="19.899999999999999" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="A54" s="25" t="s">
+        <v>162</v>
+      </c>
+      <c r="B54" s="25" t="str">
+        <f>$B$31 &amp; "/" &amp; E54</f>
+        <v>/mng_activity/rooms-create</v>
+      </c>
+      <c r="C54" s="25" t="s">
+        <v>145</v>
+      </c>
+      <c r="D54" s="22"/>
+      <c r="E54" s="25" t="str">
+        <f>$E53 &amp; "-create"</f>
+        <v>rooms-create</v>
+      </c>
+      <c r="F54" s="25" t="str">
+        <f>IF($E54="Da definire",$E54,_xlfn.CONCAT($E54,".blade.php"))</f>
+        <v>rooms-create.blade.php</v>
+      </c>
+      <c r="G54" s="25" t="s">
+        <v>168</v>
+      </c>
+      <c r="H54" s="22"/>
+      <c r="I54" s="13"/>
+    </row>
+    <row r="55" spans="1:9" ht="19.899999999999999" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="A55" s="25" t="s">
+        <v>163</v>
+      </c>
+      <c r="B55" s="25" t="str">
+        <f t="shared" ref="B54:B57" si="5">$B$31 &amp; "/" &amp; E55</f>
+        <v>/mng_activity/rooms-store</v>
+      </c>
+      <c r="C55" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="D55" s="22"/>
+      <c r="E55" s="25" t="str">
+        <f>$E53 &amp; "-store"</f>
+        <v>rooms-store</v>
+      </c>
+      <c r="F55" s="25"/>
+      <c r="G55" s="25" t="s">
+        <v>168</v>
+      </c>
+      <c r="H55" s="22"/>
+      <c r="I55" s="13"/>
+    </row>
+    <row r="56" spans="1:9" ht="19.899999999999999" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="A56" s="25" t="s">
+        <v>164</v>
+      </c>
+      <c r="B56" s="25" t="str">
+        <f t="shared" si="5"/>
+        <v>/mng_activity/rooms-edit</v>
+      </c>
+      <c r="C56" s="25" t="s">
+        <v>145</v>
+      </c>
+      <c r="D56" s="22"/>
+      <c r="E56" s="25" t="str">
+        <f>$E53 &amp; "-edit"</f>
+        <v>rooms-edit</v>
+      </c>
+      <c r="F56" s="25" t="str">
+        <f>IF($E56="Da definire",$E56,_xlfn.CONCAT($E56,".blade.php"))</f>
+        <v>rooms-edit.blade.php</v>
+      </c>
+      <c r="G56" s="25" t="s">
+        <v>168</v>
+      </c>
+      <c r="H56" s="22"/>
+      <c r="I56" s="13"/>
+    </row>
+    <row r="57" spans="1:9" ht="19.899999999999999" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="A57" s="25" t="s">
+        <v>165</v>
+      </c>
+      <c r="B57" s="25" t="str">
+        <f t="shared" si="5"/>
+        <v>/mng_activity/rooms-update</v>
+      </c>
+      <c r="C57" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="D57" s="22"/>
+      <c r="E57" s="25" t="str">
+        <f>$E53 &amp; "-update"</f>
+        <v>rooms-update</v>
+      </c>
+      <c r="F57" s="25"/>
+      <c r="G57" s="25" t="s">
+        <v>168</v>
+      </c>
+      <c r="H57" s="22"/>
+      <c r="I57" s="13"/>
+    </row>
+    <row r="58" spans="1:9" ht="19.899999999999999" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="A58" s="25" t="s">
+        <v>166</v>
+      </c>
+      <c r="B58" s="25" t="str">
+        <f>$B$31 &amp; "/" &amp; E58</f>
+        <v>/mng_activity/rooms-delete</v>
+      </c>
+      <c r="C58" s="25" t="s">
+        <v>145</v>
+      </c>
+      <c r="D58" s="22"/>
+      <c r="E58" s="25" t="str">
+        <f>$E53 &amp; "-delete"</f>
+        <v>rooms-delete</v>
+      </c>
+      <c r="F58" s="25" t="str">
+        <f>IF($E58="Da definire",$E58,_xlfn.CONCAT($E58,".blade.php"))</f>
+        <v>rooms-delete.blade.php</v>
+      </c>
+      <c r="G58" s="25" t="s">
+        <v>168</v>
+      </c>
+      <c r="H58" s="22"/>
+      <c r="I58" s="13"/>
+    </row>
+    <row r="59" spans="1:9" ht="19.899999999999999" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="A59" s="25" t="s">
+        <v>167</v>
+      </c>
+      <c r="B59" s="25" t="str">
+        <f>$B$31 &amp; "/" &amp; E59</f>
+        <v>/mng_activity/rooms-show</v>
+      </c>
+      <c r="C59" s="25" t="s">
+        <v>145</v>
+      </c>
+      <c r="D59" s="22"/>
+      <c r="E59" s="25" t="str">
+        <f>$E53 &amp; "-show"</f>
+        <v>rooms-show</v>
+      </c>
+      <c r="F59" s="25" t="str">
+        <f>IF($E59="Da definire",$E59,_xlfn.CONCAT($E59,".blade.php"))</f>
+        <v>rooms-show.blade.php</v>
+      </c>
+      <c r="G59" s="25" t="s">
+        <v>168</v>
+      </c>
+      <c r="H59" s="22"/>
+      <c r="I59" s="13"/>
+    </row>
+    <row r="60" spans="1:9" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="B52" s="25" t="str">
+      <c r="B60" s="25" t="str">
         <f t="shared" si="2"/>
         <v>/mng_activity/scheduling</v>
       </c>
-      <c r="C52" s="25" t="s">
+      <c r="C60" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="D52" s="22" t="s">
+      <c r="D60" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="E52" s="25" t="s">
+      <c r="E60" s="25" t="s">
         <v>116</v>
       </c>
-      <c r="F52" s="25" t="str">
+      <c r="F60" s="25" t="str">
         <f t="shared" si="0"/>
         <v>scheduling.blade.php</v>
       </c>
-      <c r="G52" s="25" t="s">
+      <c r="G60" s="25" t="s">
         <v>120</v>
       </c>
-      <c r="H52" s="22"/>
-      <c r="I52" s="13"/>
-    </row>
-    <row r="53" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="26"/>
-      <c r="B53" s="26" t="str">
-        <f>"/" &amp; E53</f>
+      <c r="H60" s="22"/>
+      <c r="I60" s="13"/>
+    </row>
+    <row r="61" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="26"/>
+      <c r="B61" s="26" t="str">
+        <f>"/" &amp; E61</f>
         <v>/report_stats</v>
       </c>
-      <c r="C53" s="26" t="s">
+      <c r="C61" s="26" t="s">
         <v>63</v>
       </c>
-      <c r="D53" s="23" t="s">
+      <c r="D61" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="E53" s="26" t="s">
+      <c r="E61" s="26" t="s">
         <v>97</v>
       </c>
-      <c r="F53" s="26" t="str">
+      <c r="F61" s="26" t="str">
         <f t="shared" si="0"/>
         <v>report_stats.blade.php</v>
       </c>
-      <c r="G53" s="26" t="s">
+      <c r="G61" s="26" t="s">
         <v>95</v>
       </c>
-      <c r="H53" s="23" t="s">
+      <c r="H61" s="23" t="s">
         <v>98</v>
       </c>
-      <c r="I53" s="13"/>
+      <c r="I61" s="13"/>
     </row>
   </sheetData>
   <dataConsolidate/>
   <dataValidations count="2">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C53" xr:uid="{F340BA2D-9D43-4A9F-86F9-B281B429D2E7}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C61" xr:uid="{F340BA2D-9D43-4A9F-86F9-B281B429D2E7}">
       <formula1>RefTipo</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G53" xr:uid="{DFF187B0-2821-4C72-B394-0420A8E90996}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G61" xr:uid="{DFF187B0-2821-4C72-B394-0420A8E90996}">
       <formula1>RefController_nome</formula1>
     </dataValidation>
   </dataValidations>
@@ -2725,20 +2953,20 @@
   <dimension ref="B1:G28"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="6" width="25.109375" customWidth="1"/>
-    <col min="7" max="7" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="6" width="25.140625" customWidth="1"/>
+    <col min="7" max="7" width="24.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="19" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>68</v>
       </c>
@@ -2752,7 +2980,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="3" t="s">
         <v>66</v>
       </c>
@@ -2761,7 +2989,7 @@
       </c>
       <c r="E2" s="5"/>
     </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>145</v>
       </c>
@@ -2770,7 +2998,7 @@
       </c>
       <c r="E3" s="5"/>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>65</v>
       </c>
@@ -2779,7 +3007,7 @@
       </c>
       <c r="E4" s="5"/>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>64</v>
       </c>
@@ -2787,7 +3015,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
         <v>63</v>
       </c>
@@ -2795,7 +3023,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
         <v>87</v>
       </c>
@@ -2803,7 +3031,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="s">
         <v>96</v>
       </c>
@@ -2811,7 +3039,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="s">
         <v>76</v>
       </c>
@@ -2819,32 +3047,37 @@
         <v>120</v>
       </c>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D10" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D11" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D12" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D13" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B15" s="17"/>
       <c r="C15" s="16"/>
       <c r="D15" s="16"/>
       <c r="E15" s="16"/>
     </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B16" s="9"/>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
@@ -2852,7 +3085,7 @@
       <c r="F16" s="10"/>
       <c r="G16" s="8"/>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="9"/>
       <c r="C17" s="6"/>
       <c r="D17" s="7"/>
@@ -2860,7 +3093,7 @@
       <c r="F17" s="10"/>
       <c r="G17" s="8"/>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="9"/>
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
@@ -2868,7 +3101,7 @@
       <c r="F18" s="10"/>
       <c r="G18" s="8"/>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="9"/>
       <c r="C19" s="6"/>
       <c r="D19" s="7"/>
@@ -2876,7 +3109,7 @@
       <c r="F19" s="10"/>
       <c r="G19" s="8"/>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="9"/>
       <c r="C20" s="6"/>
       <c r="D20" s="7"/>
@@ -2884,7 +3117,7 @@
       <c r="F20" s="10"/>
       <c r="G20" s="8"/>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="9"/>
       <c r="C21" s="6"/>
       <c r="D21" s="7"/>
@@ -2892,7 +3125,7 @@
       <c r="F21" s="10"/>
       <c r="G21" s="8"/>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="9"/>
       <c r="C22" s="6"/>
       <c r="D22" s="7"/>
@@ -2900,7 +3133,7 @@
       <c r="F22" s="10"/>
       <c r="G22" s="8"/>
     </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" s="9"/>
       <c r="C23" s="6"/>
       <c r="D23" s="7"/>
@@ -2908,7 +3141,7 @@
       <c r="F23" s="10"/>
       <c r="G23" s="8"/>
     </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" s="9"/>
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
@@ -2916,7 +3149,7 @@
       <c r="F24" s="10"/>
       <c r="G24" s="8"/>
     </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" s="9"/>
       <c r="C25" s="6"/>
       <c r="D25" s="7"/>
@@ -2924,7 +3157,7 @@
       <c r="F25" s="10"/>
       <c r="G25" s="8"/>
     </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" s="9"/>
       <c r="C26" s="6"/>
       <c r="D26" s="7"/>
@@ -2932,7 +3165,7 @@
       <c r="F26" s="10"/>
       <c r="G26" s="8"/>
     </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" s="9"/>
       <c r="C27" s="6"/>
       <c r="D27" s="7"/>
@@ -2940,13 +3173,13 @@
       <c r="F27" s="10"/>
       <c r="G27" s="8"/>
     </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D28" s="7"/>
       <c r="E28" s="10"/>
       <c r="F28" s="10"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="D13:D29">
+  <sortState ref="D13:D29">
     <sortCondition ref="D13"/>
   </sortState>
   <dataConsolidate/>

</xml_diff>

<commit_message>
Iniziate le CRUD per scheduling
</commit_message>
<xml_diff>
--- a/Documentazioni/Codifica pagine sito.xlsx
+++ b/Documentazioni/Codifica pagine sito.xlsx
@@ -1,18 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
   <workbookPr filterPrivacy="1" codeName="Questa_cartella_di_lavoro"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D106A1C-CF76-4E72-A4AD-0240D5AB1303}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{312E79FD-DF42-46E7-B4A9-EEEAF626DCF8}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1500" yWindow="1500" windowWidth="17280" windowHeight="8970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
     <sheet name="Foglio utile" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Main!$A$1:$H$61</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Main!$A$1:$H$68</definedName>
     <definedName name="RefController_nome">Controller[Lista Controller]</definedName>
     <definedName name="RefTipo">Tipo[]</definedName>
   </definedNames>
@@ -24,6 +24,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="179">
   <si>
     <t>Nome gabbia logica</t>
   </si>
@@ -544,6 +545,30 @@
   </si>
   <si>
     <t>M326</t>
+  </si>
+  <si>
+    <t>M351</t>
+  </si>
+  <si>
+    <t>M352</t>
+  </si>
+  <si>
+    <t>M353</t>
+  </si>
+  <si>
+    <t>M354</t>
+  </si>
+  <si>
+    <t>M355</t>
+  </si>
+  <si>
+    <t>M356</t>
+  </si>
+  <si>
+    <t>SchedulingController</t>
+  </si>
+  <si>
+    <t>M360</t>
   </si>
 </sst>
 </file>
@@ -973,8 +998,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{905F6574-56C3-4E36-86AD-16F4E970F9D2}" name="Tabella4" displayName="Tabella4" ref="A1:H61" dataDxfId="17">
-  <autoFilter ref="A1:H61" xr:uid="{34684D11-7ACD-45A4-AA96-0CE6C7239D98}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{905F6574-56C3-4E36-86AD-16F4E970F9D2}" name="Tabella4" displayName="Tabella4" ref="A1:H68" dataDxfId="17">
+  <autoFilter ref="A1:H68" xr:uid="{34684D11-7ACD-45A4-AA96-0CE6C7239D98}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{E7D98D43-EB7B-46CE-B0B0-C555D83773A6}" name="Codice gabbia logica" dataDxfId="16" totalsRowDxfId="15"/>
     <tableColumn id="8" xr3:uid="{CAF26B0C-D3E2-4A71-A7C5-519E983C334C}" name="Rotta" dataDxfId="14" totalsRowDxfId="13">
@@ -996,7 +1021,7 @@
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{45120F09-8607-4F6A-A989-7184307236A1}" name="Tipo" displayName="Tipo" ref="B1:B9" totalsRowShown="0" headerRowDxfId="2" tableBorderDxfId="1">
   <autoFilter ref="B1:B9" xr:uid="{B0803B6A-3448-4A89-AC43-1127F3DBD833}"/>
-  <sortState ref="B2:B8">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:B8">
     <sortCondition ref="B1:B8"/>
   </sortState>
   <tableColumns count="1">
@@ -1282,30 +1307,30 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Foglio2"/>
-  <dimension ref="A1:I61"/>
+  <dimension ref="A1:I68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G45" sqref="G45"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A61" sqref="A61:A66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" outlineLevelRow="2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" outlineLevelRow="2" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.5703125" style="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.5546875" style="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.109375" style="13" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13" style="12" customWidth="1"/>
-    <col min="4" max="4" width="35.5703125" style="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.42578125" style="15" customWidth="1"/>
-    <col min="6" max="6" width="24.42578125" style="13" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="88.42578125" style="13" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="89.7109375" style="11" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="28.7109375" style="13" customWidth="1"/>
-    <col min="11" max="12" width="8.85546875" style="13"/>
+    <col min="4" max="4" width="35.5546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.44140625" style="15" customWidth="1"/>
+    <col min="6" max="6" width="24.44140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="88.44140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="89.6640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="28.6640625" style="13" customWidth="1"/>
+    <col min="11" max="12" width="8.88671875" style="13"/>
     <col min="13" max="13" width="19" style="13" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="8.85546875" style="13"/>
+    <col min="14" max="16384" width="8.88671875" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
         <v>1</v>
       </c>
@@ -1332,7 +1357,7 @@
       </c>
       <c r="I1" s="13"/>
     </row>
-    <row r="2" spans="1:9" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
         <v>43</v>
       </c>
@@ -1350,7 +1375,7 @@
         <v>61</v>
       </c>
       <c r="F2" s="18" t="str">
-        <f t="shared" ref="F2:F61" si="0">IF($E2="Da definire",$E2,_xlfn.CONCAT($E2,".blade.php"))</f>
+        <f t="shared" ref="F2:F68" si="0">IF($E2="Da definire",$E2,_xlfn.CONCAT($E2,".blade.php"))</f>
         <v>welcome.blade.php</v>
       </c>
       <c r="G2" s="18" t="s">
@@ -1361,7 +1386,7 @@
       </c>
       <c r="I2" s="13"/>
     </row>
-    <row r="3" spans="1:9" ht="19.899999999999999" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="19.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A3" s="18"/>
       <c r="B3" s="18" t="str">
         <f>"/" &amp; E3</f>
@@ -1381,7 +1406,7 @@
       </c>
       <c r="I3" s="13"/>
     </row>
-    <row r="4" spans="1:9" ht="19.899999999999999" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="19.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
         <v>139</v>
       </c>
@@ -1408,7 +1433,7 @@
       </c>
       <c r="I4" s="13"/>
     </row>
-    <row r="5" spans="1:9" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="18" t="s">
         <v>44</v>
       </c>
@@ -1437,7 +1462,7 @@
       </c>
       <c r="I5" s="13"/>
     </row>
-    <row r="6" spans="1:9" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="18" t="s">
         <v>53</v>
       </c>
@@ -1466,7 +1491,7 @@
       </c>
       <c r="I6" s="13"/>
     </row>
-    <row r="7" spans="1:9" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="18" t="s">
         <v>126</v>
       </c>
@@ -1495,7 +1520,7 @@
       </c>
       <c r="I7" s="12"/>
     </row>
-    <row r="8" spans="1:9" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="18" t="s">
         <v>45</v>
       </c>
@@ -1524,7 +1549,7 @@
       </c>
       <c r="I8" s="12"/>
     </row>
-    <row r="9" spans="1:9" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="18" t="s">
         <v>47</v>
       </c>
@@ -1553,7 +1578,7 @@
       </c>
       <c r="I9" s="12"/>
     </row>
-    <row r="10" spans="1:9" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="18" t="s">
         <v>49</v>
       </c>
@@ -1582,7 +1607,7 @@
       </c>
       <c r="I10" s="13"/>
     </row>
-    <row r="11" spans="1:9" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="18" t="s">
         <v>51</v>
       </c>
@@ -1611,7 +1636,7 @@
       </c>
       <c r="I11" s="13"/>
     </row>
-    <row r="12" spans="1:9" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="18" t="s">
         <v>54</v>
       </c>
@@ -1640,7 +1665,7 @@
       </c>
       <c r="I12" s="13"/>
     </row>
-    <row r="13" spans="1:9" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="18" t="s">
         <v>57</v>
       </c>
@@ -1669,7 +1694,7 @@
       </c>
       <c r="I13" s="13"/>
     </row>
-    <row r="14" spans="1:9" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="18" t="s">
         <v>58</v>
       </c>
@@ -1698,7 +1723,7 @@
       </c>
       <c r="I14" s="13"/>
     </row>
-    <row r="15" spans="1:9" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="28" t="s">
         <v>42</v>
       </c>
@@ -1727,7 +1752,7 @@
       </c>
       <c r="I15" s="13"/>
     </row>
-    <row r="16" spans="1:9" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="26"/>
       <c r="B16" s="26" t="str">
         <f t="shared" si="1"/>
@@ -1754,7 +1779,7 @@
       </c>
       <c r="I16" s="13"/>
     </row>
-    <row r="17" spans="1:9" ht="19.899999999999999" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" ht="19.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A17" s="27" t="s">
         <v>18</v>
       </c>
@@ -1783,7 +1808,7 @@
       </c>
       <c r="I17" s="13"/>
     </row>
-    <row r="18" spans="1:9" ht="19.899999999999999" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" ht="19.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A18" s="25" t="s">
         <v>19</v>
       </c>
@@ -1810,7 +1835,7 @@
       <c r="H18" s="22"/>
       <c r="I18" s="13"/>
     </row>
-    <row r="19" spans="1:9" ht="19.899999999999999" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" ht="19.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A19" s="25" t="s">
         <v>20</v>
       </c>
@@ -1837,7 +1862,7 @@
       <c r="H19" s="22"/>
       <c r="I19" s="13"/>
     </row>
-    <row r="20" spans="1:9" ht="19.899999999999999" customHeight="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" ht="19.95" customHeight="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.3">
       <c r="A20" s="25" t="s">
         <v>21</v>
       </c>
@@ -1864,7 +1889,7 @@
       <c r="H20" s="22"/>
       <c r="I20" s="13"/>
     </row>
-    <row r="21" spans="1:9" ht="19.899999999999999" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" ht="19.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A21" s="25" t="s">
         <v>22</v>
       </c>
@@ -1891,7 +1916,7 @@
       <c r="H21" s="22"/>
       <c r="I21" s="13"/>
     </row>
-    <row r="22" spans="1:9" ht="19.899999999999999" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" ht="19.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A22" s="27" t="s">
         <v>23</v>
       </c>
@@ -1920,7 +1945,7 @@
       </c>
       <c r="I22" s="13"/>
     </row>
-    <row r="23" spans="1:9" ht="19.899999999999999" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" ht="19.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A23" s="25" t="s">
         <v>24</v>
       </c>
@@ -1947,7 +1972,7 @@
       <c r="H23" s="22"/>
       <c r="I23" s="13"/>
     </row>
-    <row r="24" spans="1:9" ht="19.899999999999999" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" ht="19.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A24" s="25" t="s">
         <v>25</v>
       </c>
@@ -1974,7 +1999,7 @@
       <c r="H24" s="22"/>
       <c r="I24" s="13"/>
     </row>
-    <row r="25" spans="1:9" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="26"/>
       <c r="B25" s="26" t="str">
         <f>"/" &amp; E25</f>
@@ -2001,7 +2026,7 @@
       </c>
       <c r="I25" s="13"/>
     </row>
-    <row r="26" spans="1:9" ht="19.899999999999999" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" ht="19.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A26" s="27" t="s">
         <v>26</v>
       </c>
@@ -2030,7 +2055,7 @@
       </c>
       <c r="I26" s="13"/>
     </row>
-    <row r="27" spans="1:9" ht="19.899999999999999" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" ht="19.95" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A27" s="25" t="s">
         <v>35</v>
       </c>
@@ -2057,7 +2082,7 @@
       <c r="H27" s="22"/>
       <c r="I27" s="13"/>
     </row>
-    <row r="28" spans="1:9" ht="19.899999999999999" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" ht="19.95" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A28" s="25" t="s">
         <v>128</v>
       </c>
@@ -2084,7 +2109,7 @@
       <c r="H28" s="22"/>
       <c r="I28" s="13"/>
     </row>
-    <row r="29" spans="1:9" ht="19.899999999999999" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" ht="19.95" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A29" s="25" t="s">
         <v>129</v>
       </c>
@@ -2111,7 +2136,7 @@
       <c r="H29" s="22"/>
       <c r="I29" s="13"/>
     </row>
-    <row r="30" spans="1:9" ht="19.899999999999999" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" ht="19.95" customHeight="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.3">
       <c r="A30" s="27" t="s">
         <v>36</v>
       </c>
@@ -2138,7 +2163,7 @@
       <c r="H30" s="21"/>
       <c r="I30" s="13"/>
     </row>
-    <row r="31" spans="1:9" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="26"/>
       <c r="B31" s="26" t="str">
         <f>"/" &amp; E31</f>
@@ -2165,7 +2190,7 @@
       </c>
       <c r="I31" s="13"/>
     </row>
-    <row r="32" spans="1:9" ht="19.899999999999999" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" ht="19.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A32" s="25" t="s">
         <v>37</v>
       </c>
@@ -2192,7 +2217,7 @@
       <c r="H32" s="22"/>
       <c r="I32" s="13"/>
     </row>
-    <row r="33" spans="1:9" ht="19.899999999999999" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" ht="19.95" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A33" s="25" t="s">
         <v>144</v>
       </c>
@@ -2218,7 +2243,7 @@
       <c r="H33" s="22"/>
       <c r="I33" s="13"/>
     </row>
-    <row r="34" spans="1:9" ht="19.899999999999999" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" ht="19.95" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A34" s="25" t="s">
         <v>146</v>
       </c>
@@ -2241,7 +2266,7 @@
       <c r="H34" s="22"/>
       <c r="I34" s="13"/>
     </row>
-    <row r="35" spans="1:9" ht="19.899999999999999" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" ht="19.95" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A35" s="25" t="s">
         <v>147</v>
       </c>
@@ -2267,7 +2292,7 @@
       <c r="H35" s="22"/>
       <c r="I35" s="13"/>
     </row>
-    <row r="36" spans="1:9" ht="19.899999999999999" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" ht="19.95" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A36" s="25" t="s">
         <v>148</v>
       </c>
@@ -2290,7 +2315,7 @@
       <c r="H36" s="22"/>
       <c r="I36" s="13"/>
     </row>
-    <row r="37" spans="1:9" ht="19.899999999999999" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" ht="19.95" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A37" s="25" t="s">
         <v>149</v>
       </c>
@@ -2316,7 +2341,7 @@
       <c r="H37" s="22"/>
       <c r="I37" s="13"/>
     </row>
-    <row r="38" spans="1:9" ht="19.899999999999999" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" ht="19.95" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A38" s="25" t="s">
         <v>169</v>
       </c>
@@ -2342,7 +2367,7 @@
       <c r="H38" s="22"/>
       <c r="I38" s="13"/>
     </row>
-    <row r="39" spans="1:9" ht="19.899999999999999" customHeight="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" ht="19.95" customHeight="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.3">
       <c r="A39" s="25" t="s">
         <v>38</v>
       </c>
@@ -2369,7 +2394,7 @@
       <c r="H39" s="22"/>
       <c r="I39" s="13"/>
     </row>
-    <row r="40" spans="1:9" ht="19.899999999999999" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" ht="19.95" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A40" s="25" t="s">
         <v>150</v>
       </c>
@@ -2395,7 +2420,7 @@
       <c r="H40" s="22"/>
       <c r="I40" s="13"/>
     </row>
-    <row r="41" spans="1:9" ht="19.899999999999999" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" ht="19.95" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A41" s="25" t="s">
         <v>151</v>
       </c>
@@ -2418,7 +2443,7 @@
       <c r="H41" s="22"/>
       <c r="I41" s="13"/>
     </row>
-    <row r="42" spans="1:9" ht="19.899999999999999" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" ht="19.95" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A42" s="25" t="s">
         <v>152</v>
       </c>
@@ -2444,7 +2469,7 @@
       <c r="H42" s="22"/>
       <c r="I42" s="13"/>
     </row>
-    <row r="43" spans="1:9" ht="19.899999999999999" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" ht="19.95" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A43" s="25" t="s">
         <v>153</v>
       </c>
@@ -2467,7 +2492,7 @@
       <c r="H43" s="22"/>
       <c r="I43" s="13"/>
     </row>
-    <row r="44" spans="1:9" ht="19.899999999999999" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" ht="19.95" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A44" s="25" t="s">
         <v>154</v>
       </c>
@@ -2493,7 +2518,7 @@
       <c r="H44" s="22"/>
       <c r="I44" s="13"/>
     </row>
-    <row r="45" spans="1:9" ht="19.899999999999999" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" ht="19.95" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A45" s="25" t="s">
         <v>170</v>
       </c>
@@ -2519,7 +2544,7 @@
       <c r="H45" s="22"/>
       <c r="I45" s="13"/>
     </row>
-    <row r="46" spans="1:9" ht="19.899999999999999" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" ht="19.95" customHeight="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.3">
       <c r="A46" s="25" t="s">
         <v>40</v>
       </c>
@@ -2546,7 +2571,7 @@
       <c r="H46" s="22"/>
       <c r="I46" s="13"/>
     </row>
-    <row r="47" spans="1:9" ht="19.899999999999999" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" ht="19.95" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A47" s="25" t="s">
         <v>156</v>
       </c>
@@ -2572,7 +2597,7 @@
       <c r="H47" s="22"/>
       <c r="I47" s="13"/>
     </row>
-    <row r="48" spans="1:9" ht="19.899999999999999" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" ht="19.8" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A48" s="25" t="s">
         <v>157</v>
       </c>
@@ -2595,7 +2620,7 @@
       <c r="H48" s="22"/>
       <c r="I48" s="13"/>
     </row>
-    <row r="49" spans="1:9" ht="19.899999999999999" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" ht="19.8" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A49" s="25" t="s">
         <v>158</v>
       </c>
@@ -2621,7 +2646,7 @@
       <c r="H49" s="22"/>
       <c r="I49" s="13"/>
     </row>
-    <row r="50" spans="1:9" ht="19.899999999999999" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" ht="19.8" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A50" s="25" t="s">
         <v>159</v>
       </c>
@@ -2644,7 +2669,7 @@
       <c r="H50" s="22"/>
       <c r="I50" s="13"/>
     </row>
-    <row r="51" spans="1:9" ht="19.899999999999999" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" ht="19.8" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A51" s="25" t="s">
         <v>160</v>
       </c>
@@ -2670,7 +2695,7 @@
       <c r="H51" s="22"/>
       <c r="I51" s="13"/>
     </row>
-    <row r="52" spans="1:9" ht="19.899999999999999" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" ht="19.8" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A52" s="25" t="s">
         <v>161</v>
       </c>
@@ -2696,7 +2721,7 @@
       <c r="H52" s="22"/>
       <c r="I52" s="13"/>
     </row>
-    <row r="53" spans="1:9" ht="19.899999999999999" customHeight="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" ht="19.95" customHeight="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.3">
       <c r="A53" s="25" t="s">
         <v>39</v>
       </c>
@@ -2723,7 +2748,7 @@
       <c r="H53" s="22"/>
       <c r="I53" s="13"/>
     </row>
-    <row r="54" spans="1:9" ht="19.899999999999999" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" ht="19.95" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A54" s="25" t="s">
         <v>162</v>
       </c>
@@ -2749,12 +2774,12 @@
       <c r="H54" s="22"/>
       <c r="I54" s="13"/>
     </row>
-    <row r="55" spans="1:9" ht="19.899999999999999" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" ht="19.95" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A55" s="25" t="s">
         <v>163</v>
       </c>
       <c r="B55" s="25" t="str">
-        <f t="shared" ref="B54:B57" si="5">$B$31 &amp; "/" &amp; E55</f>
+        <f t="shared" ref="B55:B57" si="5">$B$31 &amp; "/" &amp; E55</f>
         <v>/mng_activity/rooms-store</v>
       </c>
       <c r="C55" s="25" t="s">
@@ -2772,7 +2797,7 @@
       <c r="H55" s="22"/>
       <c r="I55" s="13"/>
     </row>
-    <row r="56" spans="1:9" ht="19.899999999999999" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" ht="19.95" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A56" s="25" t="s">
         <v>164</v>
       </c>
@@ -2798,7 +2823,7 @@
       <c r="H56" s="22"/>
       <c r="I56" s="13"/>
     </row>
-    <row r="57" spans="1:9" ht="19.899999999999999" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" ht="19.95" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A57" s="25" t="s">
         <v>165</v>
       </c>
@@ -2821,7 +2846,7 @@
       <c r="H57" s="22"/>
       <c r="I57" s="13"/>
     </row>
-    <row r="58" spans="1:9" ht="19.899999999999999" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" ht="19.95" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A58" s="25" t="s">
         <v>166</v>
       </c>
@@ -2847,7 +2872,7 @@
       <c r="H58" s="22"/>
       <c r="I58" s="13"/>
     </row>
-    <row r="59" spans="1:9" ht="19.899999999999999" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" ht="19.95" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A59" s="25" t="s">
         <v>167</v>
       </c>
@@ -2873,7 +2898,7 @@
       <c r="H59" s="22"/>
       <c r="I59" s="13"/>
     </row>
-    <row r="60" spans="1:9" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" ht="19.8" customHeight="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.3">
       <c r="A60" s="25" t="s">
         <v>41</v>
       </c>
@@ -2884,7 +2909,7 @@
       <c r="C60" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="D60" s="22" t="s">
+      <c r="D60" s="25" t="s">
         <v>31</v>
       </c>
       <c r="E60" s="25" t="s">
@@ -2895,45 +2920,208 @@
         <v>scheduling.blade.php</v>
       </c>
       <c r="G60" s="25" t="s">
-        <v>120</v>
+        <v>177</v>
       </c>
       <c r="H60" s="22"/>
       <c r="I60" s="13"/>
     </row>
-    <row r="61" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="26"/>
-      <c r="B61" s="26" t="str">
-        <f>"/" &amp; E61</f>
+    <row r="61" spans="1:9" ht="19.8" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
+      <c r="A61" s="25" t="s">
+        <v>171</v>
+      </c>
+      <c r="B61" s="25" t="str">
+        <f t="shared" ref="B61:B64" si="6">$B$31 &amp; "/" &amp; E61</f>
+        <v>/mng_activity/scheduling-create</v>
+      </c>
+      <c r="C61" s="25" t="s">
+        <v>145</v>
+      </c>
+      <c r="D61" s="22"/>
+      <c r="E61" s="25" t="str">
+        <f>$E60 &amp; "-create"</f>
+        <v>scheduling-create</v>
+      </c>
+      <c r="F61" s="25" t="str">
+        <f>IF($E61="Da definire",$E61,_xlfn.CONCAT($E61,".blade.php"))</f>
+        <v>scheduling-create.blade.php</v>
+      </c>
+      <c r="G61" s="25" t="s">
+        <v>177</v>
+      </c>
+      <c r="H61" s="22"/>
+      <c r="I61" s="13"/>
+    </row>
+    <row r="62" spans="1:9" ht="19.8" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
+      <c r="A62" s="25" t="s">
+        <v>172</v>
+      </c>
+      <c r="B62" s="25" t="str">
+        <f t="shared" si="6"/>
+        <v>/mng_activity/scheduling-store</v>
+      </c>
+      <c r="C62" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="D62" s="22"/>
+      <c r="E62" s="25" t="str">
+        <f>$E60 &amp; "-store"</f>
+        <v>scheduling-store</v>
+      </c>
+      <c r="F62" s="25"/>
+      <c r="G62" s="25" t="s">
+        <v>177</v>
+      </c>
+      <c r="H62" s="22"/>
+      <c r="I62" s="13"/>
+    </row>
+    <row r="63" spans="1:9" ht="19.8" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
+      <c r="A63" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="B63" s="25" t="str">
+        <f t="shared" si="6"/>
+        <v>/mng_activity/scheduling-edit</v>
+      </c>
+      <c r="C63" s="25" t="s">
+        <v>145</v>
+      </c>
+      <c r="D63" s="22"/>
+      <c r="E63" s="25" t="str">
+        <f>$E60 &amp; "-edit"</f>
+        <v>scheduling-edit</v>
+      </c>
+      <c r="F63" s="25" t="str">
+        <f>IF($E63="Da definire",$E63,_xlfn.CONCAT($E63,".blade.php"))</f>
+        <v>scheduling-edit.blade.php</v>
+      </c>
+      <c r="G63" s="25" t="s">
+        <v>177</v>
+      </c>
+      <c r="H63" s="22"/>
+      <c r="I63" s="13"/>
+    </row>
+    <row r="64" spans="1:9" ht="19.8" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
+      <c r="A64" s="25" t="s">
+        <v>174</v>
+      </c>
+      <c r="B64" s="25" t="str">
+        <f t="shared" si="6"/>
+        <v>/mng_activity/scheduling-update</v>
+      </c>
+      <c r="C64" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="D64" s="22"/>
+      <c r="E64" s="25" t="str">
+        <f>$E60 &amp; "-update"</f>
+        <v>scheduling-update</v>
+      </c>
+      <c r="F64" s="25"/>
+      <c r="G64" s="25" t="s">
+        <v>177</v>
+      </c>
+      <c r="H64" s="22"/>
+      <c r="I64" s="13"/>
+    </row>
+    <row r="65" spans="1:9" ht="19.8" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
+      <c r="A65" s="25" t="s">
+        <v>175</v>
+      </c>
+      <c r="B65" s="25" t="str">
+        <f>$B$31 &amp; "/" &amp; E65</f>
+        <v>/mng_activity/scheduling-delete</v>
+      </c>
+      <c r="C65" s="25" t="s">
+        <v>145</v>
+      </c>
+      <c r="D65" s="22"/>
+      <c r="E65" s="25" t="str">
+        <f>$E60 &amp; "-delete"</f>
+        <v>scheduling-delete</v>
+      </c>
+      <c r="F65" s="25" t="str">
+        <f>IF($E65="Da definire",$E65,_xlfn.CONCAT($E65,".blade.php"))</f>
+        <v>scheduling-delete.blade.php</v>
+      </c>
+      <c r="G65" s="25" t="s">
+        <v>177</v>
+      </c>
+      <c r="H65" s="22"/>
+      <c r="I65" s="13"/>
+    </row>
+    <row r="66" spans="1:9" ht="19.8" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
+      <c r="A66" s="25" t="s">
+        <v>176</v>
+      </c>
+      <c r="B66" s="25" t="str">
+        <f>$B$31 &amp; "/" &amp; E66</f>
+        <v>/mng_activity/scheduling-show</v>
+      </c>
+      <c r="C66" s="25" t="s">
+        <v>145</v>
+      </c>
+      <c r="D66" s="22"/>
+      <c r="E66" s="25" t="str">
+        <f>$E60 &amp; "-show"</f>
+        <v>scheduling-show</v>
+      </c>
+      <c r="F66" s="25" t="str">
+        <f>IF($E66="Da definire",$E66,_xlfn.CONCAT($E66,".blade.php"))</f>
+        <v>scheduling-show.blade.php</v>
+      </c>
+      <c r="G66" s="25" t="s">
+        <v>177</v>
+      </c>
+      <c r="H66" s="22"/>
+      <c r="I66" s="13"/>
+    </row>
+    <row r="67" spans="1:9" ht="19.8" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="25"/>
+      <c r="B67" s="25"/>
+      <c r="C67" s="25"/>
+      <c r="D67" s="22"/>
+      <c r="E67" s="20"/>
+      <c r="F67" s="25"/>
+      <c r="G67" s="25"/>
+      <c r="H67" s="22"/>
+      <c r="I67" s="13"/>
+    </row>
+    <row r="68" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="26" t="s">
+        <v>178</v>
+      </c>
+      <c r="B68" s="26" t="str">
+        <f>"/" &amp; E68</f>
         <v>/report_stats</v>
       </c>
-      <c r="C61" s="26" t="s">
+      <c r="C68" s="26" t="s">
         <v>63</v>
       </c>
-      <c r="D61" s="23" t="s">
+      <c r="D68" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="E61" s="26" t="s">
+      <c r="E68" s="26" t="s">
         <v>97</v>
       </c>
-      <c r="F61" s="26" t="str">
+      <c r="F68" s="26" t="str">
         <f t="shared" si="0"/>
         <v>report_stats.blade.php</v>
       </c>
-      <c r="G61" s="26" t="s">
+      <c r="G68" s="26" t="s">
         <v>95</v>
       </c>
-      <c r="H61" s="23" t="s">
+      <c r="H68" s="23" t="s">
         <v>98</v>
       </c>
-      <c r="I61" s="13"/>
+      <c r="I68" s="13"/>
     </row>
   </sheetData>
   <dataConsolidate/>
   <dataValidations count="2">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C61" xr:uid="{F340BA2D-9D43-4A9F-86F9-B281B429D2E7}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C68 C2:C67" xr:uid="{F340BA2D-9D43-4A9F-86F9-B281B429D2E7}">
       <formula1>RefTipo</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G61" xr:uid="{DFF187B0-2821-4C72-B394-0420A8E90996}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G68 G2:G67" xr:uid="{DFF187B0-2821-4C72-B394-0420A8E90996}">
       <formula1>RefController_nome</formula1>
     </dataValidation>
   </dataValidations>
@@ -2953,20 +3141,20 @@
   <dimension ref="B1:G28"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="6" width="25.140625" customWidth="1"/>
-    <col min="7" max="7" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="6" width="25.109375" customWidth="1"/>
+    <col min="7" max="7" width="24.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="19" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>68</v>
       </c>
@@ -2980,7 +3168,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="3" t="s">
         <v>66</v>
       </c>
@@ -2989,7 +3177,7 @@
       </c>
       <c r="E2" s="5"/>
     </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B3" s="2" t="s">
         <v>145</v>
       </c>
@@ -2998,7 +3186,7 @@
       </c>
       <c r="E3" s="5"/>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B4" s="3" t="s">
         <v>65</v>
       </c>
@@ -3007,7 +3195,7 @@
       </c>
       <c r="E4" s="5"/>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
         <v>64</v>
       </c>
@@ -3015,7 +3203,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B6" s="4" t="s">
         <v>63</v>
       </c>
@@ -3023,7 +3211,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B7" s="4" t="s">
         <v>87</v>
       </c>
@@ -3031,7 +3219,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B8" s="4" t="s">
         <v>96</v>
       </c>
@@ -3039,7 +3227,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B9" s="4" t="s">
         <v>76</v>
       </c>
@@ -3047,37 +3235,40 @@
         <v>120</v>
       </c>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:7" x14ac:dyDescent="0.3">
       <c r="D10" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:7" x14ac:dyDescent="0.3">
       <c r="D11" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:7" x14ac:dyDescent="0.3">
       <c r="D12" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:7" x14ac:dyDescent="0.3">
       <c r="D13" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
-    </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D14" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B15" s="17"/>
       <c r="C15" s="16"/>
       <c r="D15" s="16"/>
       <c r="E15" s="16"/>
     </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B16" s="9"/>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
@@ -3085,7 +3276,7 @@
       <c r="F16" s="10"/>
       <c r="G16" s="8"/>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B17" s="9"/>
       <c r="C17" s="6"/>
       <c r="D17" s="7"/>
@@ -3093,7 +3284,7 @@
       <c r="F17" s="10"/>
       <c r="G17" s="8"/>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B18" s="9"/>
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
@@ -3101,7 +3292,7 @@
       <c r="F18" s="10"/>
       <c r="G18" s="8"/>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B19" s="9"/>
       <c r="C19" s="6"/>
       <c r="D19" s="7"/>
@@ -3109,7 +3300,7 @@
       <c r="F19" s="10"/>
       <c r="G19" s="8"/>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B20" s="9"/>
       <c r="C20" s="6"/>
       <c r="D20" s="7"/>
@@ -3117,7 +3308,7 @@
       <c r="F20" s="10"/>
       <c r="G20" s="8"/>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B21" s="9"/>
       <c r="C21" s="6"/>
       <c r="D21" s="7"/>
@@ -3125,7 +3316,7 @@
       <c r="F21" s="10"/>
       <c r="G21" s="8"/>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B22" s="9"/>
       <c r="C22" s="6"/>
       <c r="D22" s="7"/>
@@ -3133,7 +3324,7 @@
       <c r="F22" s="10"/>
       <c r="G22" s="8"/>
     </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B23" s="9"/>
       <c r="C23" s="6"/>
       <c r="D23" s="7"/>
@@ -3141,7 +3332,7 @@
       <c r="F23" s="10"/>
       <c r="G23" s="8"/>
     </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B24" s="9"/>
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
@@ -3149,7 +3340,7 @@
       <c r="F24" s="10"/>
       <c r="G24" s="8"/>
     </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B25" s="9"/>
       <c r="C25" s="6"/>
       <c r="D25" s="7"/>
@@ -3157,7 +3348,7 @@
       <c r="F25" s="10"/>
       <c r="G25" s="8"/>
     </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B26" s="9"/>
       <c r="C26" s="6"/>
       <c r="D26" s="7"/>
@@ -3165,7 +3356,7 @@
       <c r="F26" s="10"/>
       <c r="G26" s="8"/>
     </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B27" s="9"/>
       <c r="C27" s="6"/>
       <c r="D27" s="7"/>
@@ -3173,13 +3364,13 @@
       <c r="F27" s="10"/>
       <c r="G27" s="8"/>
     </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:7" x14ac:dyDescent="0.3">
       <c r="D28" s="7"/>
       <c r="E28" s="10"/>
       <c r="F28" s="10"/>
     </row>
   </sheetData>
-  <sortState ref="D13:D29">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="D13:D29">
     <sortCondition ref="D13"/>
   </sortState>
   <dataConsolidate/>

</xml_diff>

<commit_message>
Da finire le crud di scheduling
</commit_message>
<xml_diff>
--- a/Documentazioni/Codifica pagine sito.xlsx
+++ b/Documentazioni/Codifica pagine sito.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
   <workbookPr filterPrivacy="1" codeName="Questa_cartella_di_lavoro"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{312E79FD-DF42-46E7-B4A9-EEEAF626DCF8}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89CC8A4F-28FC-4881-A060-5406D960ACAE}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1309,8 +1309,8 @@
   <sheetPr codeName="Foglio2"/>
   <dimension ref="A1:I68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A61" sqref="A61:A66"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H53" sqref="H53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" outlineLevelRow="2" x14ac:dyDescent="0.3"/>
@@ -2055,7 +2055,7 @@
       </c>
       <c r="I26" s="13"/>
     </row>
-    <row r="27" spans="1:9" ht="19.95" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" ht="19.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A27" s="25" t="s">
         <v>35</v>
       </c>
@@ -2082,7 +2082,7 @@
       <c r="H27" s="22"/>
       <c r="I27" s="13"/>
     </row>
-    <row r="28" spans="1:9" ht="19.95" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" ht="19.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A28" s="25" t="s">
         <v>128</v>
       </c>
@@ -2109,7 +2109,7 @@
       <c r="H28" s="22"/>
       <c r="I28" s="13"/>
     </row>
-    <row r="29" spans="1:9" ht="19.95" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" ht="19.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A29" s="25" t="s">
         <v>129</v>
       </c>
@@ -2136,7 +2136,7 @@
       <c r="H29" s="22"/>
       <c r="I29" s="13"/>
     </row>
-    <row r="30" spans="1:9" ht="19.95" customHeight="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" ht="19.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A30" s="27" t="s">
         <v>36</v>
       </c>
@@ -2217,7 +2217,7 @@
       <c r="H32" s="22"/>
       <c r="I32" s="13"/>
     </row>
-    <row r="33" spans="1:9" ht="19.95" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" ht="19.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A33" s="25" t="s">
         <v>144</v>
       </c>
@@ -2243,7 +2243,7 @@
       <c r="H33" s="22"/>
       <c r="I33" s="13"/>
     </row>
-    <row r="34" spans="1:9" ht="19.95" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" ht="19.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A34" s="25" t="s">
         <v>146</v>
       </c>
@@ -2266,7 +2266,7 @@
       <c r="H34" s="22"/>
       <c r="I34" s="13"/>
     </row>
-    <row r="35" spans="1:9" ht="19.95" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" ht="19.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A35" s="25" t="s">
         <v>147</v>
       </c>
@@ -2292,7 +2292,7 @@
       <c r="H35" s="22"/>
       <c r="I35" s="13"/>
     </row>
-    <row r="36" spans="1:9" ht="19.95" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" ht="19.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A36" s="25" t="s">
         <v>148</v>
       </c>
@@ -2315,7 +2315,7 @@
       <c r="H36" s="22"/>
       <c r="I36" s="13"/>
     </row>
-    <row r="37" spans="1:9" ht="19.95" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" ht="19.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A37" s="25" t="s">
         <v>149</v>
       </c>
@@ -2341,7 +2341,7 @@
       <c r="H37" s="22"/>
       <c r="I37" s="13"/>
     </row>
-    <row r="38" spans="1:9" ht="19.95" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" ht="19.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A38" s="25" t="s">
         <v>169</v>
       </c>
@@ -2367,7 +2367,7 @@
       <c r="H38" s="22"/>
       <c r="I38" s="13"/>
     </row>
-    <row r="39" spans="1:9" ht="19.95" customHeight="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" ht="19.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A39" s="25" t="s">
         <v>38</v>
       </c>
@@ -2394,7 +2394,7 @@
       <c r="H39" s="22"/>
       <c r="I39" s="13"/>
     </row>
-    <row r="40" spans="1:9" ht="19.95" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" ht="19.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A40" s="25" t="s">
         <v>150</v>
       </c>
@@ -2420,7 +2420,7 @@
       <c r="H40" s="22"/>
       <c r="I40" s="13"/>
     </row>
-    <row r="41" spans="1:9" ht="19.95" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" ht="19.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A41" s="25" t="s">
         <v>151</v>
       </c>
@@ -2443,7 +2443,7 @@
       <c r="H41" s="22"/>
       <c r="I41" s="13"/>
     </row>
-    <row r="42" spans="1:9" ht="19.95" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" ht="19.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A42" s="25" t="s">
         <v>152</v>
       </c>
@@ -2469,7 +2469,7 @@
       <c r="H42" s="22"/>
       <c r="I42" s="13"/>
     </row>
-    <row r="43" spans="1:9" ht="19.95" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" ht="19.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A43" s="25" t="s">
         <v>153</v>
       </c>
@@ -2492,7 +2492,7 @@
       <c r="H43" s="22"/>
       <c r="I43" s="13"/>
     </row>
-    <row r="44" spans="1:9" ht="19.95" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" ht="19.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A44" s="25" t="s">
         <v>154</v>
       </c>
@@ -2518,7 +2518,7 @@
       <c r="H44" s="22"/>
       <c r="I44" s="13"/>
     </row>
-    <row r="45" spans="1:9" ht="19.95" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" ht="19.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A45" s="25" t="s">
         <v>170</v>
       </c>
@@ -2544,7 +2544,7 @@
       <c r="H45" s="22"/>
       <c r="I45" s="13"/>
     </row>
-    <row r="46" spans="1:9" ht="19.95" customHeight="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" ht="19.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A46" s="25" t="s">
         <v>40</v>
       </c>
@@ -2571,7 +2571,7 @@
       <c r="H46" s="22"/>
       <c r="I46" s="13"/>
     </row>
-    <row r="47" spans="1:9" ht="19.95" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" ht="19.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A47" s="25" t="s">
         <v>156</v>
       </c>
@@ -2597,7 +2597,7 @@
       <c r="H47" s="22"/>
       <c r="I47" s="13"/>
     </row>
-    <row r="48" spans="1:9" ht="19.8" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:9" ht="19.8" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A48" s="25" t="s">
         <v>157</v>
       </c>
@@ -2620,7 +2620,7 @@
       <c r="H48" s="22"/>
       <c r="I48" s="13"/>
     </row>
-    <row r="49" spans="1:9" ht="19.8" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:9" ht="19.8" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A49" s="25" t="s">
         <v>158</v>
       </c>
@@ -2646,7 +2646,7 @@
       <c r="H49" s="22"/>
       <c r="I49" s="13"/>
     </row>
-    <row r="50" spans="1:9" ht="19.8" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:9" ht="19.8" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A50" s="25" t="s">
         <v>159</v>
       </c>
@@ -2669,7 +2669,7 @@
       <c r="H50" s="22"/>
       <c r="I50" s="13"/>
     </row>
-    <row r="51" spans="1:9" ht="19.8" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:9" ht="19.8" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A51" s="25" t="s">
         <v>160</v>
       </c>
@@ -2695,7 +2695,7 @@
       <c r="H51" s="22"/>
       <c r="I51" s="13"/>
     </row>
-    <row r="52" spans="1:9" ht="19.8" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:9" ht="19.8" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A52" s="25" t="s">
         <v>161</v>
       </c>
@@ -2721,7 +2721,7 @@
       <c r="H52" s="22"/>
       <c r="I52" s="13"/>
     </row>
-    <row r="53" spans="1:9" ht="19.95" customHeight="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:9" ht="19.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A53" s="25" t="s">
         <v>39</v>
       </c>
@@ -2748,7 +2748,7 @@
       <c r="H53" s="22"/>
       <c r="I53" s="13"/>
     </row>
-    <row r="54" spans="1:9" ht="19.95" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:9" ht="19.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A54" s="25" t="s">
         <v>162</v>
       </c>
@@ -2774,7 +2774,7 @@
       <c r="H54" s="22"/>
       <c r="I54" s="13"/>
     </row>
-    <row r="55" spans="1:9" ht="19.95" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:9" ht="19.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A55" s="25" t="s">
         <v>163</v>
       </c>
@@ -2797,7 +2797,7 @@
       <c r="H55" s="22"/>
       <c r="I55" s="13"/>
     </row>
-    <row r="56" spans="1:9" ht="19.95" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:9" ht="19.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A56" s="25" t="s">
         <v>164</v>
       </c>
@@ -2823,7 +2823,7 @@
       <c r="H56" s="22"/>
       <c r="I56" s="13"/>
     </row>
-    <row r="57" spans="1:9" ht="19.95" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:9" ht="19.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A57" s="25" t="s">
         <v>165</v>
       </c>
@@ -2846,7 +2846,7 @@
       <c r="H57" s="22"/>
       <c r="I57" s="13"/>
     </row>
-    <row r="58" spans="1:9" ht="19.95" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:9" ht="19.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A58" s="25" t="s">
         <v>166</v>
       </c>
@@ -2872,7 +2872,7 @@
       <c r="H58" s="22"/>
       <c r="I58" s="13"/>
     </row>
-    <row r="59" spans="1:9" ht="19.95" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:9" ht="19.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A59" s="25" t="s">
         <v>167</v>
       </c>
@@ -2898,7 +2898,7 @@
       <c r="H59" s="22"/>
       <c r="I59" s="13"/>
     </row>
-    <row r="60" spans="1:9" ht="19.8" customHeight="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:9" ht="19.8" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A60" s="25" t="s">
         <v>41</v>
       </c>

</xml_diff>